<commit_message>
Added Run button for batch mode and formatting additions
</commit_message>
<xml_diff>
--- a/Radiomics_Code/Output.xlsx
+++ b/Radiomics_Code/Output.xlsx
@@ -2149,7 +2149,7 @@
     <t>{'Original': {}, 'Wavelet': {}}</t>
   </si>
   <si>
-    <t>bf4858bc3421efabac1de52636489cec8278d566</t>
+    <t>1c8283e59692ba313e732483f84c87ea428df23a</t>
   </si>
   <si>
     <t>3D</t>
@@ -2158,1735 +2158,1735 @@
     <t>(1.0, 1.0, 1.0)</t>
   </si>
   <si>
-    <t>(292, 258, 244)</t>
-  </si>
-  <si>
-    <t>08597b0c96a4668bc5a76313a6dc15839ca86503</t>
-  </si>
-  <si>
-    <t>(66, 59, 84, 151, 138, 102)</t>
-  </si>
-  <si>
-    <t>(133.31353611192267, 135.61938132281816, 143.08855781417824)</t>
-  </si>
-  <si>
-    <t>151.21177202850313</t>
-  </si>
-  <si>
-    <t>156.92354826475216</t>
-  </si>
-  <si>
-    <t>158.22136391777187</t>
-  </si>
-  <si>
-    <t>172.75416058665562</t>
-  </si>
-  <si>
-    <t>475851.5416666667</t>
-  </si>
-  <si>
-    <t>0.4319305677618243</t>
-  </si>
-  <si>
-    <t>68241.90964848455</t>
-  </si>
-  <si>
-    <t>0.14341008418186005</t>
-  </si>
-  <si>
-    <t>-574.0000000000001</t>
-  </si>
-  <si>
-    <t>-297.00000000000006</t>
-  </si>
-  <si>
-    <t>104581097904.00002</t>
-  </si>
-  <si>
-    <t>3.9498248545616503</t>
-  </si>
-  <si>
-    <t>144.99999999999994</t>
-  </si>
-  <si>
-    <t>2.583865986578601</t>
-  </si>
-  <si>
-    <t>-200.00000000000003</t>
-  </si>
-  <si>
-    <t>84.4843785202992</t>
-  </si>
-  <si>
-    <t>-457.37826243229216</t>
-  </si>
-  <si>
-    <t>-479.0000000000001</t>
-  </si>
-  <si>
-    <t>-801.0000000000002</t>
-  </si>
-  <si>
-    <t>601.0000000000002</t>
-  </si>
-  <si>
-    <t>60.93326495132835</t>
-  </si>
-  <si>
-    <t>468.850091304148</t>
-  </si>
-  <si>
-    <t>0.6027926966386129</t>
-  </si>
-  <si>
-    <t>0.07378060292302353</t>
-  </si>
-  <si>
-    <t>10625.53317032524</t>
-  </si>
-  <si>
-    <t>234.2169324523216</t>
-  </si>
-  <si>
-    <t>8376.668629881078</t>
-  </si>
-  <si>
-    <t>245.3106981037346</t>
-  </si>
-  <si>
-    <t>56.33396476618688</t>
-  </si>
-  <si>
-    <t>4.441936291674851</t>
-  </si>
-  <si>
-    <t>0.8531568219301449</t>
-  </si>
-  <si>
-    <t>1.4811434354201833</t>
-  </si>
-  <si>
-    <t>2.2695604944394883</t>
-  </si>
-  <si>
-    <t>2.187981701471104</t>
-  </si>
-  <si>
-    <t>0.5427953997529509</t>
-  </si>
-  <si>
-    <t>0.49283499737080155</t>
-  </si>
-  <si>
-    <t>0.9931528673771685</t>
-  </si>
-  <si>
-    <t>0.9468466885790312</t>
-  </si>
-  <si>
-    <t>-0.26490444024758164</t>
-  </si>
-  <si>
-    <t>0.9273036676196879</t>
-  </si>
-  <si>
-    <t>0.4422196640421806</t>
-  </si>
-  <si>
-    <t>14.874175036504385</t>
-  </si>
-  <si>
-    <t>0.014533689775651492</t>
-  </si>
-  <si>
-    <t>6.750792470153604</t>
-  </si>
-  <si>
-    <t>0.866543885343715</t>
-  </si>
-  <si>
-    <t>0.037867657829419775</t>
-  </si>
-  <si>
-    <t>29.74835007300877</t>
-  </si>
-  <si>
-    <t>4.842461119577219</t>
-  </si>
-  <si>
-    <t>15.193975264465438</t>
-  </si>
-  <si>
-    <t>25136.55696859488</t>
-  </si>
-  <si>
-    <t>0.06952204763019167</t>
-  </si>
-  <si>
-    <t>17.890404198432993</t>
-  </si>
-  <si>
-    <t>260.8848606980387</t>
-  </si>
-  <si>
-    <t>2.2631319223223163</t>
-  </si>
-  <si>
-    <t>518.8029389995238</t>
-  </si>
-  <si>
-    <t>0.012873731453505332</t>
-  </si>
-  <si>
-    <t>0.005146448952463024</t>
-  </si>
-  <si>
-    <t>5.00793273056088</t>
-  </si>
-  <si>
-    <t>230587.65579992768</t>
-  </si>
-  <si>
-    <t>0.6357049121236453</t>
-  </si>
-  <si>
-    <t>0.7597482295826197</t>
-  </si>
-  <si>
-    <t>0.5159849256504354</t>
-  </si>
-  <si>
-    <t>0.8246199488642614</t>
-  </si>
-  <si>
-    <t>223.78939957959727</t>
-  </si>
-  <si>
-    <t>0.004094411356082935</t>
-  </si>
-  <si>
-    <t>1943.7230614300101</t>
-  </si>
-  <si>
-    <t>0.07249722358099325</t>
-  </si>
-  <si>
-    <t>18.160303224301433</t>
-  </si>
-  <si>
-    <t>384.9390175674164</t>
-  </si>
-  <si>
-    <t>289672.63746223564</t>
-  </si>
-  <si>
-    <t>57762585.26619671</t>
-  </si>
-  <si>
-    <t>1615.7028774456842</t>
-  </si>
-  <si>
-    <t>0.003600303142469925</t>
-  </si>
-  <si>
-    <t>7347.756928126515</t>
-  </si>
-  <si>
-    <t>0.2740575483244383</t>
-  </si>
-  <si>
-    <t>0.5358533999222819</t>
-  </si>
-  <si>
-    <t>210.3153572399438</t>
-  </si>
-  <si>
-    <t>0.0018617287853400625</t>
-  </si>
-  <si>
-    <t>6.659307887328376</t>
-  </si>
-  <si>
-    <t>0.05635439940978273</t>
-  </si>
-  <si>
-    <t>289357.7579901764</t>
-  </si>
-  <si>
-    <t>-25.4642578748014</t>
-  </si>
-  <si>
-    <t>39.764449274519784</t>
-  </si>
-  <si>
-    <t>400882130.6805982</t>
-  </si>
-  <si>
-    <t>2.2120093210224496</t>
-  </si>
-  <si>
-    <t>32.5339224702804</t>
-  </si>
-  <si>
-    <t>5.769599281193624</t>
-  </si>
-  <si>
-    <t>231.71567419682646</t>
-  </si>
-  <si>
-    <t>21.00091846881382</t>
-  </si>
-  <si>
-    <t>6.8569931585428145</t>
-  </si>
-  <si>
-    <t>5.31223264103777</t>
-  </si>
-  <si>
-    <t>-128.31301680437187</t>
-  </si>
-  <si>
-    <t>360.02869100119835</t>
-  </si>
-  <si>
-    <t>13.631287166478163</t>
-  </si>
-  <si>
-    <t>29.027909173243813</t>
-  </si>
-  <si>
-    <t>0.7143290588235565</t>
-  </si>
-  <si>
-    <t>0.26819629001847056</t>
-  </si>
-  <si>
-    <t>795.6011557937894</t>
-  </si>
-  <si>
-    <t>46.600009660228054</t>
-  </si>
-  <si>
-    <t>103.47110610161597</t>
-  </si>
-  <si>
-    <t>6.775569554551458</t>
-  </si>
-  <si>
-    <t>4.092336615168947</t>
-  </si>
-  <si>
-    <t>1.1692895513535064</t>
-  </si>
-  <si>
-    <t>0.5539878479641108</t>
-  </si>
-  <si>
-    <t>0.7645282467190208</t>
-  </si>
-  <si>
-    <t>1.503229891455092</t>
-  </si>
-  <si>
-    <t>0.5533528352707575</t>
-  </si>
-  <si>
-    <t>0.6763888595093847</t>
-  </si>
-  <si>
-    <t>0.6573815529822254</t>
-  </si>
-  <si>
-    <t>0.9955099596259736</t>
-  </si>
-  <si>
-    <t>0.9563099639181707</t>
-  </si>
-  <si>
-    <t>-0.14240383918386937</t>
-  </si>
-  <si>
-    <t>0.6240448227923836</t>
-  </si>
-  <si>
-    <t>0.48774576781330214</t>
-  </si>
-  <si>
-    <t>6.7726834592282605</t>
-  </si>
-  <si>
-    <t>0.09182792889420456</t>
-  </si>
-  <si>
-    <t>4.071899601255539</t>
-  </si>
-  <si>
-    <t>0.6553367135792691</t>
-  </si>
-  <si>
-    <t>0.177748602265821</t>
-  </si>
-  <si>
-    <t>13.545366918456521</t>
-  </si>
-  <si>
-    <t>2.9757368736627994</t>
-  </si>
-  <si>
-    <t>1.3154065416306122</t>
-  </si>
-  <si>
-    <t>70140.78074420658</t>
-  </si>
-  <si>
-    <t>0.23992556164797046</t>
-  </si>
-  <si>
-    <t>1.629753163353127</t>
-  </si>
-  <si>
-    <t>47.80231814810523</t>
-  </si>
-  <si>
-    <t>4.178304031807898</t>
-  </si>
-  <si>
-    <t>194.49604268556655</t>
-  </si>
-  <si>
-    <t>0.09839855693449989</t>
-  </si>
-  <si>
-    <t>0.024208225978680626</t>
-  </si>
-  <si>
-    <t>3.890086761640931</t>
-  </si>
-  <si>
-    <t>137424.71900691875</t>
-  </si>
-  <si>
-    <t>0.4567332526430708</t>
-  </si>
-  <si>
-    <t>0.6146064223801389</t>
-  </si>
-  <si>
-    <t>1.2976618159010316</t>
-  </si>
-  <si>
-    <t>0.690922784482531</t>
-  </si>
-  <si>
-    <t>33.3577688582534</t>
-  </si>
-  <si>
-    <t>0.016915485176820934</t>
-  </si>
-  <si>
-    <t>1192.9091995221027</t>
-  </si>
-  <si>
-    <t>0.17815250888920292</t>
-  </si>
-  <si>
-    <t>5.807480330274391</t>
-  </si>
-  <si>
-    <t>51.2410394265233</t>
-  </si>
-  <si>
-    <t>8493373.6901135</t>
-  </si>
-  <si>
-    <t>384848745.06914574</t>
-  </si>
-  <si>
-    <t>193663.95901009507</t>
-  </si>
-  <si>
-    <t>0.033267655232315035</t>
-  </si>
-  <si>
-    <t>1136.5979689366786</t>
-  </si>
-  <si>
-    <t>0.1697428269021324</t>
-  </si>
-  <si>
-    <t>0.40774287291279504</t>
-  </si>
-  <si>
-    <t>20.72355767270917</t>
-  </si>
-  <si>
-    <t>0.013963460832029215</t>
-  </si>
-  <si>
-    <t>6.377922386477243</t>
-  </si>
-  <si>
-    <t>0.01407441193718642</t>
-  </si>
-  <si>
-    <t>8488325.456038568</t>
-  </si>
-  <si>
-    <t>-29.662360349336097</t>
-  </si>
-  <si>
-    <t>34.81831904341648</t>
-  </si>
-  <si>
-    <t>309927460.69380516</t>
-  </si>
-  <si>
-    <t>2.125562654689945</t>
-  </si>
-  <si>
-    <t>33.655619035301356</t>
-  </si>
-  <si>
-    <t>3.189748230946517</t>
-  </si>
-  <si>
-    <t>144.60919910782908</t>
-  </si>
-  <si>
-    <t>20.119723651352732</t>
-  </si>
-  <si>
-    <t>2.537855204799298</t>
-  </si>
-  <si>
-    <t>2.4899097490170616</t>
-  </si>
-  <si>
-    <t>-121.73996829958438</t>
-  </si>
-  <si>
-    <t>266.34916740741346</t>
-  </si>
-  <si>
-    <t>13.95890735027715</t>
-  </si>
-  <si>
-    <t>25.52333586940477</t>
-  </si>
-  <si>
-    <t>0.018195510852768566</t>
-  </si>
-  <si>
-    <t>0.26941787680996004</t>
-  </si>
-  <si>
-    <t>644.9999648619175</t>
-  </si>
-  <si>
-    <t>31.577651371143137</t>
-  </si>
-  <si>
-    <t>23.60952094290144</t>
-  </si>
-  <si>
-    <t>0.09741250033472112</t>
-  </si>
-  <si>
-    <t>2.6339103631606764</t>
-  </si>
-  <si>
-    <t>1.7936540641510494</t>
-  </si>
-  <si>
-    <t>0.18946640264934606</t>
-  </si>
-  <si>
-    <t>0.9837755065275758</t>
-  </si>
-  <si>
-    <t>1.7250837973485331</t>
-  </si>
-  <si>
-    <t>0.7709678925083812</t>
-  </si>
-  <si>
-    <t>0.618451603728894</t>
-  </si>
-  <si>
-    <t>0.5865058844566994</t>
-  </si>
-  <si>
-    <t>0.9858881041178068</t>
-  </si>
-  <si>
-    <t>0.9229097587150904</t>
-  </si>
-  <si>
-    <t>-0.055033074182235124</t>
-  </si>
-  <si>
-    <t>0.25798848670418456</t>
-  </si>
-  <si>
-    <t>0.4897180218947289</t>
-  </si>
-  <si>
-    <t>5.600677302799255</t>
-  </si>
-  <si>
-    <t>0.08039148752429047</t>
-  </si>
-  <si>
-    <t>4.122880488356369</t>
-  </si>
-  <si>
-    <t>0.2284924260764809</t>
-  </si>
-  <si>
-    <t>0.14234946148135758</t>
-  </si>
-  <si>
-    <t>11.201354605598512</t>
-  </si>
-  <si>
-    <t>2.723481710147627</t>
-  </si>
-  <si>
-    <t>1.1068911068279315</t>
-  </si>
-  <si>
-    <t>80093.53331877809</t>
-  </si>
-  <si>
-    <t>0.2447712453787324</t>
-  </si>
-  <si>
-    <t>1.3053787733250803</t>
-  </si>
-  <si>
-    <t>32.66711115810654</t>
-  </si>
-  <si>
-    <t>3.0507258984184937</t>
-  </si>
-  <si>
-    <t>98.3839250560906</t>
-  </si>
-  <si>
-    <t>0.10702100044310808</t>
-  </si>
-  <si>
-    <t>0.03703077116473123</t>
-  </si>
-  <si>
-    <t>3.4887770521081127</t>
-  </si>
-  <si>
-    <t>181269.17983786442</t>
-  </si>
-  <si>
-    <t>0.5417678881650512</t>
-  </si>
-  <si>
-    <t>0.6887287805781911</t>
-  </si>
-  <si>
-    <t>0.8235788727378798</t>
-  </si>
-  <si>
-    <t>0.7573344971680712</t>
-  </si>
-  <si>
-    <t>24.85578325281665</t>
-  </si>
-  <si>
-    <t>0.028592845274078002</t>
-  </si>
-  <si>
-    <t>2683.518681664438</t>
-  </si>
-  <si>
-    <t>0.2110846127321984</t>
-  </si>
-  <si>
-    <t>5.149218190437369</t>
-  </si>
-  <si>
-    <t>36.29041138991583</t>
-  </si>
-  <si>
-    <t>4389287.666561787</t>
-  </si>
-  <si>
-    <t>140669701.62589476</t>
-  </si>
-  <si>
-    <t>143269.64088354917</t>
-  </si>
-  <si>
-    <t>0.05801050171951911</t>
-  </si>
-  <si>
-    <t>2565.0571068984505</t>
-  </si>
-  <si>
-    <t>0.20176646793820896</t>
-  </si>
-  <si>
-    <t>0.4378690968506863</t>
-  </si>
-  <si>
-    <t>15.987527708070088</t>
-  </si>
-  <si>
-    <t>0.0272568588069038</t>
-  </si>
-  <si>
-    <t>5.498845460167411</t>
-  </si>
-  <si>
-    <t>0.02672162469495982</t>
-  </si>
-  <si>
-    <t>4387887.195046659</t>
-  </si>
-  <si>
-    <t>-11.70447553358122</t>
-  </si>
-  <si>
-    <t>11.63046509553935</t>
-  </si>
-  <si>
-    <t>40152040.984327</t>
-  </si>
-  <si>
-    <t>1.0670342065178913</t>
-  </si>
-  <si>
-    <t>12.19492995896773</t>
-  </si>
-  <si>
-    <t>3.1573596387061964</t>
-  </si>
-  <si>
-    <t>45.5723278051013</t>
-  </si>
-  <si>
-    <t>7.283208110242709</t>
-  </si>
-  <si>
-    <t>-0.0558141349453949</t>
-  </si>
-  <si>
-    <t>-0.06264216896648644</t>
-  </si>
-  <si>
-    <t>-43.02896146421531</t>
-  </si>
-  <si>
-    <t>88.60128926931661</t>
-  </si>
-  <si>
-    <t>5.057637943272164</t>
-  </si>
-  <si>
-    <t>9.186735646991355</t>
-  </si>
-  <si>
-    <t>0.0006703620608040231</t>
-  </si>
-  <si>
-    <t>0.4921011688568814</t>
-  </si>
-  <si>
-    <t>84.39299663004192</t>
-  </si>
-  <si>
-    <t>6.241388224134808</t>
-  </si>
-  <si>
-    <t>0.6526472547051392</t>
-  </si>
-  <si>
-    <t>0.00195395133617771</t>
-  </si>
-  <si>
-    <t>0.5452231453735378</t>
-  </si>
-  <si>
-    <t>0.5178561745071713</t>
-  </si>
-  <si>
-    <t>0.02574963593589437</t>
-  </si>
-  <si>
-    <t>0.5020065806985946</t>
-  </si>
-  <si>
-    <t>1.035339240908882</t>
-  </si>
-  <si>
-    <t>0.257999917114747</t>
-  </si>
-  <si>
-    <t>0.7516165298316297</t>
-  </si>
-  <si>
-    <t>0.7505816690315604</t>
-  </si>
-  <si>
-    <t>0.9698231051762336</t>
-  </si>
-  <si>
-    <t>0.9001245146496525</t>
-  </si>
-  <si>
-    <t>-0.023937409937543144</t>
-  </si>
-  <si>
-    <t>0.11524604547770255</t>
-  </si>
-  <si>
-    <t>0.4883438746615743</t>
-  </si>
-  <si>
-    <t>2.4969073500969516</t>
-  </si>
-  <si>
-    <t>0.24973986643349774</t>
-  </si>
-  <si>
-    <t>2.1073247919076166</t>
-  </si>
-  <si>
-    <t>0.09888265353287548</t>
-  </si>
-  <si>
-    <t>0.270060129707235</t>
-  </si>
-  <si>
-    <t>4.993814700193903</t>
-  </si>
-  <si>
-    <t>1.5564466746236223</t>
-  </si>
-  <si>
-    <t>0.26576982997017723</t>
-  </si>
-  <si>
-    <t>119551.68332258324</t>
-  </si>
-  <si>
-    <t>0.48499192023654214</t>
-  </si>
-  <si>
-    <t>0.2804895347553875</t>
-  </si>
-  <si>
-    <t>6.526357467289983</t>
-  </si>
-  <si>
-    <t>6.445824361571862</t>
-  </si>
-  <si>
-    <t>41.765712807283954</t>
-  </si>
-  <si>
-    <t>1.1750343007317183</t>
-  </si>
-  <si>
-    <t>0.18613589546057624</t>
-  </si>
-  <si>
-    <t>3.0136898362465603</t>
-  </si>
-  <si>
-    <t>90206.93872618394</t>
-  </si>
-  <si>
-    <t>0.35556237436253063</t>
-  </si>
-  <si>
-    <t>0.5178074909282228</t>
-  </si>
-  <si>
-    <t>2.037013728222633</t>
-  </si>
-  <si>
-    <t>0.5763981415459345</t>
-  </si>
-  <si>
-    <t>3.7796512139044443</t>
-  </si>
-  <si>
-    <t>0.1092366185518553</t>
-  </si>
-  <si>
-    <t>1191.805</t>
-  </si>
-  <si>
-    <t>0.49658541666666667</t>
-  </si>
-  <si>
-    <t>2.2383604166666666</t>
-  </si>
-  <si>
-    <t>8.204166666666667</t>
-  </si>
-  <si>
-    <t>46405047.67125</t>
-  </si>
-  <si>
-    <t>300382637.1404167</t>
-  </si>
-  <si>
-    <t>8413417.5211169</t>
-  </si>
-  <si>
-    <t>0.5477575231481482</t>
-  </si>
-  <si>
-    <t>1045.6291666666666</t>
-  </si>
-  <si>
-    <t>0.4356788194444444</t>
-  </si>
-  <si>
-    <t>0.6676772463152078</t>
-  </si>
-  <si>
-    <t>5.3951858205783285</t>
-  </si>
-  <si>
-    <t>0.371041149081163</t>
-  </si>
-  <si>
-    <t>2.525455695497179</t>
-  </si>
-  <si>
-    <t>0.005044592092181513</t>
-  </si>
-  <si>
-    <t>46365751.71238733</t>
-  </si>
-  <si>
-    <t>-22.642700307322556</t>
-  </si>
-  <si>
-    <t>41.358847518793056</t>
-  </si>
-  <si>
-    <t>435885044.5306759</t>
-  </si>
-  <si>
-    <t>2.19645961172094</t>
-  </si>
-  <si>
-    <t>31.068706347234126</t>
-  </si>
-  <si>
-    <t>8.338729122785942</t>
-  </si>
-  <si>
-    <t>284.7735364289666</t>
-  </si>
-  <si>
-    <t>20.887471683750146</t>
-  </si>
-  <si>
-    <t>8.46199638509927</t>
-  </si>
-  <si>
-    <t>5.777428754799703</t>
-  </si>
-  <si>
-    <t>-143.44259927164518</t>
-  </si>
-  <si>
-    <t>428.2161357006118</t>
-  </si>
-  <si>
-    <t>13.110422458896986</t>
-  </si>
-  <si>
-    <t>30.26867363531997</t>
-  </si>
-  <si>
-    <t>1.243978558282094</t>
-  </si>
-  <si>
-    <t>0.27645756878305305</t>
-  </si>
-  <si>
-    <t>844.5872208200808</t>
-  </si>
-  <si>
-    <t>47.426118006126416</t>
-  </si>
-  <si>
-    <t>172.57549274380636</t>
-  </si>
-  <si>
-    <t>12.660539126261295</t>
-  </si>
-  <si>
-    <t>4.388841788947582</t>
-  </si>
-  <si>
-    <t>1.088457148048107</t>
-  </si>
-  <si>
-    <t>0.5998316696275462</t>
-  </si>
-  <si>
-    <t>0.7228294523030065</t>
-  </si>
-  <si>
-    <t>1.4655634125489743</t>
-  </si>
-  <si>
-    <t>0.5377593733672436</t>
-  </si>
-  <si>
-    <t>0.6903293721388958</t>
-  </si>
-  <si>
-    <t>0.6738866049368115</t>
-  </si>
-  <si>
-    <t>0.9966891949573218</t>
-  </si>
-  <si>
-    <t>0.962885722683825</t>
-  </si>
-  <si>
-    <t>-0.16021838853720138</t>
-  </si>
-  <si>
-    <t>0.6575737903533345</t>
-  </si>
-  <si>
-    <t>0.48096379819536395</t>
-  </si>
-  <si>
-    <t>6.826490145919698</t>
-  </si>
-  <si>
-    <t>0.10099141274332804</t>
-  </si>
-  <si>
-    <t>3.98174165581602</t>
-  </si>
-  <si>
-    <t>0.6898399673888501</t>
-  </si>
-  <si>
-    <t>0.1925401957860826</t>
-  </si>
-  <si>
-    <t>13.652980291839393</t>
-  </si>
-  <si>
-    <t>2.954866606432608</t>
-  </si>
-  <si>
-    <t>1.3693247342489223</t>
-  </si>
-  <si>
-    <t>68671.5137423949</t>
-  </si>
-  <si>
-    <t>0.2428289400061513</t>
-  </si>
-  <si>
-    <t>1.7966738987851096</t>
-  </si>
-  <si>
-    <t>49.21574879957559</t>
-  </si>
-  <si>
-    <t>4.582331567998169</t>
-  </si>
-  <si>
-    <t>215.6703519414641</t>
-  </si>
-  <si>
-    <t>0.10619184365610458</t>
-  </si>
-  <si>
-    <t>0.023567742293106923</t>
-  </si>
-  <si>
-    <t>3.9733715330626604</t>
-  </si>
-  <si>
-    <t>127290.5299291312</t>
-  </si>
-  <si>
-    <t>0.4365920940262392</t>
-  </si>
-  <si>
-    <t>0.5942437323772753</t>
-  </si>
-  <si>
-    <t>1.4771301015039155</t>
-  </si>
-  <si>
-    <t>0.673596109268832</t>
-  </si>
-  <si>
-    <t>33.79024923499775</t>
-  </si>
-  <si>
-    <t>0.015986644061082862</t>
-  </si>
-  <si>
-    <t>1176.734203500445</t>
-  </si>
-  <si>
-    <t>0.17453785278855607</t>
-  </si>
-  <si>
-    <t>6.829376363614444</t>
-  </si>
-  <si>
-    <t>56.35197270839514</t>
-  </si>
-  <si>
-    <t>8483848.059181252</t>
-  </si>
-  <si>
-    <t>377895794.74132305</t>
-  </si>
-  <si>
-    <t>195714.49680142073</t>
-  </si>
-  <si>
-    <t>0.03076395444399087</t>
-  </si>
-  <si>
-    <t>1171.7051320083062</t>
-  </si>
-  <si>
-    <t>0.1737919210928962</t>
-  </si>
-  <si>
-    <t>0.4144265900623371</t>
-  </si>
-  <si>
-    <t>23.63662115538954</t>
-  </si>
-  <si>
-    <t>0.012922954885111531</t>
-  </si>
-  <si>
-    <t>6.4895078020845265</t>
-  </si>
-  <si>
-    <t>0.014171099952286567</t>
-  </si>
-  <si>
-    <t>8478868.477305844</t>
-  </si>
-  <si>
-    <t>-9.165992872964397</t>
-  </si>
-  <si>
-    <t>8.860475549067932</t>
-  </si>
-  <si>
-    <t>23939731.670375668</t>
-  </si>
-  <si>
-    <t>1.010470940433308</t>
-  </si>
-  <si>
-    <t>9.422446499102193</t>
-  </si>
-  <si>
-    <t>3.182781385628776</t>
-  </si>
-  <si>
-    <t>33.9889851847834</t>
-  </si>
-  <si>
-    <t>5.624972199225795</t>
-  </si>
-  <si>
-    <t>-0.1516838787171337</t>
-  </si>
-  <si>
-    <t>-0.11465687353628246</t>
-  </si>
-  <si>
-    <t>-44.12247790825449</t>
-  </si>
-  <si>
-    <t>78.11146309303788</t>
-  </si>
-  <si>
-    <t>3.9105491320338803</t>
-  </si>
-  <si>
-    <t>7.093605720216283</t>
-  </si>
-  <si>
-    <t>-0.058782059670241096</t>
-  </si>
-  <si>
-    <t>0.4991369592855155</t>
-  </si>
-  <si>
-    <t>50.296234114822475</t>
-  </si>
-  <si>
-    <t>6.235080701897656</t>
-  </si>
-  <si>
-    <t>0.5496328664711359</t>
-  </si>
-  <si>
-    <t>0.002546756121776436</t>
-  </si>
-  <si>
-    <t>0.5334587742314525</t>
-  </si>
-  <si>
-    <t>0.473186280534789</t>
-  </si>
-  <si>
-    <t>0.05985913043209482</t>
-  </si>
-  <si>
-    <t>0.4721218924504417</t>
-  </si>
-  <si>
-    <t>0.9781502147725072</t>
-  </si>
-  <si>
-    <t>0.24180170064842724</t>
-  </si>
-  <si>
-    <t>0.7641161994127539</t>
-  </si>
-  <si>
-    <t>0.7640454925832139</t>
-  </si>
-  <si>
-    <t>0.9721843603620702</t>
-  </si>
-  <si>
-    <t>0.9056110722697425</t>
-  </si>
-  <si>
-    <t>-0.02827335492376283</t>
-  </si>
-  <si>
-    <t>0.1792009219578592</t>
-  </si>
-  <si>
-    <t>0.4711929364285338</t>
-  </si>
-  <si>
-    <t>2.4939952059219</t>
-  </si>
-  <si>
-    <t>0.25849556986593797</t>
-  </si>
-  <si>
-    <t>1.9906804534790092</t>
-  </si>
-  <si>
-    <t>0.15409347269830198</t>
-  </si>
-  <si>
-    <t>0.2900374308420174</t>
-  </si>
-  <si>
-    <t>4.987990411843801</t>
-  </si>
-  <si>
-    <t>1.5133431082985638</t>
-  </si>
-  <si>
-    <t>0.25166126369156044</t>
-  </si>
-  <si>
-    <t>117644.07661986111</t>
-  </si>
-  <si>
-    <t>0.4981789598537887</t>
-  </si>
-  <si>
-    <t>0.2536641715854953</t>
-  </si>
-  <si>
-    <t>6.484526426865148</t>
-  </si>
-  <si>
-    <t>7.4486954132328185</t>
-  </si>
-  <si>
-    <t>48.01370094537084</t>
-  </si>
-  <si>
-    <t>1.3574395151725773</t>
-  </si>
-  <si>
-    <t>0.18199014982493564</t>
-  </si>
-  <si>
-    <t>3.047327548424032</t>
-  </si>
-  <si>
-    <t>80812.49301128995</t>
-  </si>
-  <si>
-    <t>0.3305449382066783</t>
-  </si>
-  <si>
-    <t>0.49632092401405303</t>
-  </si>
-  <si>
-    <t>2.5866831534233556</t>
-  </si>
-  <si>
-    <t>0.5670548846223463</t>
-  </si>
-  <si>
-    <t>3.687255214464067</t>
-  </si>
-  <si>
-    <t>0.10329688782064365</t>
-  </si>
-  <si>
-    <t>125.73962264150943</t>
-  </si>
-  <si>
-    <t>0.47448914204343184</t>
-  </si>
-  <si>
-    <t>1.8300605197579207</t>
-  </si>
-  <si>
-    <t>5.875471698113207</t>
-  </si>
-  <si>
-    <t>426277967.13584906</t>
-  </si>
-  <si>
-    <t>2744531737.0867925</t>
-  </si>
-  <si>
-    <t>77696721.58142033</t>
-  </si>
-  <si>
-    <t>0.6548218029350105</t>
-  </si>
-  <si>
-    <t>116.28301886792453</t>
-  </si>
-  <si>
-    <t>0.43880384478462087</t>
-  </si>
-  <si>
-    <t>0.6837504066690014</t>
-  </si>
-  <si>
-    <t>4.6431424402127215</t>
-  </si>
-  <si>
-    <t>0.4051243002165273</t>
-  </si>
-  <si>
-    <t>2.9270180572205096</t>
-  </si>
-  <si>
-    <t>0.0005570070435117087</t>
-  </si>
-  <si>
-    <t>423054831.1721751</t>
-  </si>
-  <si>
-    <t>-10.611621888380892</t>
-  </si>
-  <si>
-    <t>10.509381641972013</t>
-  </si>
-  <si>
-    <t>33000846.0622713</t>
-  </si>
-  <si>
-    <t>1.0367621538313903</t>
-  </si>
-  <si>
-    <t>11.053134890126376</t>
-  </si>
-  <si>
-    <t>3.178686523907576</t>
-  </si>
-  <si>
-    <t>48.28213267991815</t>
-  </si>
-  <si>
-    <t>6.598383710770853</t>
-  </si>
-  <si>
-    <t>-0.0390591531811597</t>
-  </si>
-  <si>
-    <t>-0.025354989992689314</t>
-  </si>
-  <si>
-    <t>-42.652394371450264</t>
-  </si>
-  <si>
-    <t>90.9345270513684</t>
-  </si>
-  <si>
-    <t>4.5792917394235735</t>
-  </si>
-  <si>
-    <t>8.328560476882975</t>
-  </si>
-  <si>
-    <t>-0.006474319237158798</t>
-  </si>
-  <si>
-    <t>0.496125226311063</t>
-  </si>
-  <si>
-    <t>69.36339399964994</t>
-  </si>
-  <si>
-    <t>6.250882172818931</t>
-  </si>
-  <si>
-    <t>0.5792762308787864</t>
-  </si>
-  <si>
-    <t>0.000819051548952715</t>
-  </si>
-  <si>
-    <t>0.5284825965689064</t>
-  </si>
-  <si>
-    <t>0.502347842258236</t>
-  </si>
-  <si>
-    <t>0.025355268242114943</t>
-  </si>
-  <si>
-    <t>0.49449547755693773</t>
-  </si>
-  <si>
-    <t>1.010866608795705</t>
-  </si>
-  <si>
-    <t>0.250534465568057</t>
-  </si>
-  <si>
-    <t>0.7540499468278803</t>
-  </si>
-  <si>
-    <t>0.7535374976916608</t>
-  </si>
-  <si>
-    <t>0.9705915039951564</t>
-  </si>
-  <si>
-    <t>0.9013613880536424</t>
-  </si>
-  <si>
-    <t>-0.02250799945593966</t>
-  </si>
-  <si>
-    <t>0.11197871436692079</t>
-  </si>
-  <si>
-    <t>0.4877289425242697</t>
-  </si>
-  <si>
-    <t>2.4988693805963917</t>
-  </si>
-  <si>
-    <t>0.2533858800073956</t>
-  </si>
-  <si>
-    <t>2.0495845696766355</t>
-  </si>
-  <si>
-    <t>0.09616408524925714</t>
-  </si>
-  <si>
-    <t>0.2710971563088044</t>
-  </si>
-  <si>
-    <t>4.997738761192784</t>
-  </si>
-  <si>
-    <t>1.5270041586809069</t>
-  </si>
-  <si>
-    <t>0.25770760970678563</t>
-  </si>
-  <si>
-    <t>120569.0881865708</t>
-  </si>
-  <si>
-    <t>0.4925082326923277</t>
-  </si>
-  <si>
-    <t>0.26510300584487395</t>
-  </si>
-  <si>
-    <t>6.512864967453327</t>
-  </si>
-  <si>
-    <t>6.541314794547187</t>
-  </si>
-  <si>
-    <t>42.4687806861742</t>
-  </si>
-  <si>
-    <t>1.1860320070037973</t>
-  </si>
-  <si>
-    <t>0.18328628709346695</t>
-  </si>
-  <si>
-    <t>2.9843906151333846</t>
-  </si>
-  <si>
-    <t>88772.938414975</t>
-  </si>
-  <si>
-    <t>0.35248050847689366</t>
-  </si>
-  <si>
-    <t>0.5143828273030786</t>
-  </si>
-  <si>
-    <t>2.093981099955654</t>
-  </si>
-  <si>
-    <t>0.5726328653920507</t>
-  </si>
-  <si>
-    <t>3.7383702324154973</t>
-  </si>
-  <si>
-    <t>0.10593141289838567</t>
-  </si>
-  <si>
-    <t>627.3359133126935</t>
-  </si>
-  <si>
-    <t>0.485554112471125</t>
-  </si>
-  <si>
-    <t>2.2204708182767976</t>
-  </si>
-  <si>
-    <t>8.41640866873065</t>
-  </si>
-  <si>
-    <t>86907232.30882353</t>
-  </si>
-  <si>
-    <t>563856265.3537152</t>
-  </si>
-  <si>
-    <t>15720494.25660582</t>
-  </si>
-  <si>
-    <t>0.5298148864809081</t>
-  </si>
-  <si>
-    <t>646.077399380805</t>
-  </si>
-  <si>
-    <t>0.5000599066414899</t>
-  </si>
-  <si>
-    <t>0.7227176188458115</t>
-  </si>
-  <si>
-    <t>6.110920027002208</t>
-  </si>
-  <si>
-    <t>0.38062584777454367</t>
-  </si>
-  <si>
-    <t>2.375943935012831</t>
-  </si>
-  <si>
-    <t>0.002715672076291048</t>
-  </si>
-  <si>
-    <t>86771636.78705525</t>
-  </si>
-  <si>
-    <t>-4.29771125600908</t>
-  </si>
-  <si>
-    <t>4.303904038255883</t>
-  </si>
-  <si>
-    <t>5440812.246745688</t>
-  </si>
-  <si>
-    <t>0.9999999896456244</t>
-  </si>
-  <si>
-    <t>4.496668277784636</t>
-  </si>
-  <si>
-    <t>3.1473224211003714</t>
-  </si>
-  <si>
-    <t>17.614037531180582</t>
-  </si>
-  <si>
-    <t>2.6829748974001064</t>
-  </si>
-  <si>
-    <t>0.0010798253786178985</t>
-  </si>
-  <si>
-    <t>0.0005497294538947192</t>
-  </si>
-  <si>
-    <t>-17.729201954663594</t>
-  </si>
-  <si>
-    <t>35.34323948584418</t>
-  </si>
-  <si>
-    <t>1.8650852085013983</t>
-  </si>
-  <si>
-    <t>3.381732694133883</t>
-  </si>
-  <si>
-    <t>0.0006420238443508034</t>
-  </si>
-  <si>
-    <t>0.5000000071771056</t>
-  </si>
-  <si>
-    <t>11.436114848551167</t>
-  </si>
-  <si>
-    <t>2.2477173139553233</t>
-  </si>
-  <si>
-    <t>0.494424564072748</t>
-  </si>
-  <si>
-    <t>-0.00014667280791308412</t>
-  </si>
-  <si>
-    <t>0.49442460159206486</t>
-  </si>
-  <si>
-    <t>0.5055751371093273</t>
-  </si>
-  <si>
-    <t>-0.011150548023719061</t>
-  </si>
-  <si>
-    <t>0.9945432466347176</t>
-  </si>
-  <si>
-    <t>0.24811553408687093</t>
-  </si>
-  <si>
-    <t>0.7472124314453364</t>
-  </si>
-  <si>
-    <t>0.8988849725781345</t>
-  </si>
-  <si>
-    <t>0.8314749542968909</t>
-  </si>
-  <si>
-    <t>-0.0054567740168200655</t>
-  </si>
-  <si>
-    <t>0.08405098272926684</t>
-  </si>
-  <si>
-    <t>1.5001682941699956</t>
-  </si>
-  <si>
-    <t>0.251884596562433</t>
-  </si>
-  <si>
-    <t>1.9945428496397564</t>
-  </si>
-  <si>
-    <t>0.07026208118413581</t>
-  </si>
-  <si>
-    <t>0.2676112129791083</t>
-  </si>
-  <si>
-    <t>3.0003365883399913</t>
-  </si>
-  <si>
-    <t>1.4889677125304293</t>
-  </si>
-  <si>
-    <t>0.24999993467534803</t>
-  </si>
-  <si>
-    <t>125819.72947356783</t>
-  </si>
-  <si>
-    <t>0.5000002908742549</t>
-  </si>
-  <si>
-    <t>0.24999985456287252</t>
-  </si>
-  <si>
-    <t>2.49945071108083</t>
-  </si>
-  <si>
-    <t>5.383664115203465</t>
-  </si>
-  <si>
-    <t>13.46463868550998</t>
-  </si>
-  <si>
-    <t>3.3634204726268355</t>
-  </si>
-  <si>
-    <t>0.6251373222297925</t>
-  </si>
-  <si>
-    <t>2.8656986345324373</t>
-  </si>
-  <si>
-    <t>90855.50748778234</t>
-  </si>
-  <si>
-    <t>0.36014198145417187</t>
-  </si>
-  <si>
-    <t>0.5289240256944358</t>
-  </si>
-  <si>
-    <t>1.7474785794497785</t>
-  </si>
-  <si>
-    <t>0.6038159080288475</t>
-  </si>
-  <si>
-    <t>1.5086245599322785</t>
-  </si>
-  <si>
-    <t>0.37761374505298984</t>
+    <t>(246, 258, 213)</t>
+  </si>
+  <si>
+    <t>78cd76bca29745a9da351ea971d4702af8137da5</t>
+  </si>
+  <si>
+    <t>(42, 56, 51, 156, 156, 113)</t>
+  </si>
+  <si>
+    <t>(111.63374604361135, 134.81030939866048, 119.09376266556905)</t>
+  </si>
+  <si>
+    <t>157.2768260107</t>
+  </si>
+  <si>
+    <t>175.31685600648902</t>
+  </si>
+  <si>
+    <t>162.63148526653748</t>
+  </si>
+  <si>
+    <t>175.95738120351757</t>
+  </si>
+  <si>
+    <t>633942.875</t>
+  </si>
+  <si>
+    <t>0.47120025903245777</t>
+  </si>
+  <si>
+    <t>75737.68401621885</t>
+  </si>
+  <si>
+    <t>0.11947083404986426</t>
+  </si>
+  <si>
+    <t>-597.0000000000001</t>
+  </si>
+  <si>
+    <t>-301.00000000000045</t>
+  </si>
+  <si>
+    <t>155092235155.00003</t>
+  </si>
+  <si>
+    <t>3.948354718350135</t>
+  </si>
+  <si>
+    <t>149.99999999999994</t>
+  </si>
+  <si>
+    <t>2.76407940177534</t>
+  </si>
+  <si>
+    <t>-186.99999999999972</t>
+  </si>
+  <si>
+    <t>90.2349721624063</t>
+  </si>
+  <si>
+    <t>-482.066353782757</t>
+  </si>
+  <si>
+    <t>-514.0000000000002</t>
+  </si>
+  <si>
+    <t>-893.0000000000001</t>
+  </si>
+  <si>
+    <t>706.0000000000005</t>
+  </si>
+  <si>
+    <t>64.37506827114444</t>
+  </si>
+  <si>
+    <t>494.5563795639468</t>
+  </si>
+  <si>
+    <t>0.7839677757162534</t>
+  </si>
+  <si>
+    <t>0.07783573582178754</t>
+  </si>
+  <si>
+    <t>12198.04311799634</t>
+  </si>
+  <si>
+    <t>300.7281269559176</t>
+  </si>
+  <si>
+    <t>12454.359374943084</t>
+  </si>
+  <si>
+    <t>424.77649417615856</t>
+  </si>
+  <si>
+    <t>65.55601328132404</t>
+  </si>
+  <si>
+    <t>4.407194210570112</t>
+  </si>
+  <si>
+    <t>0.8733146313840882</t>
+  </si>
+  <si>
+    <t>1.441350843235845</t>
+  </si>
+  <si>
+    <t>2.2471249675846448</t>
+  </si>
+  <si>
+    <t>2.266870511229475</t>
+  </si>
+  <si>
+    <t>0.5539290307599682</t>
+  </si>
+  <si>
+    <t>0.5069120415268629</t>
+  </si>
+  <si>
+    <t>0.9949208965286106</t>
+  </si>
+  <si>
+    <t>0.9548509783875705</t>
+  </si>
+  <si>
+    <t>-0.27882629014514376</t>
+  </si>
+  <si>
+    <t>0.9347611074479393</t>
+  </si>
+  <si>
+    <t>0.4454091209660392</t>
+  </si>
+  <si>
+    <t>16.894904196462925</t>
+  </si>
+  <si>
+    <t>0.01680818698560138</t>
+  </si>
+  <si>
+    <t>6.699472098797829</t>
+  </si>
+  <si>
+    <t>0.8806131359273489</t>
+  </si>
+  <si>
+    <t>0.04898633647445115</t>
+  </si>
+  <si>
+    <t>33.78980839292586</t>
+  </si>
+  <si>
+    <t>4.847002946568311</t>
+  </si>
+  <si>
+    <t>17.490801872973535</t>
+  </si>
+  <si>
+    <t>33589.65811618929</t>
+  </si>
+  <si>
+    <t>0.07110348097851486</t>
+  </si>
+  <si>
+    <t>20.59025619425747</t>
+  </si>
+  <si>
+    <t>332.1331281167526</t>
+  </si>
+  <si>
+    <t>2.4035403114967555</t>
+  </si>
+  <si>
+    <t>700.9831122360966</t>
+  </si>
+  <si>
+    <t>0.010338729539239413</t>
+  </si>
+  <si>
+    <t>0.003906780614892993</t>
+  </si>
+  <si>
+    <t>5.079509038573013</t>
+  </si>
+  <si>
+    <t>293450.24689926446</t>
+  </si>
+  <si>
+    <t>0.6189678938851076</t>
+  </si>
+  <si>
+    <t>0.7446799605935138</t>
+  </si>
+  <si>
+    <t>0.5830450733009109</t>
+  </si>
+  <si>
+    <t>0.8142420407631377</t>
+  </si>
+  <si>
+    <t>281.33090151404184</t>
+  </si>
+  <si>
+    <t>0.003073839964502215</t>
+  </si>
+  <si>
+    <t>2218.844123008173</t>
+  </si>
+  <si>
+    <t>0.06523326051061837</t>
+  </si>
+  <si>
+    <t>21.635914464351817</t>
+  </si>
+  <si>
+    <t>477.9721291233022</t>
+  </si>
+  <si>
+    <t>505954.72808255424</t>
+  </si>
+  <si>
+    <t>122817954.12668313</t>
+  </si>
+  <si>
+    <t>2265.2755735184714</t>
+  </si>
+  <si>
+    <t>0.002842147499864418</t>
+  </si>
+  <si>
+    <t>9474.891103663198</t>
+  </si>
+  <si>
+    <t>0.27855856716831884</t>
+  </si>
+  <si>
+    <t>0.5401381787223664</t>
+  </si>
+  <si>
+    <t>263.89267911744713</t>
+  </si>
+  <si>
+    <t>0.0014683433221502</t>
+  </si>
+  <si>
+    <t>6.749649144126846</t>
+  </si>
+  <si>
+    <t>0.05364129689118926</t>
+  </si>
+  <si>
+    <t>505607.19075163326</t>
+  </si>
+  <si>
+    <t>-23.802043945541644</t>
+  </si>
+  <si>
+    <t>37.73937003600093</t>
+  </si>
+  <si>
+    <t>507021955.80751806</t>
+  </si>
+  <si>
+    <t>2.1593196072366054</t>
+  </si>
+  <si>
+    <t>30.173766742496568</t>
+  </si>
+  <si>
+    <t>6.2704808238147525</t>
+  </si>
+  <si>
+    <t>235.67542878079954</t>
+  </si>
+  <si>
+    <t>20.104050531492526</t>
+  </si>
+  <si>
+    <t>6.345136629707502</t>
+  </si>
+  <si>
+    <t>4.506504707707242</t>
+  </si>
+  <si>
+    <t>-180.98238681364526</t>
+  </si>
+  <si>
+    <t>416.6578155944448</t>
+  </si>
+  <si>
+    <t>12.699921698977501</t>
+  </si>
+  <si>
+    <t>28.277054185908018</t>
+  </si>
+  <si>
+    <t>0.7664260312622594</t>
+  </si>
+  <si>
+    <t>0.28331334449919204</t>
+  </si>
+  <si>
+    <t>759.3310345831223</t>
+  </si>
+  <si>
+    <t>77.37575157531136</t>
+  </si>
+  <si>
+    <t>106.26499376052955</t>
+  </si>
+  <si>
+    <t>7.122988317749104</t>
+  </si>
+  <si>
+    <t>3.9713949614723636</t>
+  </si>
+  <si>
+    <t>1.0663105235092185</t>
+  </si>
+  <si>
+    <t>0.5751030467807323</t>
+  </si>
+  <si>
+    <t>0.7186566030257784</t>
+  </si>
+  <si>
+    <t>1.4566926440655785</t>
+  </si>
+  <si>
+    <t>0.522133803025704</t>
+  </si>
+  <si>
+    <t>0.6908579433621042</t>
+  </si>
+  <si>
+    <t>0.6745966507018097</t>
+  </si>
+  <si>
+    <t>0.9967522105506238</t>
+  </si>
+  <si>
+    <t>0.9630642862361807</t>
+  </si>
+  <si>
+    <t>-0.15482357671027475</t>
+  </si>
+  <si>
+    <t>0.6457656976247741</t>
+  </si>
+  <si>
+    <t>0.481850420513319</t>
+  </si>
+  <si>
+    <t>8.754968623567224</t>
+  </si>
+  <si>
+    <t>0.1034085821821519</t>
+  </si>
+  <si>
+    <t>3.9474453638499702</t>
+  </si>
+  <si>
+    <t>0.6729223318424388</t>
+  </si>
+  <si>
+    <t>0.19256830604034667</t>
+  </si>
+  <si>
+    <t>17.50993724713445</t>
+  </si>
+  <si>
+    <t>2.919839211896208</t>
+  </si>
+  <si>
+    <t>1.2594263712453952</t>
+  </si>
+  <si>
+    <t>93524.63976618249</t>
+  </si>
+  <si>
+    <t>0.24968387476707146</t>
+  </si>
+  <si>
+    <t>1.5888174919777047</t>
+  </si>
+  <si>
+    <t>78.65789456306787</t>
+  </si>
+  <si>
+    <t>4.659916832952112</t>
+  </si>
+  <si>
+    <t>359.0439260867739</t>
+  </si>
+  <si>
+    <t>0.06360334845095553</t>
+  </si>
+  <si>
+    <t>0.01381618815347591</t>
+  </si>
+  <si>
+    <t>3.942256793366304</t>
+  </si>
+  <si>
+    <t>167335.1979325648</t>
+  </si>
+  <si>
+    <t>0.43301213740905015</t>
+  </si>
+  <si>
+    <t>0.5907800662185216</t>
+  </si>
+  <si>
+    <t>1.513060433986883</t>
+  </si>
+  <si>
+    <t>0.6704445475416587</t>
+  </si>
+  <si>
+    <t>53.16012003704361</t>
+  </si>
+  <si>
+    <t>0.009315608850398335</t>
+  </si>
+  <si>
+    <t>1852.2221082621083</t>
+  </si>
+  <si>
+    <t>0.2110794425369924</t>
+  </si>
+  <si>
+    <t>5.015463108253992</t>
+  </si>
+  <si>
+    <t>79.71430199430199</t>
+  </si>
+  <si>
+    <t>12106141.206723647</t>
+  </si>
+  <si>
+    <t>908128670.1747009</t>
+  </si>
+  <si>
+    <t>164110.00271116046</t>
+  </si>
+  <si>
+    <t>0.01649157942664722</t>
+  </si>
+  <si>
+    <t>1474.8582336182337</t>
+  </si>
+  <si>
+    <t>0.1680750123781463</t>
+  </si>
+  <si>
+    <t>0.4055166846177399</t>
+  </si>
+  <si>
+    <t>32.30367144880942</t>
+  </si>
+  <si>
+    <t>0.006781195092154824</t>
+  </si>
+  <si>
+    <t>6.277797286089917</t>
+  </si>
+  <si>
+    <t>0.013838489451995818</t>
+  </si>
+  <si>
+    <t>12100919.377963152</t>
+  </si>
+  <si>
+    <t>-28.745129560316553</t>
+  </si>
+  <si>
+    <t>33.02721570534765</t>
+  </si>
+  <si>
+    <t>383907805.1723418</t>
+  </si>
+  <si>
+    <t>2.077123596139603</t>
+  </si>
+  <si>
+    <t>32.24500278451681</t>
+  </si>
+  <si>
+    <t>3.3312406355114264</t>
+  </si>
+  <si>
+    <t>154.5555001613982</t>
+  </si>
+  <si>
+    <t>19.355082166037622</t>
+  </si>
+  <si>
+    <t>2.0666504461338553</t>
+  </si>
+  <si>
+    <t>1.9450135480506112</t>
+  </si>
+  <si>
+    <t>-136.62629769982587</t>
+  </si>
+  <si>
+    <t>291.181797861224</t>
+  </si>
+  <si>
+    <t>13.381603125962851</t>
+  </si>
+  <si>
+    <t>24.605616555724218</t>
+  </si>
+  <si>
+    <t>0.041110025349176474</t>
+  </si>
+  <si>
+    <t>0.27979032340783744</t>
+  </si>
+  <si>
+    <t>601.1653220208242</t>
+  </si>
+  <si>
+    <t>43.47545574329359</t>
+  </si>
+  <si>
+    <t>20.986054972153674</t>
+  </si>
+  <si>
+    <t>0.1524616199861179</t>
+  </si>
+  <si>
+    <t>2.4190384421108564</t>
+  </si>
+  <si>
+    <t>1.715685683660816</t>
+  </si>
+  <si>
+    <t>0.1698558807053826</t>
+  </si>
+  <si>
+    <t>0.9575234813438821</t>
+  </si>
+  <si>
+    <t>1.701484917604896</t>
+  </si>
+  <si>
+    <t>0.7463145256324624</t>
+  </si>
+  <si>
+    <t>0.6251042544833625</t>
+  </si>
+  <si>
+    <t>0.594709504596057</t>
+  </si>
+  <si>
+    <t>0.9901955401190604</t>
+  </si>
+  <si>
+    <t>0.9350364449830941</t>
+  </si>
+  <si>
+    <t>-0.05496570168882383</t>
+  </si>
+  <si>
+    <t>0.27335770648447555</t>
+  </si>
+  <si>
+    <t>0.49019448922181624</t>
+  </si>
+  <si>
+    <t>6.58024443271626</t>
+  </si>
+  <si>
+    <t>0.08669006395714215</t>
+  </si>
+  <si>
+    <t>4.025334226859448</t>
+  </si>
+  <si>
+    <t>0.24814397477804986</t>
+  </si>
+  <si>
+    <t>0.14852067856225828</t>
+  </si>
+  <si>
+    <t>13.16048886543252</t>
+  </si>
+  <si>
+    <t>2.658126748443304</t>
+  </si>
+  <si>
+    <t>1.0336810314429183</t>
+  </si>
+  <si>
+    <t>108171.48292388588</t>
+  </si>
+  <si>
+    <t>0.25197866958256304</t>
+  </si>
+  <si>
+    <t>1.2392355174474476</t>
+  </si>
+  <si>
+    <t>44.60042752008946</t>
+  </si>
+  <si>
+    <t>3.2048264376315654</t>
+  </si>
+  <si>
+    <t>141.2532551075798</t>
+  </si>
+  <si>
+    <t>0.07864341205531339</t>
+  </si>
+  <si>
+    <t>0.025380697380637543</t>
+  </si>
+  <si>
+    <t>3.482916452039593</t>
+  </si>
+  <si>
+    <t>233366.45002565827</t>
+  </si>
+  <si>
+    <t>0.5308709599328777</t>
+  </si>
+  <si>
+    <t>0.6779298566001315</t>
+  </si>
+  <si>
+    <t>0.8959082379411013</t>
+  </si>
+  <si>
+    <t>0.749210633891904</t>
+  </si>
+  <si>
+    <t>33.557492433784795</t>
+  </si>
+  <si>
+    <t>0.019253378385653927</t>
+  </si>
+  <si>
+    <t>3505.6081871345027</t>
+  </si>
+  <si>
+    <t>0.21354825701355404</t>
+  </si>
+  <si>
+    <t>4.948249831708663</t>
+  </si>
+  <si>
+    <t>48.130665204678365</t>
+  </si>
+  <si>
+    <t>6368287.65625</t>
+  </si>
+  <si>
+    <t>279808899.89175195</t>
+  </si>
+  <si>
+    <t>149662.95759199795</t>
+  </si>
+  <si>
+    <t>0.03385349571209013</t>
+  </si>
+  <si>
+    <t>3292.71418128655</t>
+  </si>
+  <si>
+    <t>0.2005795675734984</t>
+  </si>
+  <si>
+    <t>0.43841722735350214</t>
+  </si>
+  <si>
+    <t>21.36812517744667</t>
+  </si>
+  <si>
+    <t>0.015397461797092662</t>
+  </si>
+  <si>
+    <t>5.510851895615469</t>
+  </si>
+  <si>
+    <t>0.02588862026711833</t>
+  </si>
+  <si>
+    <t>6366795.610330389</t>
+  </si>
+  <si>
+    <t>-11.087691509011936</t>
+  </si>
+  <si>
+    <t>10.980828375674433</t>
+  </si>
+  <si>
+    <t>48403436.118667535</t>
+  </si>
+  <si>
+    <t>1.0542230352763142</t>
+  </si>
+  <si>
+    <t>11.499111255558331</t>
+  </si>
+  <si>
+    <t>3.262530269635994</t>
+  </si>
+  <si>
+    <t>48.55049498786686</t>
+  </si>
+  <si>
+    <t>6.900096939079274</t>
+  </si>
+  <si>
+    <t>-0.046360363733741916</t>
+  </si>
+  <si>
+    <t>-0.024795945960860016</t>
+  </si>
+  <si>
+    <t>-55.11847347241785</t>
+  </si>
+  <si>
+    <t>103.6689684602847</t>
+  </si>
+  <si>
+    <t>4.768791403070438</t>
+  </si>
+  <si>
+    <t>8.736930427533428</t>
+  </si>
+  <si>
+    <t>-0.013071028999716678</t>
+  </si>
+  <si>
+    <t>0.4938679580038794</t>
+  </si>
+  <si>
+    <t>76.33180401223389</t>
+  </si>
+  <si>
+    <t>12.246001479489992</t>
+  </si>
+  <si>
+    <t>0.6189694012194006</t>
+  </si>
+  <si>
+    <t>-0.0007116387037494264</t>
+  </si>
+  <si>
+    <t>0.5367209936571614</t>
+  </si>
+  <si>
+    <t>0.5118317254986441</t>
+  </si>
+  <si>
+    <t>0.02374287481983993</t>
+  </si>
+  <si>
+    <t>0.4994093778073816</t>
+  </si>
+  <si>
+    <t>1.0251499977775398</t>
+  </si>
+  <si>
+    <t>0.25480446497314574</t>
+  </si>
+  <si>
+    <t>0.752340317521779</t>
+  </si>
+  <si>
+    <t>0.7515374038475191</t>
+  </si>
+  <si>
+    <t>0.980416460051866</t>
+  </si>
+  <si>
+    <t>0.917059054290817</t>
+  </si>
+  <si>
+    <t>-0.023427723196821824</t>
+  </si>
+  <si>
+    <t>0.11718680274566529</t>
+  </si>
+  <si>
+    <t>0.48877857046919176</t>
+  </si>
+  <si>
+    <t>3.498539551814555</t>
+  </si>
+  <si>
+    <t>0.2513952978010319</t>
+  </si>
+  <si>
+    <t>2.0821215542943183</t>
+  </si>
+  <si>
+    <t>0.10068284992747746</t>
+  </si>
+  <si>
+    <t>0.2703705980946153</t>
+  </si>
+  <si>
+    <t>6.99707910362911</t>
+  </si>
+  <si>
+    <t>1.5425009517393475</t>
+  </si>
+  <si>
+    <t>0.26213817978895143</t>
+  </si>
+  <si>
+    <t>158903.61911581864</t>
+  </si>
+  <si>
+    <t>0.4882324278500002</t>
+  </si>
+  <si>
+    <t>0.27386340874599024</t>
+  </si>
+  <si>
+    <t>12.51768885914716</t>
+  </si>
+  <si>
+    <t>6.567383364299527</t>
+  </si>
+  <si>
+    <t>82.02250811416886</t>
+  </si>
+  <si>
+    <t>0.5716227555604081</t>
+  </si>
+  <si>
+    <t>0.08756382998509506</t>
+  </si>
+  <si>
+    <t>3.014426779569026</t>
+  </si>
+  <si>
+    <t>117729.05804153203</t>
+  </si>
+  <si>
+    <t>0.3513378187949874</t>
+  </si>
+  <si>
+    <t>0.5130118193983414</t>
+  </si>
+  <si>
+    <t>2.072701642012365</t>
+  </si>
+  <si>
+    <t>0.5708647451655473</t>
+  </si>
+  <si>
+    <t>7.157808591860812</t>
+  </si>
+  <si>
+    <t>0.05024930025324467</t>
+  </si>
+  <si>
+    <t>1244.4317637669592</t>
+  </si>
+  <si>
+    <t>0.4965809113196166</t>
+  </si>
+  <si>
+    <t>2.2491280304762586</t>
+  </si>
+  <si>
+    <t>14.293296089385475</t>
+  </si>
+  <si>
+    <t>79233832.23503591</t>
+  </si>
+  <si>
+    <t>989196885.4397446</t>
+  </si>
+  <si>
+    <t>6886451.085715727</t>
+  </si>
+  <si>
+    <t>0.14775028819721558</t>
+  </si>
+  <si>
+    <t>1140.491620111732</t>
+  </si>
+  <si>
+    <t>0.455104397490715</t>
+  </si>
+  <si>
+    <t>0.6854237376278367</t>
+  </si>
+  <si>
+    <t>9.861159380060393</t>
+  </si>
+  <si>
+    <t>0.10095381250217488</t>
+  </si>
+  <si>
+    <t>2.4841103260253745</t>
+  </si>
+  <si>
+    <t>0.003952051802473108</t>
+  </si>
+  <si>
+    <t>79169806.4749605</t>
+  </si>
+  <si>
+    <t>-22.67817591859521</t>
+  </si>
+  <si>
+    <t>38.067884379103745</t>
+  </si>
+  <si>
+    <t>493506298.9071958</t>
+  </si>
+  <si>
+    <t>2.1237258978762643</t>
+  </si>
+  <si>
+    <t>29.433196021636462</t>
+  </si>
+  <si>
+    <t>7.181622258796556</t>
+  </si>
+  <si>
+    <t>260.4795103636354</t>
+  </si>
+  <si>
+    <t>19.675878180664967</t>
+  </si>
+  <si>
+    <t>6.724596475141107</t>
+  </si>
+  <si>
+    <t>4.500726354926022</t>
+  </si>
+  <si>
+    <t>-138.44190065775788</t>
+  </si>
+  <si>
+    <t>398.9214110213933</t>
+  </si>
+  <si>
+    <t>12.416671663725875</t>
+  </si>
+  <si>
+    <t>27.89761850351395</t>
+  </si>
+  <si>
+    <t>1.002817681345296</t>
+  </si>
+  <si>
+    <t>0.2894573142804702</t>
+  </si>
+  <si>
+    <t>733.0569204141241</t>
+  </si>
+  <si>
+    <t>46.36749807522014</t>
+  </si>
+  <si>
+    <t>107.61498455241615</t>
+  </si>
+  <si>
+    <t>7.935308109439703</t>
+  </si>
+  <si>
+    <t>3.7833086502892703</t>
+  </si>
+  <si>
+    <t>1.0054144704141572</t>
+  </si>
+  <si>
+    <t>0.5775673747944002</t>
+  </si>
+  <si>
+    <t>0.69480454449174</t>
+  </si>
+  <si>
+    <t>1.4261292721343983</t>
+  </si>
+  <si>
+    <t>0.496880190445423</t>
+  </si>
+  <si>
+    <t>0.6978840935337259</t>
+  </si>
+  <si>
+    <t>0.6829365614990797</t>
+  </si>
+  <si>
+    <t>0.9965694540182116</t>
+  </si>
+  <si>
+    <t>0.9622819207909856</t>
+  </si>
+  <si>
+    <t>-0.15702725692842887</t>
+  </si>
+  <si>
+    <t>0.6442935745455287</t>
+  </si>
+  <si>
+    <t>0.47921059990143944</t>
+  </si>
+  <si>
+    <t>6.758179700552627</t>
+  </si>
+  <si>
+    <t>0.10889029676090067</t>
+  </si>
+  <si>
+    <t>3.8598848361069362</t>
+  </si>
+  <si>
+    <t>0.6610663149909844</t>
+  </si>
+  <si>
+    <t>0.19886089567305218</t>
+  </si>
+  <si>
+    <t>13.516359401105252</t>
+  </si>
+  <si>
+    <t>2.8765166434120704</t>
+  </si>
+  <si>
+    <t>1.1971807801758567</t>
+  </si>
+  <si>
+    <t>93351.98781297336</t>
+  </si>
+  <si>
+    <t>0.25342693002554467</t>
+  </si>
+  <si>
+    <t>1.5680230082475906</t>
+  </si>
+  <si>
+    <t>47.92047891446311</t>
+  </si>
+  <si>
+    <t>4.87135472185848</t>
+  </si>
+  <si>
+    <t>224.76780041239604</t>
+  </si>
+  <si>
+    <t>0.11433734269843149</t>
+  </si>
+  <si>
+    <t>0.023901847418799114</t>
+  </si>
+  <si>
+    <t>3.951311981156456</t>
+  </si>
+  <si>
+    <t>160720.883217656</t>
+  </si>
+  <si>
+    <t>0.42250475626550954</t>
+  </si>
+  <si>
+    <t>0.5808680320642925</t>
+  </si>
+  <si>
+    <t>1.6016825473192262</t>
+  </si>
+  <si>
+    <t>0.6607243127507572</t>
+  </si>
+  <si>
+    <t>32.189109638534816</t>
+  </si>
+  <si>
+    <t>0.015918003301791942</t>
+  </si>
+  <si>
+    <t>1741.7410870835768</t>
+  </si>
+  <si>
+    <t>0.20359334740895113</t>
+  </si>
+  <si>
+    <t>5.575782049044225</t>
+  </si>
+  <si>
+    <t>53.27212156633548</t>
+  </si>
+  <si>
+    <t>12632665.32238457</t>
+  </si>
+  <si>
+    <t>557032315.926242</t>
+  </si>
+  <si>
+    <t>294179.3671450702</t>
+  </si>
+  <si>
+    <t>0.030284256398936008</t>
+  </si>
+  <si>
+    <t>1390.1967270601988</t>
+  </si>
+  <si>
+    <t>0.1625010785575919</t>
+  </si>
+  <si>
+    <t>0.39700273598976077</t>
+  </si>
+  <si>
+    <t>21.251309565133074</t>
+  </si>
+  <si>
+    <t>0.012152459509410804</t>
+  </si>
+  <si>
+    <t>6.4034360243300705</t>
+  </si>
+  <si>
+    <t>0.013491541568299056</t>
+  </si>
+  <si>
+    <t>12627171.471741641</t>
+  </si>
+  <si>
+    <t>-8.809608232869971</t>
+  </si>
+  <si>
+    <t>8.53316187328064</t>
+  </si>
+  <si>
+    <t>29432211.11180527</t>
+  </si>
+  <si>
+    <t>1.0065760897469374</t>
+  </si>
+  <si>
+    <t>9.090990169609945</t>
+  </si>
+  <si>
+    <t>3.1402730265371184</t>
+  </si>
+  <si>
+    <t>33.829369787743516</t>
+  </si>
+  <si>
+    <t>5.410598494670352</t>
+  </si>
+  <si>
+    <t>-0.1303854314743861</t>
+  </si>
+  <si>
+    <t>-0.0977268531605957</t>
+  </si>
+  <si>
+    <t>-43.846870401755375</t>
+  </si>
+  <si>
+    <t>77.67624018949888</t>
+  </si>
+  <si>
+    <t>3.768495457704781</t>
+  </si>
+  <si>
+    <t>6.812903318422244</t>
+  </si>
+  <si>
+    <t>-0.044406226524763774</t>
+  </si>
+  <si>
+    <t>0.4995148451528526</t>
+  </si>
+  <si>
+    <t>46.398651265428065</t>
+  </si>
+  <si>
+    <t>6.2382646726666255</t>
+  </si>
+  <si>
+    <t>0.5409473239020136</t>
+  </si>
+  <si>
+    <t>0.0040998360614003864</t>
+  </si>
+  <si>
+    <t>0.5320418427218232</t>
+  </si>
+  <si>
+    <t>0.471858445715077</t>
+  </si>
+  <si>
+    <t>0.0599426098358187</t>
+  </si>
+  <si>
+    <t>0.4712001875697342</t>
+  </si>
+  <si>
+    <t>0.9772088785699782</t>
+  </si>
+  <si>
+    <t>0.24175660686716666</t>
+  </si>
+  <si>
+    <t>0.7645093952028924</t>
+  </si>
+  <si>
+    <t>0.7644657320296671</t>
+  </si>
+  <si>
+    <t>0.972255293245062</t>
+  </si>
+  <si>
+    <t>0.9057818792010163</t>
+  </si>
+  <si>
+    <t>-0.026915194493449018</t>
+  </si>
+  <si>
+    <t>0.172913808283394</t>
+  </si>
+  <si>
+    <t>0.4706262961110176</t>
+  </si>
+  <si>
+    <t>2.494637949717704</t>
+  </si>
+  <si>
+    <t>0.25846652502212025</t>
+  </si>
+  <si>
+    <t>1.9850581604248392</t>
+  </si>
+  <si>
+    <t>0.14760852461679844</t>
+  </si>
+  <si>
+    <t>0.28902503287767994</t>
+  </si>
+  <si>
+    <t>4.989275899435408</t>
+  </si>
+  <si>
+    <t>1.5103881627226485</t>
+  </si>
+  <si>
+    <t>0.2509750721092251</t>
+  </si>
+  <si>
+    <t>155486.60996348757</t>
+  </si>
+  <si>
+    <t>0.49889144267503244</t>
+  </si>
+  <si>
+    <t>0.2522329655744762</t>
+  </si>
+  <si>
+    <t>6.487990821792195</t>
+  </si>
+  <si>
+    <t>7.610469252602249</t>
+  </si>
+  <si>
+    <t>49.07257785649134</t>
+  </si>
+  <si>
+    <t>1.3858122986235368</t>
+  </si>
+  <si>
+    <t>0.18148263215815813</t>
+  </si>
+  <si>
+    <t>3.058723589915843</t>
+  </si>
+  <si>
+    <t>105421.62396940179</t>
+  </si>
+  <si>
+    <t>0.32710990659399813</t>
+  </si>
+  <si>
+    <t>0.49147254265366364</t>
+  </si>
+  <si>
+    <t>2.6711236136732306</t>
+  </si>
+  <si>
+    <t>0.5633417380260347</t>
+  </si>
+  <si>
+    <t>3.6655883927151014</t>
+  </si>
+  <si>
+    <t>0.10217779567241006</t>
+  </si>
+  <si>
+    <t>121.1003861003861</t>
+  </si>
+  <si>
+    <t>0.46756905830264905</t>
+  </si>
+  <si>
+    <t>1.8218571577644935</t>
+  </si>
+  <si>
+    <t>5.915057915057915</t>
+  </si>
+  <si>
+    <t>775405037.5868726</t>
+  </si>
+  <si>
+    <t>4995307160.208494</t>
+  </si>
+  <si>
+    <t>141248844.32260832</t>
+  </si>
+  <si>
+    <t>0.6497479622479623</t>
+  </si>
+  <si>
+    <t>140.13513513513513</t>
+  </si>
+  <si>
+    <t>0.5410622978190546</t>
+  </si>
+  <si>
+    <t>0.7619503103687546</t>
+  </si>
+  <si>
+    <t>4.826622125040997</t>
+  </si>
+  <si>
+    <t>0.47189909844247957</t>
+  </si>
+  <si>
+    <t>2.5819136750760903</t>
+  </si>
+  <si>
+    <t>0.0004084522812611871</t>
+  </si>
+  <si>
+    <t>769411029.1761305</t>
+  </si>
+  <si>
+    <t>-10.630978776512505</t>
+  </si>
+  <si>
+    <t>10.578249340845547</t>
+  </si>
+  <si>
+    <t>44389160.42773468</t>
+  </si>
+  <si>
+    <t>1.0384035911136702</t>
+  </si>
+  <si>
+    <t>11.07074418860554</t>
+  </si>
+  <si>
+    <t>3.1952028427719137</t>
+  </si>
+  <si>
+    <t>43.40257555204428</t>
+  </si>
+  <si>
+    <t>6.624961432960594</t>
+  </si>
+  <si>
+    <t>-0.02628007094336357</t>
+  </si>
+  <si>
+    <t>-0.017325918756206114</t>
+  </si>
+  <si>
+    <t>-42.407417608242056</t>
+  </si>
+  <si>
+    <t>85.80999316028634</t>
+  </si>
+  <si>
+    <t>4.5927174042512275</t>
+  </si>
+  <si>
+    <t>8.366797277300797</t>
+  </si>
+  <si>
+    <t>-0.0025848358294432937</t>
+  </si>
+  <si>
+    <t>0.49591985680497425</t>
+  </si>
+  <si>
+    <t>70.00260603731923</t>
+  </si>
+  <si>
+    <t>6.2525934835063435</t>
+  </si>
+  <si>
+    <t>0.5814739620650771</t>
+  </si>
+  <si>
+    <t>0.00025196966105141413</t>
+  </si>
+  <si>
+    <t>0.5281907767843645</t>
+  </si>
+  <si>
+    <t>0.5041462910804211</t>
+  </si>
+  <si>
+    <t>0.023287408555033848</t>
+  </si>
+  <si>
+    <t>0.49582195913765353</t>
+  </si>
+  <si>
+    <t>1.012233812888287</t>
+  </si>
+  <si>
+    <t>0.25090395695886947</t>
+  </si>
+  <si>
+    <t>0.7534641253497628</t>
+  </si>
+  <si>
+    <t>0.7529214536254499</t>
+  </si>
+  <si>
+    <t>0.9704943573089937</t>
+  </si>
+  <si>
+    <t>0.9011116820480619</t>
+  </si>
+  <si>
+    <t>-0.02281347749051697</t>
+  </si>
+  <si>
+    <t>0.11374928195838074</t>
+  </si>
+  <si>
+    <t>0.48865418177392794</t>
+  </si>
+  <si>
+    <t>2.4993163434919214</t>
+  </si>
+  <si>
+    <t>0.25327962777252494</t>
+  </si>
+  <si>
+    <t>2.052233246637429</t>
+  </si>
+  <si>
+    <t>0.09762316752565842</t>
+  </si>
+  <si>
+    <t>0.2710430912929739</t>
+  </si>
+  <si>
+    <t>4.998632686983841</t>
+  </si>
+  <si>
+    <t>1.5270097301270804</t>
+  </si>
+  <si>
+    <t>0.2580842669661964</t>
+  </si>
+  <si>
+    <t>159656.69085177575</t>
+  </si>
+  <si>
+    <t>0.49208121298026963</t>
+  </si>
+  <si>
+    <t>0.26597077573459177</t>
+  </si>
+  <si>
+    <t>6.51215371735436</t>
+  </si>
+  <si>
+    <t>6.668380060823783</t>
+  </si>
+  <si>
+    <t>43.320752829832976</t>
+  </si>
+  <si>
+    <t>1.2084903558654678</t>
+  </si>
+  <si>
+    <t>0.18347694268129283</t>
+  </si>
+  <si>
+    <t>2.9969098706069457</t>
+  </si>
+  <si>
+    <t>117127.42683027117</t>
+  </si>
+  <si>
+    <t>0.35071106541870345</t>
+  </si>
+  <si>
+    <t>0.5114745733905773</t>
+  </si>
+  <si>
+    <t>2.1404045853678384</t>
+  </si>
+  <si>
+    <t>0.5694734758780957</t>
+  </si>
+  <si>
+    <t>3.7160661694768247</t>
+  </si>
+  <si>
+    <t>0.10556628301309767</t>
+  </si>
+  <si>
+    <t>874.129650507328</t>
+  </si>
+  <si>
+    <t>0.4927450115599369</t>
+  </si>
+  <si>
+    <t>2.235262510342934</t>
+  </si>
+  <si>
+    <t>8.530439684329199</t>
+  </si>
+  <si>
+    <t>112396368.80665164</t>
+  </si>
+  <si>
+    <t>729514721.1899662</t>
+  </si>
+  <si>
+    <t>20323281.009700302</t>
+  </si>
+  <si>
+    <t>0.5258126644118752</t>
+  </si>
+  <si>
+    <t>894.499436302142</t>
+  </si>
+  <si>
+    <t>0.504227416179336</t>
+  </si>
+  <si>
+    <t>0.7300617888445314</t>
+  </si>
+  <si>
+    <t>6.2474106343078715</t>
+  </si>
+  <si>
+    <t>0.38222892656426</t>
+  </si>
+  <si>
+    <t>2.3718181015605606</t>
+  </si>
+  <si>
+    <t>0.0027976615712638838</t>
+  </si>
+  <si>
+    <t>112268604.46978751</t>
+  </si>
+  <si>
+    <t>-4.239571556346607</t>
+  </si>
+  <si>
+    <t>4.247038027046694</t>
+  </si>
+  <si>
+    <t>7100357.203068243</t>
+  </si>
+  <si>
+    <t>0.9999998417511424</t>
+  </si>
+  <si>
+    <t>4.428815211987702</t>
+  </si>
+  <si>
+    <t>3.1935872041468727</t>
+  </si>
+  <si>
+    <t>17.899031030391804</t>
+  </si>
+  <si>
+    <t>2.6494519455527548</t>
+  </si>
+  <si>
+    <t>0.0005843546841485427</t>
+  </si>
+  <si>
+    <t>-0.002160410320928544</t>
+  </si>
+  <si>
+    <t>-17.086001110892887</t>
+  </si>
+  <si>
+    <t>34.98503214128469</t>
+  </si>
+  <si>
+    <t>1.8369640667316982</t>
+  </si>
+  <si>
+    <t>3.3462692286237914</t>
+  </si>
+  <si>
+    <t>0.002461160194135485</t>
+  </si>
+  <si>
+    <t>0.5000001096897451</t>
+  </si>
+  <si>
+    <t>11.197517408964066</t>
+  </si>
+  <si>
+    <t>2.2464727919821352</t>
+  </si>
+  <si>
+    <t>0.49443870715804117</t>
+  </si>
+  <si>
+    <t>0.00024324057551431495</t>
+  </si>
+  <si>
+    <t>0.4944387148918304</t>
+  </si>
+  <si>
+    <t>0.5055609333818329</t>
+  </si>
+  <si>
+    <t>-0.011122221067931724</t>
+  </si>
+  <si>
+    <t>0.9945000555538156</t>
+  </si>
+  <si>
+    <t>0.2481006236866842</t>
+  </si>
+  <si>
+    <t>0.7472195333090835</t>
+  </si>
+  <si>
+    <t>0.8988878133236334</t>
+  </si>
+  <si>
+    <t>0.8314796888727223</t>
+  </si>
+  <si>
+    <t>-0.005499952863089552</t>
+  </si>
+  <si>
+    <t>0.08460494966885602</t>
+  </si>
+  <si>
+    <t>1.499751086224351</t>
+  </si>
+  <si>
+    <t>0.25189955217648424</t>
+  </si>
+  <si>
+    <t>1.9944995409038127</t>
+  </si>
+  <si>
+    <t>0.07072562914872645</t>
+  </si>
+  <si>
+    <t>0.26780865361918704</t>
+  </si>
+  <si>
+    <t>2.999502172448702</t>
+  </si>
+  <si>
+    <t>1.48893860752198</t>
+  </si>
+  <si>
+    <t>0.2499999120684158</t>
+  </si>
+  <si>
+    <t>166454.5188552955</t>
+  </si>
+  <si>
+    <t>0.5000001715074961</t>
+  </si>
+  <si>
+    <t>0.24999991424625195</t>
+  </si>
+  <si>
+    <t>2.5000354889146146</t>
+  </si>
+  <si>
+    <t>5.492601316967868</t>
+  </si>
+  <si>
+    <t>13.71684356849421</t>
+  </si>
+  <si>
+    <t>3.4365407540862813</t>
+  </si>
+  <si>
+    <t>0.6249911277713464</t>
+  </si>
+  <si>
+    <t>2.8801103718520205</t>
+  </si>
+  <si>
+    <t>119149.7070081807</t>
+  </si>
+  <si>
+    <t>0.3569820722890613</t>
+  </si>
+  <si>
+    <t>0.5250093014786651</t>
+  </si>
+  <si>
+    <t>1.7989646948062785</t>
+  </si>
+  <si>
+    <t>0.6004418464003302</t>
+  </si>
+  <si>
+    <t>1.5014959376934707</t>
+  </si>
+  <si>
+    <t>0.37517832357704517</t>
   </si>
   <si>
     <t>1.0</t>
@@ -3901,253 +3901,253 @@
     <t>2.5</t>
   </si>
   <si>
-    <t>56586181574.5</t>
-  </si>
-  <si>
-    <t>141485792548.0</t>
-  </si>
-  <si>
-    <t>35361278831.125</t>
+    <t>100521041602.5</t>
+  </si>
+  <si>
+    <t>251161358008.5</t>
+  </si>
+  <si>
+    <t>62860962501.0</t>
   </si>
   <si>
     <t>0.625</t>
   </si>
   <si>
-    <t>1.7672160050246035e-11</t>
-  </si>
-  <si>
-    <t>4.417404827093883e-11</t>
-  </si>
-  <si>
-    <t>1.1046687995072838e-11</t>
+    <t>9.948174646585382e-12</t>
+  </si>
+  <si>
+    <t>2.4884415180864975e-11</t>
+  </si>
+  <si>
+    <t>6.214114513015484e-12</t>
   </si>
   <si>
     <t>0.9999999999999993</t>
   </si>
   <si>
-    <t>4.203826743484594e-06</t>
-  </si>
-  <si>
-    <t>812.25</t>
-  </si>
-  <si>
-    <t>-1619.1081995851182</t>
-  </si>
-  <si>
-    <t>-840.2701656663288</t>
-  </si>
-  <si>
-    <t>835302739929.7059</t>
-  </si>
-  <si>
-    <t>5.436237236322261</t>
-  </si>
-  <si>
-    <t>408.83566873836025</t>
-  </si>
-  <si>
-    <t>2.5869220797881836</t>
-  </si>
-  <si>
-    <t>-492.5127863697029</t>
-  </si>
-  <si>
-    <t>238.01134329644657</t>
-  </si>
-  <si>
-    <t>-1292.9070271546439</t>
-  </si>
-  <si>
-    <t>-1355.9105958962273</t>
-  </si>
-  <si>
-    <t>-2240.8888357866263</t>
-  </si>
-  <si>
-    <t>1748.3760494169233</t>
-  </si>
-  <si>
-    <t>171.90455359464494</t>
-  </si>
-  <si>
-    <t>1325.0411308752748</t>
-  </si>
-  <si>
-    <t>0.6205658525820439</t>
-  </si>
-  <si>
-    <t>0.02649619283459808</t>
-  </si>
-  <si>
-    <t>84125.41764536759</t>
-  </si>
-  <si>
-    <t>1537.8113466909558</t>
-  </si>
-  <si>
-    <t>526734.1548127129</t>
-  </si>
-  <si>
-    <t>5602.307694958565</t>
-  </si>
-  <si>
-    <t>446.5778100635107</t>
-  </si>
-  <si>
-    <t>30.94704861021112</t>
-  </si>
-  <si>
-    <t>0.8697052038964688</t>
-  </si>
-  <si>
-    <t>3.8442879255971296</t>
-  </si>
-  <si>
-    <t>3.4685676346530077</t>
-  </si>
-  <si>
-    <t>15.679858499598861</t>
-  </si>
-  <si>
-    <t>0.3555709851713331</t>
-  </si>
-  <si>
-    <t>0.271957620591282</t>
-  </si>
-  <si>
-    <t>0.9940865070666691</t>
-  </si>
-  <si>
-    <t>0.9511185151786804</t>
-  </si>
-  <si>
-    <t>-0.22292644962837935</t>
-  </si>
-  <si>
-    <t>0.9465803831029037</t>
-  </si>
-  <si>
-    <t>0.2748527657755641</t>
-  </si>
-  <si>
-    <t>37.86661306265658</t>
-  </si>
-  <si>
-    <t>0.0022589693612906714</t>
-  </si>
-  <si>
-    <t>9.54567356972713</t>
-  </si>
-  <si>
-    <t>0.8898482146090679</t>
-  </si>
-  <si>
-    <t>0.006415531867068358</t>
-  </si>
-  <si>
-    <t>75.73322612531315</t>
-  </si>
-  <si>
-    <t>6.331653552498666</t>
-  </si>
-  <si>
-    <t>119.38121466843046</t>
-  </si>
-  <si>
-    <t>10972.692155342735</t>
-  </si>
-  <si>
-    <t>0.025785576765906634</t>
-  </si>
-  <si>
-    <t>137.47512189218145</t>
-  </si>
-  <si>
-    <t>1681.9420306909649</t>
-  </si>
-  <si>
-    <t>1.4069006379873839</t>
-  </si>
-  <si>
-    <t>2197.3523547351033</t>
-  </si>
-  <si>
-    <t>0.001267218833353338</t>
-  </si>
-  <si>
-    <t>0.0008480672336439796</t>
-  </si>
-  <si>
-    <t>5.982790014263695</t>
-  </si>
-  <si>
-    <t>349017.4048282809</t>
-  </si>
-  <si>
-    <t>0.8196000680932246</t>
-  </si>
-  <si>
-    <t>0.894350881453541</t>
-  </si>
-  <si>
-    <t>0.15450232301491734</t>
-  </si>
-  <si>
-    <t>0.9235192570498183</t>
-  </si>
-  <si>
-    <t>1583.5351217757338</t>
-  </si>
-  <si>
-    <t>0.0007698324035632933</t>
-  </si>
-  <si>
-    <t>2845.504142204827</t>
-  </si>
-  <si>
-    <t>0.023202088569837142</t>
-  </si>
-  <si>
-    <t>138.02094499393164</t>
-  </si>
-  <si>
-    <t>2284.006172537508</t>
-  </si>
-  <si>
-    <t>2887.0637883235486</t>
-  </si>
-  <si>
-    <t>2475895.1160551207</t>
-  </si>
-  <si>
-    <t>3.5267327083613056</t>
-  </si>
-  <si>
-    <t>0.0006155112539546652</t>
-  </si>
-  <si>
-    <t>48938.258317025444</t>
-  </si>
-  <si>
-    <t>0.399039940615015</t>
-  </si>
-  <si>
-    <t>0.6563362426291645</t>
-  </si>
-  <si>
-    <t>1569.6774775258182</t>
-  </si>
-  <si>
-    <t>0.0003822600410359764</t>
-  </si>
-  <si>
-    <t>7.626655404661116</t>
-  </si>
-  <si>
-    <t>0.25777865591047533</t>
-  </si>
-  <si>
-    <t>2872.01484210219</t>
+    <t>3.1540716699705567e-06</t>
+  </si>
+  <si>
+    <t>22052.25</t>
+  </si>
+  <si>
+    <t>-1683.183368022202</t>
+  </si>
+  <si>
+    <t>-852.228051514049</t>
+  </si>
+  <si>
+    <t>1239002845930.162</t>
+  </si>
+  <si>
+    <t>5.425486927102052</t>
+  </si>
+  <si>
+    <t>422.25723158316737</t>
+  </si>
+  <si>
+    <t>2.7687836908700096</t>
+  </si>
+  <si>
+    <t>-505.09801386947845</t>
+  </si>
+  <si>
+    <t>254.4367274347488</t>
+  </si>
+  <si>
+    <t>-1362.8168262259383</t>
+  </si>
+  <si>
+    <t>-1455.9037888195842</t>
+  </si>
+  <si>
+    <t>-2496.931064709147</t>
+  </si>
+  <si>
+    <t>1991.8330508396684</t>
+  </si>
+  <si>
+    <t>181.86976218574574</t>
+  </si>
+  <si>
+    <t>1397.8382909623735</t>
+  </si>
+  <si>
+    <t>0.8013774794576782</t>
+  </si>
+  <si>
+    <t>0.028253632533345473</t>
+  </si>
+  <si>
+    <t>96682.1858360699</t>
+  </si>
+  <si>
+    <t>2157.179088265563</t>
+  </si>
+  <si>
+    <t>785879.4117938057</t>
+  </si>
+  <si>
+    <t>9662.242130564675</t>
+  </si>
+  <si>
+    <t>520.3215572454344</t>
+  </si>
+  <si>
+    <t>30.78048669116347</t>
+  </si>
+  <si>
+    <t>0.8875900934132984</t>
+  </si>
+  <si>
+    <t>3.7324092265601028</t>
+  </si>
+  <si>
+    <t>3.4286442600187264</t>
+  </si>
+  <si>
+    <t>16.334647338013585</t>
+  </si>
+  <si>
+    <t>0.3674725789247338</t>
+  </si>
+  <si>
+    <t>0.286183259388522</t>
+  </si>
+  <si>
+    <t>0.9953484052740866</t>
+  </si>
+  <si>
+    <t>0.9575049234707329</t>
+  </si>
+  <si>
+    <t>-0.2355454692105641</t>
+  </si>
+  <si>
+    <t>0.9529112091032318</t>
+  </si>
+  <si>
+    <t>0.2873995257930549</t>
+  </si>
+  <si>
+    <t>45.10840675170629</t>
+  </si>
+  <si>
+    <t>0.002723900932382153</t>
+  </si>
+  <si>
+    <t>9.466287500017355</t>
+  </si>
+  <si>
+    <t>0.8987165217352895</t>
+  </si>
+  <si>
+    <t>0.008732724718673281</t>
+  </si>
+  <si>
+    <t>90.21681350341262</t>
+  </si>
+  <si>
+    <t>6.331600175993382</t>
+  </si>
+  <si>
+    <t>137.77551098414943</t>
+  </si>
+  <si>
+    <t>15203.334288711789</t>
+  </si>
+  <si>
+    <t>0.02706316171258089</t>
+  </si>
+  <si>
+    <t>158.4142436357866</t>
+  </si>
+  <si>
+    <t>2329.3669435884262</t>
+  </si>
+  <si>
+    <t>1.4495960189483488</t>
+  </si>
+  <si>
+    <t>3136.41208187981</t>
+  </si>
+  <si>
+    <t>0.0008836187714630876</t>
+  </si>
+  <si>
+    <t>0.0005780626999763104</t>
+  </si>
+  <si>
+    <t>6.015484540372294</t>
+  </si>
+  <si>
+    <t>453910.6504006697</t>
+  </si>
+  <si>
+    <t>0.8074212388538814</t>
+  </si>
+  <si>
+    <t>0.8857799042690723</t>
+  </si>
+  <si>
+    <t>0.17261332135270083</t>
+  </si>
+  <si>
+    <t>0.9176600666820783</t>
+  </si>
+  <si>
+    <t>2179.227874172549</t>
+  </si>
+  <si>
+    <t>0.0005224430602443629</t>
+  </si>
+  <si>
+    <t>3312.9528213020576</t>
+  </si>
+  <si>
+    <t>0.021977052932098083</t>
+  </si>
+  <si>
+    <t>158.7136470541457</t>
+  </si>
+  <si>
+    <t>3095.3784976052434</t>
+  </si>
+  <si>
+    <t>9981.645410160138</t>
+  </si>
+  <si>
+    <t>12905141.072147852</t>
+  </si>
+  <si>
+    <t>7.879103844810533</t>
+  </si>
+  <si>
+    <t>0.00044843241988227133</t>
+  </si>
+  <si>
+    <t>59986.35338914466</t>
+  </si>
+  <si>
+    <t>0.3979299841398422</t>
+  </si>
+  <si>
+    <t>0.6555594475585891</t>
+  </si>
+  <si>
+    <t>2103.4100233204904</t>
+  </si>
+  <si>
+    <t>0.000279523474354909</t>
+  </si>
+  <si>
+    <t>7.734235184389572</t>
+  </si>
+  <si>
+    <t>0.23773184398069078</t>
+  </si>
+  <si>
+    <t>9963.951440347708</t>
   </si>
 </sst>
 </file>
@@ -4612,7 +4612,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-441.2011302479646</v>
+        <v>-228.7198702921083</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4620,7 +4620,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-32766.00000000001</v>
+        <v>-3258</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4628,7 +4628,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>32763.00000000005</v>
+        <v>17935.99999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4668,7 +4668,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>475757</v>
+        <v>634101</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4700,7 +4700,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.7218477668554207</v>
+        <v>0.7718453225485958</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4708,7 +4708,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.4131096291617009</v>
+        <v>0.4521425931392275</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4716,7 +4716,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>69.67057432385974</v>
+        <v>74.90454581447806</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4724,7 +4724,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>168.6491173426244</v>
+        <v>165.6657588802142</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4772,7 +4772,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>121.7389887359112</v>
+        <v>127.8683410981568</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4804,7 +4804,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>475757</v>
+        <v>634101</v>
       </c>
     </row>
     <row r="38" spans="1:2">

</xml_diff>

<commit_message>
Added Batch Name Entry Feature
</commit_message>
<xml_diff>
--- a/Radiomics_Code/Output.xlsx
+++ b/Radiomics_Code/Output.xlsx
@@ -2134,7 +2134,7 @@
     <t>1.19.2</t>
   </si>
   <si>
-    <t>2.0.2</t>
+    <t>1.2.4</t>
   </si>
   <si>
     <t>1.1.1</t>
@@ -2149,7 +2149,7 @@
     <t>{'Original': {}, 'Wavelet': {}}</t>
   </si>
   <si>
-    <t>1c8283e59692ba313e732483f84c87ea428df23a</t>
+    <t>a90ca85757e33e2e9c2d48451af5be8ccf58b7dd</t>
   </si>
   <si>
     <t>3D</t>
@@ -2158,1735 +2158,1735 @@
     <t>(1.0, 1.0, 1.0)</t>
   </si>
   <si>
-    <t>(246, 258, 213)</t>
-  </si>
-  <si>
-    <t>78cd76bca29745a9da351ea971d4702af8137da5</t>
-  </si>
-  <si>
-    <t>(42, 56, 51, 156, 156, 113)</t>
-  </si>
-  <si>
-    <t>(111.63374604361135, 134.81030939866048, 119.09376266556905)</t>
-  </si>
-  <si>
-    <t>157.2768260107</t>
-  </si>
-  <si>
-    <t>175.31685600648902</t>
-  </si>
-  <si>
-    <t>162.63148526653748</t>
-  </si>
-  <si>
-    <t>175.95738120351757</t>
-  </si>
-  <si>
-    <t>633942.875</t>
-  </si>
-  <si>
-    <t>0.47120025903245777</t>
-  </si>
-  <si>
-    <t>75737.68401621885</t>
-  </si>
-  <si>
-    <t>0.11947083404986426</t>
-  </si>
-  <si>
-    <t>-597.0000000000001</t>
-  </si>
-  <si>
-    <t>-301.00000000000045</t>
-  </si>
-  <si>
-    <t>155092235155.00003</t>
-  </si>
-  <si>
-    <t>3.948354718350135</t>
-  </si>
-  <si>
-    <t>149.99999999999994</t>
-  </si>
-  <si>
-    <t>2.76407940177534</t>
-  </si>
-  <si>
-    <t>-186.99999999999972</t>
-  </si>
-  <si>
-    <t>90.2349721624063</t>
-  </si>
-  <si>
-    <t>-482.066353782757</t>
-  </si>
-  <si>
-    <t>-514.0000000000002</t>
-  </si>
-  <si>
-    <t>-893.0000000000001</t>
-  </si>
-  <si>
-    <t>706.0000000000005</t>
-  </si>
-  <si>
-    <t>64.37506827114444</t>
-  </si>
-  <si>
-    <t>494.5563795639468</t>
-  </si>
-  <si>
-    <t>0.7839677757162534</t>
-  </si>
-  <si>
-    <t>0.07783573582178754</t>
-  </si>
-  <si>
-    <t>12198.04311799634</t>
-  </si>
-  <si>
-    <t>300.7281269559176</t>
-  </si>
-  <si>
-    <t>12454.359374943084</t>
-  </si>
-  <si>
-    <t>424.77649417615856</t>
-  </si>
-  <si>
-    <t>65.55601328132404</t>
-  </si>
-  <si>
-    <t>4.407194210570112</t>
-  </si>
-  <si>
-    <t>0.8733146313840882</t>
-  </si>
-  <si>
-    <t>1.441350843235845</t>
-  </si>
-  <si>
-    <t>2.2471249675846448</t>
-  </si>
-  <si>
-    <t>2.266870511229475</t>
-  </si>
-  <si>
-    <t>0.5539290307599682</t>
-  </si>
-  <si>
-    <t>0.5069120415268629</t>
-  </si>
-  <si>
-    <t>0.9949208965286106</t>
-  </si>
-  <si>
-    <t>0.9548509783875705</t>
-  </si>
-  <si>
-    <t>-0.27882629014514376</t>
-  </si>
-  <si>
-    <t>0.9347611074479393</t>
-  </si>
-  <si>
-    <t>0.4454091209660392</t>
-  </si>
-  <si>
-    <t>16.894904196462925</t>
-  </si>
-  <si>
-    <t>0.01680818698560138</t>
-  </si>
-  <si>
-    <t>6.699472098797829</t>
-  </si>
-  <si>
-    <t>0.8806131359273489</t>
-  </si>
-  <si>
-    <t>0.04898633647445115</t>
-  </si>
-  <si>
-    <t>33.78980839292586</t>
-  </si>
-  <si>
-    <t>4.847002946568311</t>
-  </si>
-  <si>
-    <t>17.490801872973535</t>
-  </si>
-  <si>
-    <t>33589.65811618929</t>
-  </si>
-  <si>
-    <t>0.07110348097851486</t>
-  </si>
-  <si>
-    <t>20.59025619425747</t>
-  </si>
-  <si>
-    <t>332.1331281167526</t>
-  </si>
-  <si>
-    <t>2.4035403114967555</t>
-  </si>
-  <si>
-    <t>700.9831122360966</t>
-  </si>
-  <si>
-    <t>0.010338729539239413</t>
-  </si>
-  <si>
-    <t>0.003906780614892993</t>
-  </si>
-  <si>
-    <t>5.079509038573013</t>
-  </si>
-  <si>
-    <t>293450.24689926446</t>
-  </si>
-  <si>
-    <t>0.6189678938851076</t>
-  </si>
-  <si>
-    <t>0.7446799605935138</t>
-  </si>
-  <si>
-    <t>0.5830450733009109</t>
-  </si>
-  <si>
-    <t>0.8142420407631377</t>
-  </si>
-  <si>
-    <t>281.33090151404184</t>
-  </si>
-  <si>
-    <t>0.003073839964502215</t>
-  </si>
-  <si>
-    <t>2218.844123008173</t>
-  </si>
-  <si>
-    <t>0.06523326051061837</t>
-  </si>
-  <si>
-    <t>21.635914464351817</t>
-  </si>
-  <si>
-    <t>477.9721291233022</t>
-  </si>
-  <si>
-    <t>505954.72808255424</t>
-  </si>
-  <si>
-    <t>122817954.12668313</t>
-  </si>
-  <si>
-    <t>2265.2755735184714</t>
-  </si>
-  <si>
-    <t>0.002842147499864418</t>
-  </si>
-  <si>
-    <t>9474.891103663198</t>
-  </si>
-  <si>
-    <t>0.27855856716831884</t>
-  </si>
-  <si>
-    <t>0.5401381787223664</t>
-  </si>
-  <si>
-    <t>263.89267911744713</t>
-  </si>
-  <si>
-    <t>0.0014683433221502</t>
-  </si>
-  <si>
-    <t>6.749649144126846</t>
-  </si>
-  <si>
-    <t>0.05364129689118926</t>
-  </si>
-  <si>
-    <t>505607.19075163326</t>
-  </si>
-  <si>
-    <t>-23.802043945541644</t>
-  </si>
-  <si>
-    <t>37.73937003600093</t>
-  </si>
-  <si>
-    <t>507021955.80751806</t>
-  </si>
-  <si>
-    <t>2.1593196072366054</t>
-  </si>
-  <si>
-    <t>30.173766742496568</t>
-  </si>
-  <si>
-    <t>6.2704808238147525</t>
-  </si>
-  <si>
-    <t>235.67542878079954</t>
-  </si>
-  <si>
-    <t>20.104050531492526</t>
-  </si>
-  <si>
-    <t>6.345136629707502</t>
-  </si>
-  <si>
-    <t>4.506504707707242</t>
-  </si>
-  <si>
-    <t>-180.98238681364526</t>
-  </si>
-  <si>
-    <t>416.6578155944448</t>
-  </si>
-  <si>
-    <t>12.699921698977501</t>
-  </si>
-  <si>
-    <t>28.277054185908018</t>
-  </si>
-  <si>
-    <t>0.7664260312622594</t>
-  </si>
-  <si>
-    <t>0.28331334449919204</t>
-  </si>
-  <si>
-    <t>759.3310345831223</t>
-  </si>
-  <si>
-    <t>77.37575157531136</t>
-  </si>
-  <si>
-    <t>106.26499376052955</t>
-  </si>
-  <si>
-    <t>7.122988317749104</t>
-  </si>
-  <si>
-    <t>3.9713949614723636</t>
-  </si>
-  <si>
-    <t>1.0663105235092185</t>
-  </si>
-  <si>
-    <t>0.5751030467807323</t>
-  </si>
-  <si>
-    <t>0.7186566030257784</t>
-  </si>
-  <si>
-    <t>1.4566926440655785</t>
-  </si>
-  <si>
-    <t>0.522133803025704</t>
-  </si>
-  <si>
-    <t>0.6908579433621042</t>
-  </si>
-  <si>
-    <t>0.6745966507018097</t>
-  </si>
-  <si>
-    <t>0.9967522105506238</t>
-  </si>
-  <si>
-    <t>0.9630642862361807</t>
-  </si>
-  <si>
-    <t>-0.15482357671027475</t>
-  </si>
-  <si>
-    <t>0.6457656976247741</t>
-  </si>
-  <si>
-    <t>0.481850420513319</t>
-  </si>
-  <si>
-    <t>8.754968623567224</t>
-  </si>
-  <si>
-    <t>0.1034085821821519</t>
-  </si>
-  <si>
-    <t>3.9474453638499702</t>
-  </si>
-  <si>
-    <t>0.6729223318424388</t>
-  </si>
-  <si>
-    <t>0.19256830604034667</t>
-  </si>
-  <si>
-    <t>17.50993724713445</t>
-  </si>
-  <si>
-    <t>2.919839211896208</t>
-  </si>
-  <si>
-    <t>1.2594263712453952</t>
-  </si>
-  <si>
-    <t>93524.63976618249</t>
-  </si>
-  <si>
-    <t>0.24968387476707146</t>
-  </si>
-  <si>
-    <t>1.5888174919777047</t>
-  </si>
-  <si>
-    <t>78.65789456306787</t>
-  </si>
-  <si>
-    <t>4.659916832952112</t>
-  </si>
-  <si>
-    <t>359.0439260867739</t>
-  </si>
-  <si>
-    <t>0.06360334845095553</t>
-  </si>
-  <si>
-    <t>0.01381618815347591</t>
-  </si>
-  <si>
-    <t>3.942256793366304</t>
-  </si>
-  <si>
-    <t>167335.1979325648</t>
-  </si>
-  <si>
-    <t>0.43301213740905015</t>
-  </si>
-  <si>
-    <t>0.5907800662185216</t>
-  </si>
-  <si>
-    <t>1.513060433986883</t>
-  </si>
-  <si>
-    <t>0.6704445475416587</t>
-  </si>
-  <si>
-    <t>53.16012003704361</t>
-  </si>
-  <si>
-    <t>0.009315608850398335</t>
-  </si>
-  <si>
-    <t>1852.2221082621083</t>
-  </si>
-  <si>
-    <t>0.2110794425369924</t>
-  </si>
-  <si>
-    <t>5.015463108253992</t>
-  </si>
-  <si>
-    <t>79.71430199430199</t>
-  </si>
-  <si>
-    <t>12106141.206723647</t>
-  </si>
-  <si>
-    <t>908128670.1747009</t>
-  </si>
-  <si>
-    <t>164110.00271116046</t>
-  </si>
-  <si>
-    <t>0.01649157942664722</t>
-  </si>
-  <si>
-    <t>1474.8582336182337</t>
-  </si>
-  <si>
-    <t>0.1680750123781463</t>
-  </si>
-  <si>
-    <t>0.4055166846177399</t>
-  </si>
-  <si>
-    <t>32.30367144880942</t>
-  </si>
-  <si>
-    <t>0.006781195092154824</t>
-  </si>
-  <si>
-    <t>6.277797286089917</t>
-  </si>
-  <si>
-    <t>0.013838489451995818</t>
-  </si>
-  <si>
-    <t>12100919.377963152</t>
-  </si>
-  <si>
-    <t>-28.745129560316553</t>
-  </si>
-  <si>
-    <t>33.02721570534765</t>
-  </si>
-  <si>
-    <t>383907805.1723418</t>
-  </si>
-  <si>
-    <t>2.077123596139603</t>
-  </si>
-  <si>
-    <t>32.24500278451681</t>
-  </si>
-  <si>
-    <t>3.3312406355114264</t>
-  </si>
-  <si>
-    <t>154.5555001613982</t>
-  </si>
-  <si>
-    <t>19.355082166037622</t>
-  </si>
-  <si>
-    <t>2.0666504461338553</t>
-  </si>
-  <si>
-    <t>1.9450135480506112</t>
-  </si>
-  <si>
-    <t>-136.62629769982587</t>
-  </si>
-  <si>
-    <t>291.181797861224</t>
-  </si>
-  <si>
-    <t>13.381603125962851</t>
-  </si>
-  <si>
-    <t>24.605616555724218</t>
-  </si>
-  <si>
-    <t>0.041110025349176474</t>
-  </si>
-  <si>
-    <t>0.27979032340783744</t>
-  </si>
-  <si>
-    <t>601.1653220208242</t>
-  </si>
-  <si>
-    <t>43.47545574329359</t>
-  </si>
-  <si>
-    <t>20.986054972153674</t>
-  </si>
-  <si>
-    <t>0.1524616199861179</t>
-  </si>
-  <si>
-    <t>2.4190384421108564</t>
-  </si>
-  <si>
-    <t>1.715685683660816</t>
-  </si>
-  <si>
-    <t>0.1698558807053826</t>
-  </si>
-  <si>
-    <t>0.9575234813438821</t>
-  </si>
-  <si>
-    <t>1.701484917604896</t>
-  </si>
-  <si>
-    <t>0.7463145256324624</t>
-  </si>
-  <si>
-    <t>0.6251042544833625</t>
-  </si>
-  <si>
-    <t>0.594709504596057</t>
-  </si>
-  <si>
-    <t>0.9901955401190604</t>
-  </si>
-  <si>
-    <t>0.9350364449830941</t>
-  </si>
-  <si>
-    <t>-0.05496570168882383</t>
-  </si>
-  <si>
-    <t>0.27335770648447555</t>
-  </si>
-  <si>
-    <t>0.49019448922181624</t>
-  </si>
-  <si>
-    <t>6.58024443271626</t>
-  </si>
-  <si>
-    <t>0.08669006395714215</t>
-  </si>
-  <si>
-    <t>4.025334226859448</t>
-  </si>
-  <si>
-    <t>0.24814397477804986</t>
-  </si>
-  <si>
-    <t>0.14852067856225828</t>
-  </si>
-  <si>
-    <t>13.16048886543252</t>
-  </si>
-  <si>
-    <t>2.658126748443304</t>
-  </si>
-  <si>
-    <t>1.0336810314429183</t>
-  </si>
-  <si>
-    <t>108171.48292388588</t>
-  </si>
-  <si>
-    <t>0.25197866958256304</t>
-  </si>
-  <si>
-    <t>1.2392355174474476</t>
-  </si>
-  <si>
-    <t>44.60042752008946</t>
-  </si>
-  <si>
-    <t>3.2048264376315654</t>
-  </si>
-  <si>
-    <t>141.2532551075798</t>
-  </si>
-  <si>
-    <t>0.07864341205531339</t>
-  </si>
-  <si>
-    <t>0.025380697380637543</t>
-  </si>
-  <si>
-    <t>3.482916452039593</t>
-  </si>
-  <si>
-    <t>233366.45002565827</t>
-  </si>
-  <si>
-    <t>0.5308709599328777</t>
-  </si>
-  <si>
-    <t>0.6779298566001315</t>
-  </si>
-  <si>
-    <t>0.8959082379411013</t>
-  </si>
-  <si>
-    <t>0.749210633891904</t>
-  </si>
-  <si>
-    <t>33.557492433784795</t>
-  </si>
-  <si>
-    <t>0.019253378385653927</t>
-  </si>
-  <si>
-    <t>3505.6081871345027</t>
-  </si>
-  <si>
-    <t>0.21354825701355404</t>
-  </si>
-  <si>
-    <t>4.948249831708663</t>
-  </si>
-  <si>
-    <t>48.130665204678365</t>
-  </si>
-  <si>
-    <t>6368287.65625</t>
-  </si>
-  <si>
-    <t>279808899.89175195</t>
-  </si>
-  <si>
-    <t>149662.95759199795</t>
-  </si>
-  <si>
-    <t>0.03385349571209013</t>
-  </si>
-  <si>
-    <t>3292.71418128655</t>
-  </si>
-  <si>
-    <t>0.2005795675734984</t>
-  </si>
-  <si>
-    <t>0.43841722735350214</t>
-  </si>
-  <si>
-    <t>21.36812517744667</t>
-  </si>
-  <si>
-    <t>0.015397461797092662</t>
-  </si>
-  <si>
-    <t>5.510851895615469</t>
-  </si>
-  <si>
-    <t>0.02588862026711833</t>
-  </si>
-  <si>
-    <t>6366795.610330389</t>
-  </si>
-  <si>
-    <t>-11.087691509011936</t>
-  </si>
-  <si>
-    <t>10.980828375674433</t>
-  </si>
-  <si>
-    <t>48403436.118667535</t>
-  </si>
-  <si>
-    <t>1.0542230352763142</t>
-  </si>
-  <si>
-    <t>11.499111255558331</t>
-  </si>
-  <si>
-    <t>3.262530269635994</t>
-  </si>
-  <si>
-    <t>48.55049498786686</t>
-  </si>
-  <si>
-    <t>6.900096939079274</t>
-  </si>
-  <si>
-    <t>-0.046360363733741916</t>
-  </si>
-  <si>
-    <t>-0.024795945960860016</t>
-  </si>
-  <si>
-    <t>-55.11847347241785</t>
-  </si>
-  <si>
-    <t>103.6689684602847</t>
-  </si>
-  <si>
-    <t>4.768791403070438</t>
-  </si>
-  <si>
-    <t>8.736930427533428</t>
-  </si>
-  <si>
-    <t>-0.013071028999716678</t>
-  </si>
-  <si>
-    <t>0.4938679580038794</t>
-  </si>
-  <si>
-    <t>76.33180401223389</t>
-  </si>
-  <si>
-    <t>12.246001479489992</t>
-  </si>
-  <si>
-    <t>0.6189694012194006</t>
-  </si>
-  <si>
-    <t>-0.0007116387037494264</t>
-  </si>
-  <si>
-    <t>0.5367209936571614</t>
-  </si>
-  <si>
-    <t>0.5118317254986441</t>
-  </si>
-  <si>
-    <t>0.02374287481983993</t>
-  </si>
-  <si>
-    <t>0.4994093778073816</t>
-  </si>
-  <si>
-    <t>1.0251499977775398</t>
-  </si>
-  <si>
-    <t>0.25480446497314574</t>
-  </si>
-  <si>
-    <t>0.752340317521779</t>
-  </si>
-  <si>
-    <t>0.7515374038475191</t>
-  </si>
-  <si>
-    <t>0.980416460051866</t>
-  </si>
-  <si>
-    <t>0.917059054290817</t>
-  </si>
-  <si>
-    <t>-0.023427723196821824</t>
-  </si>
-  <si>
-    <t>0.11718680274566529</t>
-  </si>
-  <si>
-    <t>0.48877857046919176</t>
-  </si>
-  <si>
-    <t>3.498539551814555</t>
-  </si>
-  <si>
-    <t>0.2513952978010319</t>
-  </si>
-  <si>
-    <t>2.0821215542943183</t>
-  </si>
-  <si>
-    <t>0.10068284992747746</t>
-  </si>
-  <si>
-    <t>0.2703705980946153</t>
-  </si>
-  <si>
-    <t>6.99707910362911</t>
-  </si>
-  <si>
-    <t>1.5425009517393475</t>
-  </si>
-  <si>
-    <t>0.26213817978895143</t>
-  </si>
-  <si>
-    <t>158903.61911581864</t>
-  </si>
-  <si>
-    <t>0.4882324278500002</t>
-  </si>
-  <si>
-    <t>0.27386340874599024</t>
-  </si>
-  <si>
-    <t>12.51768885914716</t>
-  </si>
-  <si>
-    <t>6.567383364299527</t>
-  </si>
-  <si>
-    <t>82.02250811416886</t>
-  </si>
-  <si>
-    <t>0.5716227555604081</t>
-  </si>
-  <si>
-    <t>0.08756382998509506</t>
-  </si>
-  <si>
-    <t>3.014426779569026</t>
-  </si>
-  <si>
-    <t>117729.05804153203</t>
-  </si>
-  <si>
-    <t>0.3513378187949874</t>
-  </si>
-  <si>
-    <t>0.5130118193983414</t>
-  </si>
-  <si>
-    <t>2.072701642012365</t>
-  </si>
-  <si>
-    <t>0.5708647451655473</t>
-  </si>
-  <si>
-    <t>7.157808591860812</t>
-  </si>
-  <si>
-    <t>0.05024930025324467</t>
-  </si>
-  <si>
-    <t>1244.4317637669592</t>
-  </si>
-  <si>
-    <t>0.4965809113196166</t>
-  </si>
-  <si>
-    <t>2.2491280304762586</t>
-  </si>
-  <si>
-    <t>14.293296089385475</t>
-  </si>
-  <si>
-    <t>79233832.23503591</t>
-  </si>
-  <si>
-    <t>989196885.4397446</t>
-  </si>
-  <si>
-    <t>6886451.085715727</t>
-  </si>
-  <si>
-    <t>0.14775028819721558</t>
-  </si>
-  <si>
-    <t>1140.491620111732</t>
-  </si>
-  <si>
-    <t>0.455104397490715</t>
-  </si>
-  <si>
-    <t>0.6854237376278367</t>
-  </si>
-  <si>
-    <t>9.861159380060393</t>
-  </si>
-  <si>
-    <t>0.10095381250217488</t>
-  </si>
-  <si>
-    <t>2.4841103260253745</t>
-  </si>
-  <si>
-    <t>0.003952051802473108</t>
-  </si>
-  <si>
-    <t>79169806.4749605</t>
-  </si>
-  <si>
-    <t>-22.67817591859521</t>
-  </si>
-  <si>
-    <t>38.067884379103745</t>
-  </si>
-  <si>
-    <t>493506298.9071958</t>
-  </si>
-  <si>
-    <t>2.1237258978762643</t>
-  </si>
-  <si>
-    <t>29.433196021636462</t>
-  </si>
-  <si>
-    <t>7.181622258796556</t>
-  </si>
-  <si>
-    <t>260.4795103636354</t>
-  </si>
-  <si>
-    <t>19.675878180664967</t>
-  </si>
-  <si>
-    <t>6.724596475141107</t>
-  </si>
-  <si>
-    <t>4.500726354926022</t>
-  </si>
-  <si>
-    <t>-138.44190065775788</t>
-  </si>
-  <si>
-    <t>398.9214110213933</t>
-  </si>
-  <si>
-    <t>12.416671663725875</t>
-  </si>
-  <si>
-    <t>27.89761850351395</t>
-  </si>
-  <si>
-    <t>1.002817681345296</t>
-  </si>
-  <si>
-    <t>0.2894573142804702</t>
-  </si>
-  <si>
-    <t>733.0569204141241</t>
-  </si>
-  <si>
-    <t>46.36749807522014</t>
-  </si>
-  <si>
-    <t>107.61498455241615</t>
-  </si>
-  <si>
-    <t>7.935308109439703</t>
-  </si>
-  <si>
-    <t>3.7833086502892703</t>
-  </si>
-  <si>
-    <t>1.0054144704141572</t>
-  </si>
-  <si>
-    <t>0.5775673747944002</t>
-  </si>
-  <si>
-    <t>0.69480454449174</t>
-  </si>
-  <si>
-    <t>1.4261292721343983</t>
-  </si>
-  <si>
-    <t>0.496880190445423</t>
-  </si>
-  <si>
-    <t>0.6978840935337259</t>
-  </si>
-  <si>
-    <t>0.6829365614990797</t>
-  </si>
-  <si>
-    <t>0.9965694540182116</t>
-  </si>
-  <si>
-    <t>0.9622819207909856</t>
-  </si>
-  <si>
-    <t>-0.15702725692842887</t>
-  </si>
-  <si>
-    <t>0.6442935745455287</t>
-  </si>
-  <si>
-    <t>0.47921059990143944</t>
-  </si>
-  <si>
-    <t>6.758179700552627</t>
-  </si>
-  <si>
-    <t>0.10889029676090067</t>
-  </si>
-  <si>
-    <t>3.8598848361069362</t>
-  </si>
-  <si>
-    <t>0.6610663149909844</t>
-  </si>
-  <si>
-    <t>0.19886089567305218</t>
-  </si>
-  <si>
-    <t>13.516359401105252</t>
-  </si>
-  <si>
-    <t>2.8765166434120704</t>
-  </si>
-  <si>
-    <t>1.1971807801758567</t>
-  </si>
-  <si>
-    <t>93351.98781297336</t>
-  </si>
-  <si>
-    <t>0.25342693002554467</t>
-  </si>
-  <si>
-    <t>1.5680230082475906</t>
-  </si>
-  <si>
-    <t>47.92047891446311</t>
-  </si>
-  <si>
-    <t>4.87135472185848</t>
-  </si>
-  <si>
-    <t>224.76780041239604</t>
-  </si>
-  <si>
-    <t>0.11433734269843149</t>
-  </si>
-  <si>
-    <t>0.023901847418799114</t>
-  </si>
-  <si>
-    <t>3.951311981156456</t>
-  </si>
-  <si>
-    <t>160720.883217656</t>
-  </si>
-  <si>
-    <t>0.42250475626550954</t>
-  </si>
-  <si>
-    <t>0.5808680320642925</t>
-  </si>
-  <si>
-    <t>1.6016825473192262</t>
-  </si>
-  <si>
-    <t>0.6607243127507572</t>
-  </si>
-  <si>
-    <t>32.189109638534816</t>
-  </si>
-  <si>
-    <t>0.015918003301791942</t>
-  </si>
-  <si>
-    <t>1741.7410870835768</t>
-  </si>
-  <si>
-    <t>0.20359334740895113</t>
-  </si>
-  <si>
-    <t>5.575782049044225</t>
-  </si>
-  <si>
-    <t>53.27212156633548</t>
-  </si>
-  <si>
-    <t>12632665.32238457</t>
-  </si>
-  <si>
-    <t>557032315.926242</t>
-  </si>
-  <si>
-    <t>294179.3671450702</t>
-  </si>
-  <si>
-    <t>0.030284256398936008</t>
-  </si>
-  <si>
-    <t>1390.1967270601988</t>
-  </si>
-  <si>
-    <t>0.1625010785575919</t>
-  </si>
-  <si>
-    <t>0.39700273598976077</t>
-  </si>
-  <si>
-    <t>21.251309565133074</t>
-  </si>
-  <si>
-    <t>0.012152459509410804</t>
-  </si>
-  <si>
-    <t>6.4034360243300705</t>
-  </si>
-  <si>
-    <t>0.013491541568299056</t>
-  </si>
-  <si>
-    <t>12627171.471741641</t>
-  </si>
-  <si>
-    <t>-8.809608232869971</t>
-  </si>
-  <si>
-    <t>8.53316187328064</t>
-  </si>
-  <si>
-    <t>29432211.11180527</t>
-  </si>
-  <si>
-    <t>1.0065760897469374</t>
-  </si>
-  <si>
-    <t>9.090990169609945</t>
-  </si>
-  <si>
-    <t>3.1402730265371184</t>
-  </si>
-  <si>
-    <t>33.829369787743516</t>
-  </si>
-  <si>
-    <t>5.410598494670352</t>
-  </si>
-  <si>
-    <t>-0.1303854314743861</t>
-  </si>
-  <si>
-    <t>-0.0977268531605957</t>
-  </si>
-  <si>
-    <t>-43.846870401755375</t>
-  </si>
-  <si>
-    <t>77.67624018949888</t>
-  </si>
-  <si>
-    <t>3.768495457704781</t>
-  </si>
-  <si>
-    <t>6.812903318422244</t>
-  </si>
-  <si>
-    <t>-0.044406226524763774</t>
-  </si>
-  <si>
-    <t>0.4995148451528526</t>
-  </si>
-  <si>
-    <t>46.398651265428065</t>
-  </si>
-  <si>
-    <t>6.2382646726666255</t>
-  </si>
-  <si>
-    <t>0.5409473239020136</t>
-  </si>
-  <si>
-    <t>0.0040998360614003864</t>
-  </si>
-  <si>
-    <t>0.5320418427218232</t>
-  </si>
-  <si>
-    <t>0.471858445715077</t>
-  </si>
-  <si>
-    <t>0.0599426098358187</t>
-  </si>
-  <si>
-    <t>0.4712001875697342</t>
-  </si>
-  <si>
-    <t>0.9772088785699782</t>
-  </si>
-  <si>
-    <t>0.24175660686716666</t>
-  </si>
-  <si>
-    <t>0.7645093952028924</t>
-  </si>
-  <si>
-    <t>0.7644657320296671</t>
-  </si>
-  <si>
-    <t>0.972255293245062</t>
-  </si>
-  <si>
-    <t>0.9057818792010163</t>
-  </si>
-  <si>
-    <t>-0.026915194493449018</t>
-  </si>
-  <si>
-    <t>0.172913808283394</t>
-  </si>
-  <si>
-    <t>0.4706262961110176</t>
-  </si>
-  <si>
-    <t>2.494637949717704</t>
-  </si>
-  <si>
-    <t>0.25846652502212025</t>
-  </si>
-  <si>
-    <t>1.9850581604248392</t>
-  </si>
-  <si>
-    <t>0.14760852461679844</t>
-  </si>
-  <si>
-    <t>0.28902503287767994</t>
-  </si>
-  <si>
-    <t>4.989275899435408</t>
-  </si>
-  <si>
-    <t>1.5103881627226485</t>
-  </si>
-  <si>
-    <t>0.2509750721092251</t>
-  </si>
-  <si>
-    <t>155486.60996348757</t>
-  </si>
-  <si>
-    <t>0.49889144267503244</t>
-  </si>
-  <si>
-    <t>0.2522329655744762</t>
-  </si>
-  <si>
-    <t>6.487990821792195</t>
-  </si>
-  <si>
-    <t>7.610469252602249</t>
-  </si>
-  <si>
-    <t>49.07257785649134</t>
-  </si>
-  <si>
-    <t>1.3858122986235368</t>
-  </si>
-  <si>
-    <t>0.18148263215815813</t>
-  </si>
-  <si>
-    <t>3.058723589915843</t>
-  </si>
-  <si>
-    <t>105421.62396940179</t>
-  </si>
-  <si>
-    <t>0.32710990659399813</t>
-  </si>
-  <si>
-    <t>0.49147254265366364</t>
-  </si>
-  <si>
-    <t>2.6711236136732306</t>
-  </si>
-  <si>
-    <t>0.5633417380260347</t>
-  </si>
-  <si>
-    <t>3.6655883927151014</t>
-  </si>
-  <si>
-    <t>0.10217779567241006</t>
-  </si>
-  <si>
-    <t>121.1003861003861</t>
-  </si>
-  <si>
-    <t>0.46756905830264905</t>
-  </si>
-  <si>
-    <t>1.8218571577644935</t>
-  </si>
-  <si>
-    <t>5.915057915057915</t>
-  </si>
-  <si>
-    <t>775405037.5868726</t>
-  </si>
-  <si>
-    <t>4995307160.208494</t>
-  </si>
-  <si>
-    <t>141248844.32260832</t>
-  </si>
-  <si>
-    <t>0.6497479622479623</t>
-  </si>
-  <si>
-    <t>140.13513513513513</t>
-  </si>
-  <si>
-    <t>0.5410622978190546</t>
-  </si>
-  <si>
-    <t>0.7619503103687546</t>
-  </si>
-  <si>
-    <t>4.826622125040997</t>
-  </si>
-  <si>
-    <t>0.47189909844247957</t>
-  </si>
-  <si>
-    <t>2.5819136750760903</t>
-  </si>
-  <si>
-    <t>0.0004084522812611871</t>
-  </si>
-  <si>
-    <t>769411029.1761305</t>
-  </si>
-  <si>
-    <t>-10.630978776512505</t>
-  </si>
-  <si>
-    <t>10.578249340845547</t>
-  </si>
-  <si>
-    <t>44389160.42773468</t>
-  </si>
-  <si>
-    <t>1.0384035911136702</t>
-  </si>
-  <si>
-    <t>11.07074418860554</t>
-  </si>
-  <si>
-    <t>3.1952028427719137</t>
-  </si>
-  <si>
-    <t>43.40257555204428</t>
-  </si>
-  <si>
-    <t>6.624961432960594</t>
-  </si>
-  <si>
-    <t>-0.02628007094336357</t>
-  </si>
-  <si>
-    <t>-0.017325918756206114</t>
-  </si>
-  <si>
-    <t>-42.407417608242056</t>
-  </si>
-  <si>
-    <t>85.80999316028634</t>
-  </si>
-  <si>
-    <t>4.5927174042512275</t>
-  </si>
-  <si>
-    <t>8.366797277300797</t>
-  </si>
-  <si>
-    <t>-0.0025848358294432937</t>
-  </si>
-  <si>
-    <t>0.49591985680497425</t>
-  </si>
-  <si>
-    <t>70.00260603731923</t>
-  </si>
-  <si>
-    <t>6.2525934835063435</t>
-  </si>
-  <si>
-    <t>0.5814739620650771</t>
-  </si>
-  <si>
-    <t>0.00025196966105141413</t>
-  </si>
-  <si>
-    <t>0.5281907767843645</t>
-  </si>
-  <si>
-    <t>0.5041462910804211</t>
-  </si>
-  <si>
-    <t>0.023287408555033848</t>
-  </si>
-  <si>
-    <t>0.49582195913765353</t>
-  </si>
-  <si>
-    <t>1.012233812888287</t>
-  </si>
-  <si>
-    <t>0.25090395695886947</t>
-  </si>
-  <si>
-    <t>0.7534641253497628</t>
-  </si>
-  <si>
-    <t>0.7529214536254499</t>
-  </si>
-  <si>
-    <t>0.9704943573089937</t>
-  </si>
-  <si>
-    <t>0.9011116820480619</t>
-  </si>
-  <si>
-    <t>-0.02281347749051697</t>
-  </si>
-  <si>
-    <t>0.11374928195838074</t>
-  </si>
-  <si>
-    <t>0.48865418177392794</t>
-  </si>
-  <si>
-    <t>2.4993163434919214</t>
-  </si>
-  <si>
-    <t>0.25327962777252494</t>
-  </si>
-  <si>
-    <t>2.052233246637429</t>
-  </si>
-  <si>
-    <t>0.09762316752565842</t>
-  </si>
-  <si>
-    <t>0.2710430912929739</t>
-  </si>
-  <si>
-    <t>4.998632686983841</t>
-  </si>
-  <si>
-    <t>1.5270097301270804</t>
-  </si>
-  <si>
-    <t>0.2580842669661964</t>
-  </si>
-  <si>
-    <t>159656.69085177575</t>
-  </si>
-  <si>
-    <t>0.49208121298026963</t>
-  </si>
-  <si>
-    <t>0.26597077573459177</t>
-  </si>
-  <si>
-    <t>6.51215371735436</t>
-  </si>
-  <si>
-    <t>6.668380060823783</t>
-  </si>
-  <si>
-    <t>43.320752829832976</t>
-  </si>
-  <si>
-    <t>1.2084903558654678</t>
-  </si>
-  <si>
-    <t>0.18347694268129283</t>
-  </si>
-  <si>
-    <t>2.9969098706069457</t>
-  </si>
-  <si>
-    <t>117127.42683027117</t>
-  </si>
-  <si>
-    <t>0.35071106541870345</t>
-  </si>
-  <si>
-    <t>0.5114745733905773</t>
-  </si>
-  <si>
-    <t>2.1404045853678384</t>
-  </si>
-  <si>
-    <t>0.5694734758780957</t>
-  </si>
-  <si>
-    <t>3.7160661694768247</t>
-  </si>
-  <si>
-    <t>0.10556628301309767</t>
-  </si>
-  <si>
-    <t>874.129650507328</t>
-  </si>
-  <si>
-    <t>0.4927450115599369</t>
-  </si>
-  <si>
-    <t>2.235262510342934</t>
-  </si>
-  <si>
-    <t>8.530439684329199</t>
-  </si>
-  <si>
-    <t>112396368.80665164</t>
-  </si>
-  <si>
-    <t>729514721.1899662</t>
-  </si>
-  <si>
-    <t>20323281.009700302</t>
-  </si>
-  <si>
-    <t>0.5258126644118752</t>
-  </si>
-  <si>
-    <t>894.499436302142</t>
-  </si>
-  <si>
-    <t>0.504227416179336</t>
-  </si>
-  <si>
-    <t>0.7300617888445314</t>
-  </si>
-  <si>
-    <t>6.2474106343078715</t>
-  </si>
-  <si>
-    <t>0.38222892656426</t>
-  </si>
-  <si>
-    <t>2.3718181015605606</t>
-  </si>
-  <si>
-    <t>0.0027976615712638838</t>
-  </si>
-  <si>
-    <t>112268604.46978751</t>
-  </si>
-  <si>
-    <t>-4.239571556346607</t>
-  </si>
-  <si>
-    <t>4.247038027046694</t>
-  </si>
-  <si>
-    <t>7100357.203068243</t>
-  </si>
-  <si>
-    <t>0.9999998417511424</t>
-  </si>
-  <si>
-    <t>4.428815211987702</t>
-  </si>
-  <si>
-    <t>3.1935872041468727</t>
-  </si>
-  <si>
-    <t>17.899031030391804</t>
-  </si>
-  <si>
-    <t>2.6494519455527548</t>
-  </si>
-  <si>
-    <t>0.0005843546841485427</t>
-  </si>
-  <si>
-    <t>-0.002160410320928544</t>
-  </si>
-  <si>
-    <t>-17.086001110892887</t>
-  </si>
-  <si>
-    <t>34.98503214128469</t>
-  </si>
-  <si>
-    <t>1.8369640667316982</t>
-  </si>
-  <si>
-    <t>3.3462692286237914</t>
-  </si>
-  <si>
-    <t>0.002461160194135485</t>
-  </si>
-  <si>
-    <t>0.5000001096897451</t>
-  </si>
-  <si>
-    <t>11.197517408964066</t>
-  </si>
-  <si>
-    <t>2.2464727919821352</t>
-  </si>
-  <si>
-    <t>0.49443870715804117</t>
-  </si>
-  <si>
-    <t>0.00024324057551431495</t>
-  </si>
-  <si>
-    <t>0.4944387148918304</t>
-  </si>
-  <si>
-    <t>0.5055609333818329</t>
-  </si>
-  <si>
-    <t>-0.011122221067931724</t>
-  </si>
-  <si>
-    <t>0.9945000555538156</t>
-  </si>
-  <si>
-    <t>0.2481006236866842</t>
-  </si>
-  <si>
-    <t>0.7472195333090835</t>
-  </si>
-  <si>
-    <t>0.8988878133236334</t>
-  </si>
-  <si>
-    <t>0.8314796888727223</t>
-  </si>
-  <si>
-    <t>-0.005499952863089552</t>
-  </si>
-  <si>
-    <t>0.08460494966885602</t>
-  </si>
-  <si>
-    <t>1.499751086224351</t>
-  </si>
-  <si>
-    <t>0.25189955217648424</t>
-  </si>
-  <si>
-    <t>1.9944995409038127</t>
-  </si>
-  <si>
-    <t>0.07072562914872645</t>
-  </si>
-  <si>
-    <t>0.26780865361918704</t>
-  </si>
-  <si>
-    <t>2.999502172448702</t>
-  </si>
-  <si>
-    <t>1.48893860752198</t>
-  </si>
-  <si>
-    <t>0.2499999120684158</t>
-  </si>
-  <si>
-    <t>166454.5188552955</t>
-  </si>
-  <si>
-    <t>0.5000001715074961</t>
-  </si>
-  <si>
-    <t>0.24999991424625195</t>
-  </si>
-  <si>
-    <t>2.5000354889146146</t>
-  </si>
-  <si>
-    <t>5.492601316967868</t>
-  </si>
-  <si>
-    <t>13.71684356849421</t>
-  </si>
-  <si>
-    <t>3.4365407540862813</t>
-  </si>
-  <si>
-    <t>0.6249911277713464</t>
-  </si>
-  <si>
-    <t>2.8801103718520205</t>
-  </si>
-  <si>
-    <t>119149.7070081807</t>
-  </si>
-  <si>
-    <t>0.3569820722890613</t>
-  </si>
-  <si>
-    <t>0.5250093014786651</t>
-  </si>
-  <si>
-    <t>1.7989646948062785</t>
-  </si>
-  <si>
-    <t>0.6004418464003302</t>
-  </si>
-  <si>
-    <t>1.5014959376934707</t>
-  </si>
-  <si>
-    <t>0.37517832357704517</t>
+    <t>(301, 262, 252)</t>
+  </si>
+  <si>
+    <t>873329176c5a1a87a89a5aed8d2f14224774c647</t>
+  </si>
+  <si>
+    <t>(79, 84, 38, 151, 142, 110)</t>
+  </si>
+  <si>
+    <t>(147.41899725968807, 158.85562938067272, 98.63745484355901)</t>
+  </si>
+  <si>
+    <t>149.09057649630307</t>
+  </si>
+  <si>
+    <t>166.20770138594662</t>
+  </si>
+  <si>
+    <t>159.3643623900902</t>
+  </si>
+  <si>
+    <t>167.30212192318422</t>
+  </si>
+  <si>
+    <t>476609.625</t>
+  </si>
+  <si>
+    <t>0.41920244310979</t>
+  </si>
+  <si>
+    <t>70388.57803168587</t>
+  </si>
+  <si>
+    <t>0.14768601878672902</t>
+  </si>
+  <si>
+    <t>-554.0</t>
+  </si>
+  <si>
+    <t>-299.0000000000001</t>
+  </si>
+  <si>
+    <t>97928135018.00002</t>
+  </si>
+  <si>
+    <t>3.897388727180078</t>
+  </si>
+  <si>
+    <t>131.00000000000006</t>
+  </si>
+  <si>
+    <t>2.6921959409964806</t>
+  </si>
+  <si>
+    <t>-189.0000000000001</t>
+  </si>
+  <si>
+    <t>77.6062418675275</t>
+  </si>
+  <si>
+    <t>-442.8819191828126</t>
+  </si>
+  <si>
+    <t>-459.0</t>
+  </si>
+  <si>
+    <t>-859.0000000000002</t>
+  </si>
+  <si>
+    <t>670.0000000000001</t>
+  </si>
+  <si>
+    <t>55.07213795633091</t>
+  </si>
+  <si>
+    <t>453.12283559183925</t>
+  </si>
+  <si>
+    <t>0.49183745848603755</t>
+  </si>
+  <si>
+    <t>0.07695351795528375</t>
+  </si>
+  <si>
+    <t>9175.909795737643</t>
+  </si>
+  <si>
+    <t>316.32374109265413</t>
+  </si>
+  <si>
+    <t>6273.201952796737</t>
+  </si>
+  <si>
+    <t>143.65314787243864</t>
+  </si>
+  <si>
+    <t>48.10378893149224</t>
+  </si>
+  <si>
+    <t>4.495897912363345</t>
+  </si>
+  <si>
+    <t>0.8284166020469172</t>
+  </si>
+  <si>
+    <t>1.5196268221136449</t>
+  </si>
+  <si>
+    <t>2.287292517427908</t>
+  </si>
+  <si>
+    <t>2.1273710170000735</t>
+  </si>
+  <si>
+    <t>0.5321340444564144</t>
+  </si>
+  <si>
+    <t>0.4793382443766854</t>
+  </si>
+  <si>
+    <t>0.9944232226630395</t>
+  </si>
+  <si>
+    <t>0.9507378761886518</t>
+  </si>
+  <si>
+    <t>-0.24406882346097417</t>
+  </si>
+  <si>
+    <t>0.9119135200949936</t>
+  </si>
+  <si>
+    <t>0.4392287580916952</t>
+  </si>
+  <si>
+    <t>17.47625476415888</t>
+  </si>
+  <si>
+    <t>0.014285654128574066</t>
+  </si>
+  <si>
+    <t>6.736809119735909</t>
+  </si>
+  <si>
+    <t>0.8451606945831439</t>
+  </si>
+  <si>
+    <t>0.0347943439949817</t>
+  </si>
+  <si>
+    <t>34.95250952831776</t>
+  </si>
+  <si>
+    <t>4.780438005344774</t>
+  </si>
+  <si>
+    <t>13.149921710963895</t>
+  </si>
+  <si>
+    <t>26993.43765724858</t>
+  </si>
+  <si>
+    <t>0.07323424078604257</t>
+  </si>
+  <si>
+    <t>15.518972552875052</t>
+  </si>
+  <si>
+    <t>342.6786777476542</t>
+  </si>
+  <si>
+    <t>2.146800461621195</t>
+  </si>
+  <si>
+    <t>671.9958481642926</t>
+  </si>
+  <si>
+    <t>0.008144791747935443</t>
+  </si>
+  <si>
+    <t>0.003546272265979649</t>
+  </si>
+  <si>
+    <t>4.909838340141035</t>
+  </si>
+  <si>
+    <t>239847.0776656182</t>
+  </si>
+  <si>
+    <t>0.6488731079572664</t>
+  </si>
+  <si>
+    <t>0.7726334589652359</t>
+  </si>
+  <si>
+    <t>0.45939865926347606</t>
+  </si>
+  <si>
+    <t>0.8326554087839662</t>
+  </si>
+  <si>
+    <t>293.5402446580625</t>
+  </si>
+  <si>
+    <t>0.0028822571831264372</t>
+  </si>
+  <si>
+    <t>2106.1066235864296</t>
+  </si>
+  <si>
+    <t>0.07732804463160632</t>
+  </si>
+  <si>
+    <t>17.431806080168574</t>
+  </si>
+  <si>
+    <t>483.1283962402702</t>
+  </si>
+  <si>
+    <t>342504.01318108384</t>
+  </si>
+  <si>
+    <t>97863381.64789249</t>
+  </si>
+  <si>
+    <t>1263.3790576811582</t>
+  </si>
+  <si>
+    <t>0.0026623417591559295</t>
+  </si>
+  <si>
+    <t>7119.336466441475</t>
+  </si>
+  <si>
+    <t>0.26139434815837403</t>
+  </si>
+  <si>
+    <t>0.5227686171928956</t>
+  </si>
+  <si>
+    <t>255.38207051040487</t>
+  </si>
+  <si>
+    <t>0.001378283766474774</t>
+  </si>
+  <si>
+    <t>6.716825881159491</t>
+  </si>
+  <si>
+    <t>0.05710415911001713</t>
+  </si>
+  <si>
+    <t>342197.3479648055</t>
+  </si>
+  <si>
+    <t>-27.452449258683266</t>
+  </si>
+  <si>
+    <t>42.42723606449577</t>
+  </si>
+  <si>
+    <t>461881460.54501057</t>
+  </si>
+  <si>
+    <t>2.303276767541524</t>
+  </si>
+  <si>
+    <t>35.21422124044498</t>
+  </si>
+  <si>
+    <t>6.010374246736705</t>
+  </si>
+  <si>
+    <t>254.45614788544464</t>
+  </si>
+  <si>
+    <t>22.542163429957604</t>
+  </si>
+  <si>
+    <t>7.299480628126834</t>
+  </si>
+  <si>
+    <t>5.79872799448302</t>
+  </si>
+  <si>
+    <t>-134.40099729722948</t>
+  </si>
+  <si>
+    <t>388.8571451826741</t>
+  </si>
+  <si>
+    <t>14.719590464858657</t>
+  </si>
+  <si>
+    <t>31.11913185864649</t>
+  </si>
+  <si>
+    <t>0.73147994264525</t>
+  </si>
+  <si>
+    <t>0.25115567729149035</t>
+  </si>
+  <si>
+    <t>915.1179501954282</t>
+  </si>
+  <si>
+    <t>46.915840138937384</t>
+  </si>
+  <si>
+    <t>138.01508498731133</t>
+  </si>
+  <si>
+    <t>8.204305158455982</t>
+  </si>
+  <si>
+    <t>4.646114533675597</t>
+  </si>
+  <si>
+    <t>1.2969420853439855</t>
+  </si>
+  <si>
+    <t>0.561662181822639</t>
+  </si>
+  <si>
+    <t>0.8113787273874933</t>
+  </si>
+  <si>
+    <t>1.5565961712173895</t>
+  </si>
+  <si>
+    <t>0.6031665317965511</t>
+  </si>
+  <si>
+    <t>0.6633229223568088</t>
+  </si>
+  <si>
+    <t>0.6416322517305021</t>
+  </si>
+  <si>
+    <t>0.995587814335566</t>
+  </si>
+  <si>
+    <t>0.9562959262397926</t>
+  </si>
+  <si>
+    <t>-0.14155902969911716</t>
+  </si>
+  <si>
+    <t>0.6304298243824931</t>
+  </si>
+  <si>
+    <t>0.4904281393818367</t>
+  </si>
+  <si>
+    <t>6.788116801435418</t>
+  </si>
+  <si>
+    <t>0.08138993921199947</t>
+  </si>
+  <si>
+    <t>4.237285431815671</t>
+  </si>
+  <si>
+    <t>0.6613280416381726</t>
+  </si>
+  <si>
+    <t>0.16090516024948825</t>
+  </si>
+  <si>
+    <t>13.576233602870836</t>
+  </si>
+  <si>
+    <t>3.071523601107041</t>
+  </si>
+  <si>
+    <t>1.4857641547548952</t>
+  </si>
+  <si>
+    <t>68419.10869681576</t>
+  </si>
+  <si>
+    <t>0.2268283035747635</t>
+  </si>
+  <si>
+    <t>1.8388435982400932</t>
+  </si>
+  <si>
+    <t>48.27028148547257</t>
+  </si>
+  <si>
+    <t>3.853918921513841</t>
+  </si>
+  <si>
+    <t>180.93778019666695</t>
+  </si>
+  <si>
+    <t>0.09132135738520214</t>
+  </si>
+  <si>
+    <t>0.024460718211021512</t>
+  </si>
+  <si>
+    <t>3.908739425932297</t>
+  </si>
+  <si>
+    <t>147125.59376695895</t>
+  </si>
+  <si>
+    <t>0.4750517073176624</t>
+  </si>
+  <si>
+    <t>0.6325253141375484</t>
+  </si>
+  <si>
+    <t>1.1558693915050517</t>
+  </si>
+  <si>
+    <t>0.7064619632115694</t>
+  </si>
+  <si>
+    <t>34.454202585369586</t>
+  </si>
+  <si>
+    <t>0.017491798584521514</t>
+  </si>
+  <si>
+    <t>1126.3837160751566</t>
+  </si>
+  <si>
+    <t>0.15676878442242959</t>
+  </si>
+  <si>
+    <t>7.105960118529626</t>
+  </si>
+  <si>
+    <t>54.060403618649964</t>
+  </si>
+  <si>
+    <t>7425005.020320111</t>
+  </si>
+  <si>
+    <t>339848531.3152401</t>
+  </si>
+  <si>
+    <t>168328.11781764994</t>
+  </si>
+  <si>
+    <t>0.03509645054744694</t>
+  </si>
+  <si>
+    <t>1239.6246346555324</t>
+  </si>
+  <si>
+    <t>0.17252952465630234</t>
+  </si>
+  <si>
+    <t>0.41179719606941984</t>
+  </si>
+  <si>
+    <t>21.738335644729073</t>
+  </si>
+  <si>
+    <t>0.014909004032049998</t>
+  </si>
+  <si>
+    <t>6.556386761117183</t>
+  </si>
+  <si>
+    <t>0.015064377412449445</t>
+  </si>
+  <si>
+    <t>7420598.481254219</t>
+  </si>
+  <si>
+    <t>-30.99673963439823</t>
+  </si>
+  <si>
+    <t>37.021168763908044</t>
+  </si>
+  <si>
+    <t>348094413.8514012</t>
+  </si>
+  <si>
+    <t>2.198931759313996</t>
+  </si>
+  <si>
+    <t>35.490971439093435</t>
+  </si>
+  <si>
+    <t>3.201688796864167</t>
+  </si>
+  <si>
+    <t>155.03418232277045</t>
+  </si>
+  <si>
+    <t>21.262613802145356</t>
+  </si>
+  <si>
+    <t>2.9821777741178113</t>
+  </si>
+  <si>
+    <t>2.899999576140371</t>
+  </si>
+  <si>
+    <t>-138.7303492568759</t>
+  </si>
+  <si>
+    <t>293.76453157964636</t>
+  </si>
+  <si>
+    <t>14.738933957352401</t>
+  </si>
+  <si>
+    <t>27.01535846441306</t>
+  </si>
+  <si>
+    <t>0.01892123179948021</t>
+  </si>
+  <si>
+    <t>0.2564831351662572</t>
+  </si>
+  <si>
+    <t>720.9362086842922</t>
+  </si>
+  <si>
+    <t>44.132176687249995</t>
+  </si>
+  <si>
+    <t>30.939985374345213</t>
+  </si>
+  <si>
+    <t>0.14031663550530327</t>
+  </si>
+  <si>
+    <t>3.0218514386514235</t>
+  </si>
+  <si>
+    <t>1.8752994042284472</t>
+  </si>
+  <si>
+    <t>0.23359786273985478</t>
+  </si>
+  <si>
+    <t>1.007426637432759</t>
+  </si>
+  <si>
+    <t>1.7509762834103841</t>
+  </si>
+  <si>
+    <t>0.8038143302969535</t>
+  </si>
+  <si>
+    <t>0.6131993125790932</t>
+  </si>
+  <si>
+    <t>0.5799768471933692</t>
+  </si>
+  <si>
+    <t>0.9893125445474202</t>
+  </si>
+  <si>
+    <t>0.9319509790055414</t>
+  </si>
+  <si>
+    <t>-0.05811834003033205</t>
+  </si>
+  <si>
+    <t>0.28071913990089004</t>
+  </si>
+  <si>
+    <t>0.488321963066296</t>
+  </si>
+  <si>
+    <t>6.6215961460536095</t>
+  </si>
+  <si>
+    <t>0.07366887548333355</t>
+  </si>
+  <si>
+    <t>4.257074910585179</t>
+  </si>
+  <si>
+    <t>0.24316899519356738</t>
+  </si>
+  <si>
+    <t>0.1338921477335873</t>
+  </si>
+  <si>
+    <t>13.243192292107219</t>
+  </si>
+  <si>
+    <t>2.8257598438517095</t>
+  </si>
+  <si>
+    <t>1.2242877107199674</t>
+  </si>
+  <si>
+    <t>77637.35345507303</t>
+  </si>
+  <si>
+    <t>0.2344593225227857</t>
+  </si>
+  <si>
+    <t>1.4308439841818397</t>
+  </si>
+  <si>
+    <t>45.246970350141936</t>
+  </si>
+  <si>
+    <t>2.9680886943008966</t>
+  </si>
+  <si>
+    <t>132.8758610444759</t>
+  </si>
+  <si>
+    <t>0.07298166254636647</t>
+  </si>
+  <si>
+    <t>0.02552496228633007</t>
+  </si>
+  <si>
+    <t>3.5389846294460625</t>
+  </si>
+  <si>
+    <t>185495.526528917</t>
+  </si>
+  <si>
+    <t>0.54865621365228</t>
+  </si>
+  <si>
+    <t>0.6951249349032778</t>
+  </si>
+  <si>
+    <t>0.789889864603539</t>
+  </si>
+  <si>
+    <t>0.7626932594168776</t>
+  </si>
+  <si>
+    <t>34.630781532949314</t>
+  </si>
+  <si>
+    <t>0.019726734800817505</t>
+  </si>
+  <si>
+    <t>2572.096554993679</t>
+  </si>
+  <si>
+    <t>0.203231396570297</t>
+  </si>
+  <si>
+    <t>5.610563305222629</t>
+  </si>
+  <si>
+    <t>48.83786346396966</t>
+  </si>
+  <si>
+    <t>4165689.013511378</t>
+  </si>
+  <si>
+    <t>184274128.60880214</t>
+  </si>
+  <si>
+    <t>97588.51309230455</t>
+  </si>
+  <si>
+    <t>0.035801258923240986</t>
+  </si>
+  <si>
+    <t>2645.8693109987357</t>
+  </si>
+  <si>
+    <t>0.20906047021165738</t>
+  </si>
+  <si>
+    <t>0.44902769963196887</t>
+  </si>
+  <si>
+    <t>21.92611122348676</t>
+  </si>
+  <si>
+    <t>0.016679901066139362</t>
+  </si>
+  <si>
+    <t>5.539948113089338</t>
+  </si>
+  <si>
+    <t>0.026535109329430782</t>
+  </si>
+  <si>
+    <t>4164268.784966095</t>
+  </si>
+  <si>
+    <t>-11.662070272462202</t>
+  </si>
+  <si>
+    <t>11.478173617280206</t>
+  </si>
+  <si>
+    <t>39954204.919842206</t>
+  </si>
+  <si>
+    <t>1.0688467583901922</t>
+  </si>
+  <si>
+    <t>12.060781063115245</t>
+  </si>
+  <si>
+    <t>3.2295631717633158</t>
+  </si>
+  <si>
+    <t>47.25681010949555</t>
+  </si>
+  <si>
+    <t>7.237524204297984</t>
+  </si>
+  <si>
+    <t>-0.08285988424022567</t>
+  </si>
+  <si>
+    <t>-0.045385059434024655</t>
+  </si>
+  <si>
+    <t>-56.7946744556509</t>
+  </si>
+  <si>
+    <t>104.05148456514644</t>
+  </si>
+  <si>
+    <t>5.0091109158976455</t>
+  </si>
+  <si>
+    <t>9.15257832128129</t>
+  </si>
+  <si>
+    <t>-0.021065318246950206</t>
+  </si>
+  <si>
+    <t>0.4918384679920214</t>
+  </si>
+  <si>
+    <t>83.76282416677189</t>
+  </si>
+  <si>
+    <t>12.238182824990519</t>
+  </si>
+  <si>
+    <t>0.6667442613911636</t>
+  </si>
+  <si>
+    <t>-0.0018209798058019854</t>
+  </si>
+  <si>
+    <t>0.5523121372054152</t>
+  </si>
+  <si>
+    <t>0.512080125075699</t>
+  </si>
+  <si>
+    <t>0.03778418803994048</t>
+  </si>
+  <si>
+    <t>0.4963663330696877</t>
+  </si>
+  <si>
+    <t>1.0360545400755112</t>
+  </si>
+  <si>
+    <t>0.2584234248710028</t>
+  </si>
+  <si>
+    <t>0.7544114869624233</t>
+  </si>
+  <si>
+    <t>0.7533881174940056</t>
+  </si>
+  <si>
+    <t>0.980432946197983</t>
+  </si>
+  <si>
+    <t>0.9176446748866222</t>
+  </si>
+  <si>
+    <t>-0.022919001412160245</t>
+  </si>
+  <si>
+    <t>0.11213572301180218</t>
+  </si>
+  <si>
+    <t>0.48284570740719995</t>
+  </si>
+  <si>
+    <t>3.496873546085738</t>
+  </si>
+  <si>
+    <t>0.2492422661120111</t>
+  </si>
+  <si>
+    <t>2.110586509972948</t>
+  </si>
+  <si>
+    <t>0.09758507295020188</t>
+  </si>
+  <si>
+    <t>0.26886818112580346</t>
+  </si>
+  <si>
+    <t>6.993747092171476</t>
+  </si>
+  <si>
+    <t>1.565563307389433</t>
+  </si>
+  <si>
+    <t>0.2660980655702786</t>
+  </si>
+  <si>
+    <t>118633.91977933598</t>
+  </si>
+  <si>
+    <t>0.48446221341910317</t>
+  </si>
+  <si>
+    <t>0.2816165197277786</t>
+  </si>
+  <si>
+    <t>12.519858389304117</t>
+  </si>
+  <si>
+    <t>6.532359849792186</t>
+  </si>
+  <si>
+    <t>81.50171217414193</t>
+  </si>
+  <si>
+    <t>0.5695480223675322</t>
+  </si>
+  <si>
+    <t>0.08785599861475185</t>
+  </si>
+  <si>
+    <t>3.0357337343825797</t>
+  </si>
+  <si>
+    <t>88498.61223091828</t>
+  </si>
+  <si>
+    <t>0.3515569060967833</t>
+  </si>
+  <si>
+    <t>0.5131282892089513</t>
+  </si>
+  <si>
+    <t>2.077570935218635</t>
+  </si>
+  <si>
+    <t>0.5732763438457954</t>
+  </si>
+  <si>
+    <t>7.1933747221114945</t>
+  </si>
+  <si>
+    <t>0.05071391388327055</t>
+  </si>
+  <si>
+    <t>1196.1410839884154</t>
+  </si>
+  <si>
+    <t>0.49488667107505807</t>
+  </si>
+  <si>
+    <t>2.232193388131819</t>
+  </si>
+  <si>
+    <t>13.837815473727762</t>
+  </si>
+  <si>
+    <t>46284904.23707075</t>
+  </si>
+  <si>
+    <t>577425648.9366984</t>
+  </si>
+  <si>
+    <t>4025673.6023062333</t>
+  </si>
+  <si>
+    <t>0.15174562129361469</t>
+  </si>
+  <si>
+    <t>1036.043442283823</t>
+  </si>
+  <si>
+    <t>0.4286485073578084</t>
+  </si>
+  <si>
+    <t>0.6592648297500854</t>
+  </si>
+  <si>
+    <t>9.233703242498706</t>
+  </si>
+  <si>
+    <t>0.09908677574172658</t>
+  </si>
+  <si>
+    <t>2.590874013176724</t>
+  </si>
+  <si>
+    <t>0.005067585275698025</t>
+  </si>
+  <si>
+    <t>46245964.0647722</t>
+  </si>
+  <si>
+    <t>-25.31232060212171</t>
+  </si>
+  <si>
+    <t>41.075014562422055</t>
+  </si>
+  <si>
+    <t>432328935.7560903</t>
+  </si>
+  <si>
+    <t>2.2368780434695483</t>
+  </si>
+  <si>
+    <t>33.07534408044431</t>
+  </si>
+  <si>
+    <t>7.064277447792561</t>
+  </si>
+  <si>
+    <t>257.69123023420605</t>
+  </si>
+  <si>
+    <t>21.46204417759037</t>
+  </si>
+  <si>
+    <t>7.481378357413428</t>
+  </si>
+  <si>
+    <t>5.608415929790858</t>
+  </si>
+  <si>
+    <t>-141.86641882133432</t>
+  </si>
+  <si>
+    <t>399.55764905554037</t>
+  </si>
+  <si>
+    <t>13.857461235998143</t>
+  </si>
+  <si>
+    <t>30.107130116677354</t>
+  </si>
+  <si>
+    <t>0.9354175371854468</t>
+  </si>
+  <si>
+    <t>0.26444174456790615</t>
+  </si>
+  <si>
+    <t>850.4682617357661</t>
+  </si>
+  <si>
+    <t>46.856826115754934</t>
+  </si>
+  <si>
+    <t>144.0592774064484</t>
+  </si>
+  <si>
+    <t>9.437273789361225</t>
+  </si>
+  <si>
+    <t>4.319345669916762</t>
+  </si>
+  <si>
+    <t>1.1918382525034716</t>
+  </si>
+  <si>
+    <t>0.5648489403311292</t>
+  </si>
+  <si>
+    <t>0.7702846962311567</t>
+  </si>
+  <si>
+    <t>1.5106551069450755</t>
+  </si>
+  <si>
+    <t>0.5655027362298307</t>
+  </si>
+  <si>
+    <t>0.6751855736637365</t>
+  </si>
+  <si>
+    <t>0.6559023933523318</t>
+  </si>
+  <si>
+    <t>0.9959420613224992</t>
+  </si>
+  <si>
+    <t>0.9583991517188704</t>
+  </si>
+  <si>
+    <t>-0.14512550685823145</t>
+  </si>
+  <si>
+    <t>0.6278536888462136</t>
+  </si>
+  <si>
+    <t>0.4874821472686856</t>
+  </si>
+  <si>
+    <t>6.787850050944944</t>
+  </si>
+  <si>
+    <t>0.09065213538241491</t>
+  </si>
+  <si>
+    <t>4.093125228293528</t>
+  </si>
+  <si>
+    <t>0.6676890023438963</t>
+  </si>
+  <si>
+    <t>0.17520944753205234</t>
+  </si>
+  <si>
+    <t>13.575700101889888</t>
+  </si>
+  <si>
+    <t>2.9928180178642254</t>
+  </si>
+  <si>
+    <t>1.377795980605059</t>
+  </si>
+  <si>
+    <t>69414.83606819369</t>
+  </si>
+  <si>
+    <t>0.23615702765727078</t>
+  </si>
+  <si>
+    <t>1.7542564579422826</t>
+  </si>
+  <si>
+    <t>48.41955193375596</t>
+  </si>
+  <si>
+    <t>4.144471814199442</t>
+  </si>
+  <si>
+    <t>194.02944487251432</t>
+  </si>
+  <si>
+    <t>0.09731021569467616</t>
+  </si>
+  <si>
+    <t>0.02405230877525303</t>
+  </si>
+  <si>
+    <t>3.9128381012498332</t>
+  </si>
+  <si>
+    <t>138739.300935743</t>
+  </si>
+  <si>
+    <t>0.45827183607066596</t>
+  </si>
+  <si>
+    <t>0.6163998742659532</t>
+  </si>
+  <si>
+    <t>1.2761980837980846</t>
+  </si>
+  <si>
+    <t>0.6918196005603012</t>
+  </si>
+  <si>
+    <t>33.96361315789965</t>
+  </si>
+  <si>
+    <t>0.01679475180222019</t>
+  </si>
+  <si>
+    <t>1138.543804034582</t>
+  </si>
+  <si>
+    <t>0.16405530317501182</t>
+  </si>
+  <si>
+    <t>6.606585782624222</t>
+  </si>
+  <si>
+    <t>55.153746397694526</t>
+  </si>
+  <si>
+    <t>7788309.268731988</t>
+  </si>
+  <si>
+    <t>347360050.298415</t>
+  </si>
+  <si>
+    <t>179704.22347306655</t>
+  </si>
+  <si>
+    <t>0.03194572031297528</t>
+  </si>
+  <si>
+    <t>1204.3368876080692</t>
+  </si>
+  <si>
+    <t>0.17353557458329527</t>
+  </si>
+  <si>
+    <t>0.41241028991553674</t>
+  </si>
+  <si>
+    <t>22.729350003995087</t>
+  </si>
+  <si>
+    <t>0.013400351853814985</t>
+  </si>
+  <si>
+    <t>6.495297947513132</t>
+  </si>
+  <si>
+    <t>0.014550699964147411</t>
+  </si>
+  <si>
+    <t>7783586.11339873</t>
+  </si>
+  <si>
+    <t>-9.74331317386002</t>
+  </si>
+  <si>
+    <t>9.560070009483459</t>
+  </si>
+  <si>
+    <t>27384333.05694929</t>
+  </si>
+  <si>
+    <t>1.0165304005271452</t>
+  </si>
+  <si>
+    <t>10.127912749021995</t>
+  </si>
+  <si>
+    <t>3.1189394711900413</t>
+  </si>
+  <si>
+    <t>38.942830236380956</t>
+  </si>
+  <si>
+    <t>6.023315968720801</t>
+  </si>
+  <si>
+    <t>-0.0967446565295133</t>
+  </si>
+  <si>
+    <t>-0.06810203020405053</t>
+  </si>
+  <si>
+    <t>-43.74977836913596</t>
+  </si>
+  <si>
+    <t>82.69260860551691</t>
+  </si>
+  <si>
+    <t>4.199944900828623</t>
+  </si>
+  <si>
+    <t>7.577279229581549</t>
+  </si>
+  <si>
+    <t>-0.024736588270704057</t>
+  </si>
+  <si>
+    <t>0.49848756308512143</t>
+  </si>
+  <si>
+    <t>57.40580099448093</t>
+  </si>
+  <si>
+    <t>6.247554847347296</t>
+  </si>
+  <si>
+    <t>0.5570057348363386</t>
+  </si>
+  <si>
+    <t>0.0016261578072145533</t>
+  </si>
+  <si>
+    <t>0.5339543524458424</t>
+  </si>
+  <si>
+    <t>0.47764418309796636</t>
+  </si>
+  <si>
+    <t>0.05565122586594953</t>
+  </si>
+  <si>
+    <t>0.47524460761996046</t>
+  </si>
+  <si>
+    <t>0.9824085530470851</t>
+  </si>
+  <si>
+    <t>0.24253218854765604</t>
+  </si>
+  <si>
+    <t>0.7627763159053258</t>
+  </si>
+  <si>
+    <t>0.7626176537378206</t>
+  </si>
+  <si>
+    <t>0.971945961571734</t>
+  </si>
+  <si>
+    <t>0.905030914664586</t>
+  </si>
+  <si>
+    <t>-0.03013292854154585</t>
+  </si>
+  <si>
+    <t>0.18851328952826288</t>
+  </si>
+  <si>
+    <t>0.4731573468697493</t>
+  </si>
+  <si>
+    <t>2.496693197186256</t>
+  </si>
+  <si>
+    <t>0.2584357343355521</t>
+  </si>
+  <si>
+    <t>2.000905874136291</t>
+  </si>
+  <si>
+    <t>0.16092093009139574</t>
+  </si>
+  <si>
+    <t>0.2903129550750517</t>
+  </si>
+  <si>
+    <t>4.993386394372512</t>
+  </si>
+  <si>
+    <t>1.515230216147756</t>
+  </si>
+  <si>
+    <t>0.25289963388595216</t>
+  </si>
+  <si>
+    <t>118377.32917513141</t>
+  </si>
+  <si>
+    <t>0.4969471865875045</t>
+  </si>
+  <si>
+    <t>0.2561335793933361</t>
+  </si>
+  <si>
+    <t>6.4953103494520015</t>
+  </si>
+  <si>
+    <t>7.4033139000754415</t>
+  </si>
+  <si>
+    <t>47.929462002710686</t>
+  </si>
+  <si>
+    <t>1.3437313174482217</t>
+  </si>
+  <si>
+    <t>0.18206172067689258</t>
+  </si>
+  <si>
+    <t>3.047351367828271</t>
+  </si>
+  <si>
+    <t>82239.0363747722</t>
+  </si>
+  <si>
+    <t>0.3326036811156144</t>
+  </si>
+  <si>
+    <t>0.4993509278208191</t>
+  </si>
+  <si>
+    <t>2.540722701360259</t>
+  </si>
+  <si>
+    <t>0.5690210879157348</t>
+  </si>
+  <si>
+    <t>3.704151758864415</t>
+  </si>
+  <si>
+    <t>0.10390348649164863</t>
+  </si>
+  <si>
+    <t>221.6828282828283</t>
+  </si>
+  <si>
+    <t>0.44784409754106724</t>
+  </si>
+  <si>
+    <t>2.12070605040302</t>
+  </si>
+  <si>
+    <t>7.832323232323232</t>
+  </si>
+  <si>
+    <t>229055647.65858585</t>
+  </si>
+  <si>
+    <t>1480874754.420202</t>
+  </si>
+  <si>
+    <t>41579131.08869248</t>
+  </si>
+  <si>
+    <t>0.5459876543209877</t>
+  </si>
+  <si>
+    <t>226.74141414141414</t>
+  </si>
+  <si>
+    <t>0.45806346291194777</t>
+  </si>
+  <si>
+    <t>0.6902818462402509</t>
+  </si>
+  <si>
+    <t>5.760103395062195</t>
+  </si>
+  <si>
+    <t>0.34969128787880066</t>
+  </si>
+  <si>
+    <t>2.7091579981421794</t>
+  </si>
+  <si>
+    <t>0.0010378381098347217</t>
+  </si>
+  <si>
+    <t>228127235.60182023</t>
+  </si>
+  <si>
+    <t>-11.113954962695813</t>
+  </si>
+  <si>
+    <t>11.004728799212263</t>
+  </si>
+  <si>
+    <t>36225668.2192334</t>
+  </si>
+  <si>
+    <t>1.049404100845884</t>
+  </si>
+  <si>
+    <t>11.515850522370215</t>
+  </si>
+  <si>
+    <t>3.1874425907367314</t>
+  </si>
+  <si>
+    <t>40.41205292988452</t>
+  </si>
+  <si>
+    <t>6.898958186449761</t>
+  </si>
+  <si>
+    <t>-0.042126452551670884</t>
+  </si>
+  <si>
+    <t>-0.04068330825802319</t>
+  </si>
+  <si>
+    <t>-49.817811401328115</t>
+  </si>
+  <si>
+    <t>90.22986433121264</t>
+  </si>
+  <si>
+    <t>4.7795101605708625</t>
+  </si>
+  <si>
+    <t>8.715060577702726</t>
+  </si>
+  <si>
+    <t>-0.0030111120472740335</t>
+  </si>
+  <si>
+    <t>0.4945086074811243</t>
+  </si>
+  <si>
+    <t>75.95050623502352</t>
+  </si>
+  <si>
+    <t>6.249495099318305</t>
+  </si>
+  <si>
+    <t>0.6115042580495936</t>
+  </si>
+  <si>
+    <t>0.0021111464372240464</t>
+  </si>
+  <si>
+    <t>0.5375893127650218</t>
+  </si>
+  <si>
+    <t>0.5064538068403063</t>
+  </si>
+  <si>
+    <t>0.029823456928439292</t>
+  </si>
+  <si>
+    <t>0.4953264450764848</t>
+  </si>
+  <si>
+    <t>1.0215947758453667</t>
+  </si>
+  <si>
+    <t>0.2537252678763675</t>
+  </si>
+  <si>
+    <t>0.7541777268912019</t>
+  </si>
+  <si>
+    <t>0.7534495136381397</t>
+  </si>
+  <si>
+    <t>0.9704084235660938</t>
+  </si>
+  <si>
+    <t>0.9013040675161227</t>
+  </si>
+  <si>
+    <t>-0.02297608794615539</t>
+  </si>
+  <si>
+    <t>0.10938742702306054</t>
+  </si>
+  <si>
+    <t>0.48571855058699587</t>
+  </si>
+  <si>
+    <t>2.4983415686173296</t>
+  </si>
+  <si>
+    <t>0.2518179523560974</t>
+  </si>
+  <si>
+    <t>2.074370071841239</t>
+  </si>
+  <si>
+    <t>0.09452360615982837</t>
+  </si>
+  <si>
+    <t>0.2700706123487521</t>
+  </si>
+  <si>
+    <t>4.996683137234659</t>
+  </si>
+  <si>
+    <t>1.5418896781229654</t>
+  </si>
+  <si>
+    <t>0.26101077990133204</t>
+  </si>
+  <si>
+    <t>120107.40469180768</t>
+  </si>
+  <si>
+    <t>0.4894462577366284</t>
+  </si>
+  <si>
+    <t>0.27134541107607074</t>
+  </si>
+  <si>
+    <t>6.519418133954142</t>
+  </si>
+  <si>
+    <t>6.610419209649824</t>
+  </si>
+  <si>
+    <t>42.88797399058473</t>
+  </si>
+  <si>
+    <t>1.2008912419905156</t>
+  </si>
+  <si>
+    <t>0.18434949464141576</t>
+  </si>
+  <si>
+    <t>3.0035925673710597</t>
+  </si>
+  <si>
+    <t>89011.27374673277</t>
+  </si>
+  <si>
+    <t>0.3526691697701626</t>
+  </si>
+  <si>
+    <t>0.5142704756104819</t>
+  </si>
+  <si>
+    <t>2.1448692245968624</t>
+  </si>
+  <si>
+    <t>0.5734263492661617</t>
+  </si>
+  <si>
+    <t>3.7511723974061324</t>
+  </si>
+  <si>
+    <t>0.10705670432648987</t>
+  </si>
+  <si>
+    <t>862.5587392550143</t>
+  </si>
+  <si>
+    <t>0.49430300243840364</t>
+  </si>
+  <si>
+    <t>2.238538599847292</t>
+  </si>
+  <si>
+    <t>8.487106017191977</t>
+  </si>
+  <si>
+    <t>64461670.31232092</t>
+  </si>
+  <si>
+    <t>417796745.48194844</t>
+  </si>
+  <si>
+    <t>11672361.478326967</t>
+  </si>
+  <si>
+    <t>0.5294293218720153</t>
+  </si>
+  <si>
+    <t>822.374212034384</t>
+  </si>
+  <si>
+    <t>0.4712746200770109</t>
+  </si>
+  <si>
+    <t>0.701020773638989</t>
+  </si>
+  <si>
+    <t>5.902380611270429</t>
+  </si>
+  <si>
+    <t>0.3738544402658426</t>
+  </si>
+  <si>
+    <t>2.427014040401765</t>
+  </si>
+  <si>
+    <t>0.0036586414174981604</t>
+  </si>
+  <si>
+    <t>64386963.48258749</t>
+  </si>
+  <si>
+    <t>-4.366398087517293</t>
+  </si>
+  <si>
+    <t>4.366757285861174</t>
+  </si>
+  <si>
+    <t>5624020.713767576</t>
+  </si>
+  <si>
+    <t>0.9999997050196525</t>
+  </si>
+  <si>
+    <t>4.545901319079837</t>
+  </si>
+  <si>
+    <t>3.152436296641418</t>
+  </si>
+  <si>
+    <t>18.625893711070276</t>
+  </si>
+  <si>
+    <t>2.719859808920952</t>
+  </si>
+  <si>
+    <t>0.0009768589271358158</t>
+  </si>
+  <si>
+    <t>0.0027746657734626368</t>
+  </si>
+  <si>
+    <t>-15.87259813231157</t>
+  </si>
+  <si>
+    <t>34.49849184338184</t>
+  </si>
+  <si>
+    <t>1.8854176183248965</t>
+  </si>
+  <si>
+    <t>3.433884341559541</t>
+  </si>
+  <si>
+    <t>0.0018766524438670975</t>
+  </si>
+  <si>
+    <t>0.5000002044647818</t>
+  </si>
+  <si>
+    <t>11.791560716954452</t>
+  </si>
+  <si>
+    <t>2.248783706319103</t>
+  </si>
+  <si>
+    <t>0.4950765817007532</t>
+  </si>
+  <si>
+    <t>-0.0003929308447897645</t>
+  </si>
+  <si>
+    <t>0.4950766450099237</t>
+  </si>
+  <si>
+    <t>0.5049225207125239</t>
+  </si>
+  <si>
+    <t>-0.009845896805701488</t>
+  </si>
+  <si>
+    <t>0.9947416465253216</t>
+  </si>
+  <si>
+    <t>0.24818344249320928</t>
+  </si>
+  <si>
+    <t>0.747538739643738</t>
+  </si>
+  <si>
+    <t>0.8990154958574953</t>
+  </si>
+  <si>
+    <t>0.8316924930958254</t>
+  </si>
+  <si>
+    <t>-0.005258397862198987</t>
+  </si>
+  <si>
+    <t>0.08218028444362267</t>
+  </si>
+  <si>
+    <t>1.5004149888917884</t>
+  </si>
+  <si>
+    <t>0.25181697464556696</t>
+  </si>
+  <si>
+    <t>1.994740401987435</t>
+  </si>
+  <si>
+    <t>0.06868442699957587</t>
+  </si>
+  <si>
+    <t>0.2673428404606731</t>
+  </si>
+  <si>
+    <t>3.0008299777835767</t>
+  </si>
+  <si>
+    <t>1.4898178812749114</t>
+  </si>
+  <si>
+    <t>0.2499997914306119</t>
+  </si>
+  <si>
+    <t>126137.76063438939</t>
+  </si>
+  <si>
+    <t>0.500000265737813</t>
+  </si>
+  <si>
+    <t>0.2499998671310935</t>
+  </si>
+  <si>
+    <t>2.4995824566659337</t>
+  </si>
+  <si>
+    <t>5.375396699468739</t>
+  </si>
+  <si>
+    <t>13.44173703324701</t>
+  </si>
+  <si>
+    <t>3.3588116160241714</t>
+  </si>
+  <si>
+    <t>0.6251043858335166</t>
+  </si>
+  <si>
+    <t>2.8657236610047603</t>
+  </si>
+  <si>
+    <t>91035.85763107147</t>
+  </si>
+  <si>
+    <t>0.36000985090777005</t>
+  </si>
+  <si>
+    <t>0.528931329953653</t>
+  </si>
+  <si>
+    <t>1.7404325488178698</t>
+  </si>
+  <si>
+    <t>0.6036472718009267</t>
+  </si>
+  <si>
+    <t>1.5076897065876158</t>
+  </si>
+  <si>
+    <t>0.37763666310425453</t>
   </si>
   <si>
     <t>1.0</t>
@@ -3901,253 +3901,253 @@
     <t>2.5</t>
   </si>
   <si>
-    <t>100521041602.5</t>
-  </si>
-  <si>
-    <t>251161358008.5</t>
-  </si>
-  <si>
-    <t>62860962501.0</t>
+    <t>56871064308.5</t>
+  </si>
+  <si>
+    <t>142286763770.0</t>
+  </si>
+  <si>
+    <t>35517139443.125</t>
   </si>
   <si>
     <t>0.625</t>
   </si>
   <si>
-    <t>9.948174646585382e-12</t>
-  </si>
-  <si>
-    <t>2.4884415180864975e-11</t>
-  </si>
-  <si>
-    <t>6.214114513015484e-12</t>
+    <t>1.758366311372392e-11</t>
+  </si>
+  <si>
+    <t>4.392542480607133e-11</t>
+  </si>
+  <si>
+    <t>1.0998222690637066e-11</t>
   </si>
   <si>
     <t>0.9999999999999993</t>
   </si>
   <si>
-    <t>3.1540716699705567e-06</t>
-  </si>
-  <si>
-    <t>22052.25</t>
-  </si>
-  <si>
-    <t>-1683.183368022202</t>
-  </si>
-  <si>
-    <t>-852.228051514049</t>
-  </si>
-  <si>
-    <t>1239002845930.162</t>
-  </si>
-  <si>
-    <t>5.425486927102052</t>
-  </si>
-  <si>
-    <t>422.25723158316737</t>
-  </si>
-  <si>
-    <t>2.7687836908700096</t>
-  </si>
-  <si>
-    <t>-505.09801386947845</t>
-  </si>
-  <si>
-    <t>254.4367274347488</t>
-  </si>
-  <si>
-    <t>-1362.8168262259383</t>
-  </si>
-  <si>
-    <t>-1455.9037888195842</t>
-  </si>
-  <si>
-    <t>-2496.931064709147</t>
-  </si>
-  <si>
-    <t>1991.8330508396684</t>
-  </si>
-  <si>
-    <t>181.86976218574574</t>
-  </si>
-  <si>
-    <t>1397.8382909623735</t>
-  </si>
-  <si>
-    <t>0.8013774794576782</t>
-  </si>
-  <si>
-    <t>0.028253632533345473</t>
-  </si>
-  <si>
-    <t>96682.1858360699</t>
-  </si>
-  <si>
-    <t>2157.179088265563</t>
-  </si>
-  <si>
-    <t>785879.4117938057</t>
-  </si>
-  <si>
-    <t>9662.242130564675</t>
-  </si>
-  <si>
-    <t>520.3215572454344</t>
-  </si>
-  <si>
-    <t>30.78048669116347</t>
-  </si>
-  <si>
-    <t>0.8875900934132984</t>
-  </si>
-  <si>
-    <t>3.7324092265601028</t>
-  </si>
-  <si>
-    <t>3.4286442600187264</t>
-  </si>
-  <si>
-    <t>16.334647338013585</t>
-  </si>
-  <si>
-    <t>0.3674725789247338</t>
-  </si>
-  <si>
-    <t>0.286183259388522</t>
-  </si>
-  <si>
-    <t>0.9953484052740866</t>
-  </si>
-  <si>
-    <t>0.9575049234707329</t>
-  </si>
-  <si>
-    <t>-0.2355454692105641</t>
-  </si>
-  <si>
-    <t>0.9529112091032318</t>
-  </si>
-  <si>
-    <t>0.2873995257930549</t>
-  </si>
-  <si>
-    <t>45.10840675170629</t>
-  </si>
-  <si>
-    <t>0.002723900932382153</t>
-  </si>
-  <si>
-    <t>9.466287500017355</t>
-  </si>
-  <si>
-    <t>0.8987165217352895</t>
-  </si>
-  <si>
-    <t>0.008732724718673281</t>
-  </si>
-  <si>
-    <t>90.21681350341262</t>
-  </si>
-  <si>
-    <t>6.331600175993382</t>
-  </si>
-  <si>
-    <t>137.77551098414943</t>
-  </si>
-  <si>
-    <t>15203.334288711789</t>
-  </si>
-  <si>
-    <t>0.02706316171258089</t>
-  </si>
-  <si>
-    <t>158.4142436357866</t>
-  </si>
-  <si>
-    <t>2329.3669435884262</t>
-  </si>
-  <si>
-    <t>1.4495960189483488</t>
-  </si>
-  <si>
-    <t>3136.41208187981</t>
-  </si>
-  <si>
-    <t>0.0008836187714630876</t>
-  </si>
-  <si>
-    <t>0.0005780626999763104</t>
-  </si>
-  <si>
-    <t>6.015484540372294</t>
-  </si>
-  <si>
-    <t>453910.6504006697</t>
-  </si>
-  <si>
-    <t>0.8074212388538814</t>
-  </si>
-  <si>
-    <t>0.8857799042690723</t>
-  </si>
-  <si>
-    <t>0.17261332135270083</t>
-  </si>
-  <si>
-    <t>0.9176600666820783</t>
-  </si>
-  <si>
-    <t>2179.227874172549</t>
-  </si>
-  <si>
-    <t>0.0005224430602443629</t>
-  </si>
-  <si>
-    <t>3312.9528213020576</t>
-  </si>
-  <si>
-    <t>0.021977052932098083</t>
-  </si>
-  <si>
-    <t>158.7136470541457</t>
-  </si>
-  <si>
-    <t>3095.3784976052434</t>
-  </si>
-  <si>
-    <t>9981.645410160138</t>
-  </si>
-  <si>
-    <t>12905141.072147852</t>
-  </si>
-  <si>
-    <t>7.879103844810533</t>
-  </si>
-  <si>
-    <t>0.00044843241988227133</t>
-  </si>
-  <si>
-    <t>59986.35338914466</t>
-  </si>
-  <si>
-    <t>0.3979299841398422</t>
-  </si>
-  <si>
-    <t>0.6555594475585891</t>
-  </si>
-  <si>
-    <t>2103.4100233204904</t>
-  </si>
-  <si>
-    <t>0.000279523474354909</t>
-  </si>
-  <si>
-    <t>7.734235184389572</t>
-  </si>
-  <si>
-    <t>0.23773184398069078</t>
-  </si>
-  <si>
-    <t>9963.951440347708</t>
+    <t>4.193285292261502e-06</t>
+  </si>
+  <si>
+    <t>23256.25</t>
+  </si>
+  <si>
+    <t>-1560.9119209295436</t>
+  </si>
+  <si>
+    <t>-847.0618997757402</t>
+  </si>
+  <si>
+    <t>781949606313.0084</t>
+  </si>
+  <si>
+    <t>5.383948488821796</t>
+  </si>
+  <si>
+    <t>368.65178428068793</t>
+  </si>
+  <si>
+    <t>2.701168891629534</t>
+  </si>
+  <si>
+    <t>-473.1283502312075</t>
+  </si>
+  <si>
+    <t>218.00836970285954</t>
+  </si>
+  <si>
+    <t>-1251.852775147744</t>
+  </si>
+  <si>
+    <t>-1298.303923393185</t>
+  </si>
+  <si>
+    <t>-2409.9796528110182</t>
+  </si>
+  <si>
+    <t>1936.8513025798106</t>
+  </si>
+  <si>
+    <t>154.71442177360504</t>
+  </si>
+  <si>
+    <t>1280.4174677506571</t>
+  </si>
+  <si>
+    <t>0.5119859512512627</t>
+  </si>
+  <si>
+    <t>0.027649587719087283</t>
+  </si>
+  <si>
+    <t>72333.52107589657</t>
+  </si>
+  <si>
+    <t>2256.6555400320995</t>
+  </si>
+  <si>
+    <t>391126.17337834195</t>
+  </si>
+  <si>
+    <t>3293.33313031585</t>
+  </si>
+  <si>
+    <t>379.6932132011015</t>
+  </si>
+  <si>
+    <t>31.012004596622276</t>
+  </si>
+  <si>
+    <t>0.8483267147670942</t>
+  </si>
+  <si>
+    <t>3.9487338839871695</t>
+  </si>
+  <si>
+    <t>3.4980638047460793</t>
+  </si>
+  <si>
+    <t>14.946965442884048</t>
+  </si>
+  <si>
+    <t>0.34263848355484466</t>
+  </si>
+  <si>
+    <t>0.2562026376297314</t>
+  </si>
+  <si>
+    <t>0.9951675724838398</t>
+  </si>
+  <si>
+    <t>0.954361254059529</t>
+  </si>
+  <si>
+    <t>-0.20433413675024617</t>
+  </si>
+  <si>
+    <t>0.9335702546539226</t>
+  </si>
+  <si>
+    <t>0.2613788078821788</t>
+  </si>
+  <si>
+    <t>46.577532038766485</t>
+  </si>
+  <si>
+    <t>0.002158986336287326</t>
+  </si>
+  <si>
+    <t>9.547779478083102</t>
+  </si>
+  <si>
+    <t>0.8727962150460016</t>
+  </si>
+  <si>
+    <t>0.005826433892687327</t>
+  </si>
+  <si>
+    <t>93.15506407753294</t>
+  </si>
+  <si>
+    <t>6.268432662544385</t>
+  </si>
+  <si>
+    <t>102.67630444943099</t>
+  </si>
+  <si>
+    <t>11660.591598789142</t>
+  </si>
+  <si>
+    <t>0.027063589137005236</t>
+  </si>
+  <si>
+    <t>118.27099861701966</t>
+  </si>
+  <si>
+    <t>2404.335309084695</t>
+  </si>
+  <si>
+    <t>1.3625755405564524</t>
+  </si>
+  <si>
+    <t>3126.163734112196</t>
+  </si>
+  <si>
+    <t>0.0007279948776348746</t>
+  </si>
+  <si>
+    <t>0.000515747198933074</t>
+  </si>
+  <si>
+    <t>5.89475892249926</t>
+  </si>
+  <si>
+    <t>358730.1652694468</t>
+  </si>
+  <si>
+    <t>0.8321037577400274</t>
+  </si>
+  <si>
+    <t>0.9032975189137328</t>
+  </si>
+  <si>
+    <t>0.1353222358055168</t>
+  </si>
+  <si>
+    <t>0.9294820981469409</t>
+  </si>
+  <si>
+    <t>2262.6108476221325</t>
+  </si>
+  <si>
+    <t>0.0004745915501467656</t>
+  </si>
+  <si>
+    <t>3133.7443369667776</t>
+  </si>
+  <si>
+    <t>0.024038602494318</t>
+  </si>
+  <si>
+    <t>129.45687728712295</t>
+  </si>
+  <si>
+    <t>3017.9394920337827</t>
+  </si>
+  <si>
+    <t>842.4002285924687</t>
+  </si>
+  <si>
+    <t>1359831.9954971885</t>
+  </si>
+  <si>
+    <t>0.5439319864447265</t>
+  </si>
+  <si>
+    <t>0.00042134360386933314</t>
+  </si>
+  <si>
+    <t>50824.909928430614</t>
+  </si>
+  <si>
+    <t>0.3898722024533849</t>
+  </si>
+  <si>
+    <t>0.6487486766927004</t>
+  </si>
+  <si>
+    <t>2054.0389540378837</t>
+  </si>
+  <si>
+    <t>0.00026087046454628676</t>
+  </si>
+  <si>
+    <t>7.653119734200569</t>
+  </si>
+  <si>
+    <t>0.2733246252775431</t>
+  </si>
+  <si>
+    <t>829.0144857537744</t>
   </si>
 </sst>
 </file>
@@ -4612,7 +4612,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-228.7198702921083</v>
+        <v>-533.6795878212815</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4620,7 +4620,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-3258</v>
+        <v>-32768.00000000013</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4628,7 +4628,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>17935.99999999999</v>
+        <v>32766.9999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4668,7 +4668,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>634101</v>
+        <v>476953</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4700,7 +4700,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.7718453225485958</v>
+        <v>0.7603064575404428</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4708,7 +4708,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.4521425931392275</v>
+        <v>0.4168015100057532</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4716,7 +4716,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>74.90454581447806</v>
+        <v>69.03670767584686</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4724,7 +4724,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>165.6657588802142</v>
+        <v>165.6344951218961</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4772,7 +4772,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>127.8683410981568</v>
+        <v>125.9329762326286</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4804,7 +4804,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>634101</v>
+        <v>476953</v>
       </c>
     </row>
     <row r="38" spans="1:2">

</xml_diff>

<commit_message>
Added Requirements txt and fixed canvas size
</commit_message>
<xml_diff>
--- a/Radiomics_Code/Output.xlsx
+++ b/Radiomics_Code/Output.xlsx
@@ -2131,7 +2131,7 @@
     <t>v3.0.1</t>
   </si>
   <si>
-    <t>1.19.2</t>
+    <t>1.19.5</t>
   </si>
   <si>
     <t>1.2.4</t>
@@ -2149,7 +2149,7 @@
     <t>{'Original': {}, 'Wavelet': {}}</t>
   </si>
   <si>
-    <t>9d48fd53743d76e5cb43ef55ee5c4c24dfcb0ac6</t>
+    <t>9faee00c7c4fd5780b7351656d5ddc4924cf1da8</t>
   </si>
   <si>
     <t>3D</t>
@@ -2158,1738 +2158,1738 @@
     <t>(1.0, 1.0, 1.0)</t>
   </si>
   <si>
-    <t>(327, 254, 246)</t>
-  </si>
-  <si>
-    <t>afd9a674e4c3d742bb9c7f67cd0fd1122ec64a73</t>
-  </si>
-  <si>
-    <t>(49, 63, 54, 148, 117, 107)</t>
-  </si>
-  <si>
-    <t>(132.49732898125748, 131.52383262241779, 113.64188320121674)</t>
-  </si>
-  <si>
-    <t>147.50254235097103</t>
-  </si>
-  <si>
-    <t>129.72663566130126</t>
-  </si>
-  <si>
-    <t>152.620444239951</t>
-  </si>
-  <si>
-    <t>163.55427233796127</t>
-  </si>
-  <si>
-    <t>319659.0416666667</t>
-  </si>
-  <si>
-    <t>0.4320762919423122</t>
-  </si>
-  <si>
-    <t>52325.69627737957</t>
-  </si>
-  <si>
-    <t>0.16369221406833734</t>
-  </si>
-  <si>
-    <t>-590.0000000000001</t>
-  </si>
-  <si>
-    <t>-278.0000000000001</t>
-  </si>
-  <si>
-    <t>66808864861.00001</t>
-  </si>
-  <si>
-    <t>4.178746267324081</t>
-  </si>
-  <si>
-    <t>175.0000000000001</t>
-  </si>
-  <si>
-    <t>2.2978262284986974</t>
-  </si>
-  <si>
-    <t>-200.00000000000003</t>
-  </si>
-  <si>
-    <t>95.87855302473753</t>
-  </si>
-  <si>
-    <t>-442.5276099154725</t>
-  </si>
-  <si>
-    <t>-451.0000000000001</t>
-  </si>
-  <si>
-    <t>-894.0000000000001</t>
-  </si>
-  <si>
-    <t>694.0000000000001</t>
-  </si>
-  <si>
-    <t>71.73840987059125</t>
-  </si>
-  <si>
-    <t>457.25003922447956</t>
-  </si>
-  <si>
-    <t>0.10059944848071939</t>
-  </si>
-  <si>
-    <t>0.059419012398684426</t>
-  </si>
-  <si>
-    <t>13246.912833287506</t>
-  </si>
-  <si>
-    <t>357.3513719133053</t>
-  </si>
-  <si>
-    <t>12687.74276997176</t>
-  </si>
-  <si>
-    <t>51.52793469130607</t>
-  </si>
-  <si>
-    <t>73.8068338404101</t>
-  </si>
-  <si>
-    <t>4.69875210467553</t>
-  </si>
-  <si>
-    <t>0.8799361205271083</t>
-  </si>
-  <si>
-    <t>1.5428981606903434</t>
-  </si>
-  <si>
-    <t>2.30742046842347</t>
-  </si>
-  <si>
-    <t>2.250525394859874</t>
-  </si>
-  <si>
-    <t>0.5305224004511854</t>
-  </si>
-  <si>
-    <t>0.47746822356349966</t>
-  </si>
-  <si>
-    <t>0.9941870336016652</t>
-  </si>
-  <si>
-    <t>0.9501059565497857</t>
-  </si>
-  <si>
-    <t>-0.28392900911934515</t>
-  </si>
-  <si>
-    <t>0.9458365903847855</t>
-  </si>
-  <si>
-    <t>0.43701891460346415</t>
-  </si>
-  <si>
-    <t>18.44099965123958</t>
-  </si>
-  <si>
-    <t>0.010006684069020572</t>
-  </si>
-  <si>
-    <t>7.1066872743002385</t>
-  </si>
-  <si>
-    <t>0.8933789898380607</t>
-  </si>
-  <si>
-    <t>0.02256160367911377</t>
-  </si>
-  <si>
-    <t>36.88199930247915</t>
-  </si>
-  <si>
-    <t>5.095033239093942</t>
-  </si>
-  <si>
-    <t>19.62639648627141</t>
-  </si>
-  <si>
-    <t>14528.068699474756</t>
-  </si>
-  <si>
-    <t>0.05869976964509446</t>
-  </si>
-  <si>
-    <t>21.61232918210451</t>
-  </si>
-  <si>
-    <t>386.2619237489314</t>
-  </si>
-  <si>
-    <t>2.1359263731931746</t>
-  </si>
-  <si>
-    <t>760.3633986797777</t>
-  </si>
-  <si>
-    <t>0.007970213981292915</t>
-  </si>
-  <si>
-    <t>0.003540637115301527</t>
-  </si>
-  <si>
-    <t>5.159800838669942</t>
-  </si>
-  <si>
-    <t>162075.2254621251</t>
-  </si>
-  <si>
-    <t>0.6530369667996836</t>
-  </si>
-  <si>
-    <t>0.7745362157691091</t>
-  </si>
-  <si>
-    <t>0.45796930560174265</t>
-  </si>
-  <si>
-    <t>0.8351455637391634</t>
-  </si>
-  <si>
-    <t>330.5058704031417</t>
-  </si>
-  <si>
-    <t>0.0029036287605257683</t>
-  </si>
-  <si>
-    <t>1183.0364188163885</t>
-  </si>
-  <si>
-    <t>0.06648886746565438</t>
-  </si>
-  <si>
-    <t>23.43152003107961</t>
-  </si>
-  <si>
-    <t>494.1334794582139</t>
-  </si>
-  <si>
-    <t>198301.2377339403</t>
-  </si>
-  <si>
-    <t>59689383.94098803</t>
-  </si>
-  <si>
-    <t>730.4694300882412</t>
-  </si>
-  <si>
-    <t>0.003345403436891983</t>
-  </si>
-  <si>
-    <t>4746.83004552352</t>
-  </si>
-  <si>
-    <t>0.26678075903577364</t>
-  </si>
-  <si>
-    <t>0.529095423909932</t>
-  </si>
-  <si>
-    <t>264.0076639344217</t>
-  </si>
-  <si>
-    <t>0.0015862957085870841</t>
-  </si>
-  <si>
-    <t>6.884757525618148</t>
-  </si>
-  <si>
-    <t>0.05568299529637824</t>
-  </si>
-  <si>
-    <t>197978.7190919659</t>
-  </si>
-  <si>
-    <t>-25.51203764836236</t>
-  </si>
-  <si>
-    <t>39.092150638566736</t>
-  </si>
-  <si>
-    <t>264914516.96221948</t>
-  </si>
-  <si>
-    <t>2.201485713705976</t>
-  </si>
-  <si>
-    <t>32.49557772926738</t>
-  </si>
-  <si>
-    <t>6.264860027327233</t>
-  </si>
-  <si>
-    <t>226.5402995786013</t>
-  </si>
-  <si>
-    <t>20.836879865760775</t>
-  </si>
-  <si>
-    <t>6.580330223122493</t>
-  </si>
-  <si>
-    <t>5.337225475375555</t>
-  </si>
-  <si>
-    <t>-133.52121913991138</t>
-  </si>
-  <si>
-    <t>360.0615187185127</t>
-  </si>
-  <si>
-    <t>13.581481389394733</t>
-  </si>
-  <si>
-    <t>28.793176793128666</t>
-  </si>
-  <si>
-    <t>0.6959461876475647</t>
-  </si>
-  <si>
-    <t>0.2697617495005678</t>
-  </si>
-  <si>
-    <t>785.7462839950239</t>
-  </si>
-  <si>
-    <t>46.47880393913091</t>
-  </si>
-  <si>
-    <t>103.74824015637844</t>
-  </si>
-  <si>
-    <t>6.03842015334409</t>
-  </si>
-  <si>
-    <t>3.987677779061705</t>
-  </si>
-  <si>
-    <t>1.1818743150870317</t>
-  </si>
-  <si>
-    <t>0.5412489957150141</t>
-  </si>
-  <si>
-    <t>0.769152509769648</t>
-  </si>
-  <si>
-    <t>1.5096800951386116</t>
-  </si>
-  <si>
-    <t>0.5598180858386999</t>
-  </si>
-  <si>
-    <t>0.6749678397054678</t>
-  </si>
-  <si>
-    <t>0.6557704550235525</t>
-  </si>
-  <si>
-    <t>0.995463367549031</t>
-  </si>
-  <si>
-    <t>0.9560616028032975</t>
-  </si>
-  <si>
-    <t>-0.13649075787437412</t>
-  </si>
-  <si>
-    <t>0.6118475904926853</t>
-  </si>
-  <si>
-    <t>0.4888604767605165</t>
-  </si>
-  <si>
-    <t>6.765895819162205</t>
-  </si>
-  <si>
-    <t>0.09173964262340108</t>
-  </si>
-  <si>
-    <t>4.065986753659068</t>
-  </si>
-  <si>
-    <t>0.645724779827243</t>
-  </si>
-  <si>
-    <t>0.1780232264694059</t>
-  </si>
-  <si>
-    <t>13.531791638324409</t>
-  </si>
-  <si>
-    <t>2.9623123497551136</t>
-  </si>
-  <si>
-    <t>1.2923880235371845</t>
-  </si>
-  <si>
-    <t>47889.02552994006</t>
-  </si>
-  <si>
-    <t>0.24197989044704532</t>
-  </si>
-  <si>
-    <t>1.6150339886182432</t>
-  </si>
-  <si>
-    <t>47.5404322510035</t>
-  </si>
-  <si>
-    <t>4.060010659669246</t>
-  </si>
-  <si>
-    <t>188.79771514202045</t>
-  </si>
-  <si>
-    <t>0.09573073545288163</t>
-  </si>
-  <si>
-    <t>0.024383833407871317</t>
-  </si>
-  <si>
-    <t>3.860664857807931</t>
-  </si>
-  <si>
-    <t>93745.79538362559</t>
-  </si>
-  <si>
-    <t>0.46128383300858994</t>
-  </si>
-  <si>
-    <t>0.6194076936798527</t>
-  </si>
-  <si>
-    <t>1.2454245442217307</t>
-  </si>
-  <si>
-    <t>0.6952784151158592</t>
-  </si>
-  <si>
-    <t>33.324330192818984</t>
-  </si>
-  <si>
-    <t>0.017187390619252743</t>
-  </si>
-  <si>
-    <t>859.8965230064543</t>
-  </si>
-  <si>
-    <t>0.1790332132014271</t>
-  </si>
-  <si>
-    <t>6.28014094702505</t>
-  </si>
-  <si>
-    <t>52.002290235269626</t>
-  </si>
-  <si>
-    <t>5330557.012492192</t>
-  </si>
-  <si>
-    <t>240226370.47636893</t>
-  </si>
-  <si>
-    <t>122059.25952148494</t>
-  </si>
-  <si>
-    <t>0.033812245387146805</t>
-  </si>
-  <si>
-    <t>801.3631063918384</t>
-  </si>
-  <si>
-    <t>0.1668463681848508</t>
-  </si>
-  <si>
-    <t>0.406583613636579</t>
-  </si>
-  <si>
-    <t>21.15305900619362</t>
-  </si>
-  <si>
-    <t>0.014201345174298607</t>
-  </si>
-  <si>
-    <t>6.4271067954032</t>
-  </si>
-  <si>
-    <t>0.015030934997386877</t>
-  </si>
-  <si>
-    <t>5326130.843344014</t>
-  </si>
-  <si>
-    <t>-30.083883735961955</t>
-  </si>
-  <si>
-    <t>36.00981796884413</t>
-  </si>
-  <si>
-    <t>219937372.93598503</t>
-  </si>
-  <si>
-    <t>2.158327811569458</t>
-  </si>
-  <si>
-    <t>34.39600470654029</t>
-  </si>
-  <si>
-    <t>3.213039709804077</t>
-  </si>
-  <si>
-    <t>155.47282306350138</t>
-  </si>
-  <si>
-    <t>20.62252842241267</t>
-  </si>
-  <si>
-    <t>2.9942013564147647</t>
-  </si>
-  <si>
-    <t>3.0043248842088786</t>
-  </si>
-  <si>
-    <t>-146.24136678422326</t>
-  </si>
-  <si>
-    <t>301.71418984772464</t>
-  </si>
-  <si>
-    <t>14.280062782898415</t>
-  </si>
-  <si>
-    <t>26.23531129278557</t>
-  </si>
-  <si>
-    <t>0.015090802358947168</t>
-  </si>
-  <si>
-    <t>0.26375325716822035</t>
-  </si>
-  <si>
-    <t>679.3263168666065</t>
-  </si>
-  <si>
-    <t>44.10045361336615</t>
-  </si>
-  <si>
-    <t>26.59211762196139</t>
-  </si>
-  <si>
-    <t>0.12555605752097734</t>
-  </si>
-  <si>
-    <t>2.804466378599034</t>
-  </si>
-  <si>
-    <t>1.8465241942093331</t>
-  </si>
-  <si>
-    <t>0.2056243058623634</t>
-  </si>
-  <si>
-    <t>0.9956861811572124</t>
-  </si>
-  <si>
-    <t>1.7420821306744807</t>
-  </si>
-  <si>
-    <t>0.7988717889611052</t>
-  </si>
-  <si>
-    <t>0.6163733149861196</t>
-  </si>
-  <si>
-    <t>0.5839277792699209</t>
-  </si>
-  <si>
-    <t>0.9894826490308293</t>
-  </si>
-  <si>
-    <t>0.9327068662709294</t>
-  </si>
-  <si>
-    <t>-0.05643929926371068</t>
-  </si>
-  <si>
-    <t>0.26609362247322665</t>
-  </si>
-  <si>
-    <t>0.4886639623607635</t>
-  </si>
-  <si>
-    <t>6.622761212825874</t>
-  </si>
-  <si>
-    <t>0.07728025459221696</t>
-  </si>
-  <si>
-    <t>4.188435656340294</t>
-  </si>
-  <si>
-    <t>0.2338059162297923</t>
-  </si>
-  <si>
-    <t>0.14099208786979284</t>
-  </si>
-  <si>
-    <t>13.245522425651748</t>
-  </si>
-  <si>
-    <t>2.7700687648190327</t>
-  </si>
-  <si>
-    <t>1.1627476432020918</t>
-  </si>
-  <si>
-    <t>53142.622478835954</t>
-  </si>
-  <si>
-    <t>0.24035430561186885</t>
-  </si>
-  <si>
-    <t>1.3588103565403746</t>
-  </si>
-  <si>
-    <t>45.14813185763215</t>
-  </si>
-  <si>
-    <t>2.999458850263378</t>
-  </si>
-  <si>
-    <t>134.2846781498745</t>
-  </si>
-  <si>
-    <t>0.0733038862318152</t>
-  </si>
-  <si>
-    <t>0.0253845712309258</t>
-  </si>
-  <si>
-    <t>3.506485389578383</t>
-  </si>
-  <si>
-    <t>123462.8560717573</t>
-  </si>
-  <si>
-    <t>0.5464490977978179</t>
-  </si>
-  <si>
-    <t>0.6928527048292588</t>
-  </si>
-  <si>
-    <t>0.802946708375117</t>
-  </si>
-  <si>
-    <t>0.7608696636200195</t>
-  </si>
-  <si>
-    <t>34.45730735358451</t>
-  </si>
-  <si>
-    <t>0.019572678474611048</t>
-  </si>
-  <si>
-    <t>1812.146888155649</t>
-  </si>
-  <si>
-    <t>0.20618351213512903</t>
-  </si>
-  <si>
-    <t>5.279833689856402</t>
-  </si>
-  <si>
-    <t>48.58129480031858</t>
-  </si>
-  <si>
-    <t>2811490.266355672</t>
-  </si>
-  <si>
-    <t>125574355.67186256</t>
-  </si>
-  <si>
-    <t>65137.634336952164</t>
-  </si>
-  <si>
-    <t>0.03480650625555799</t>
-  </si>
-  <si>
-    <t>1751.4874274661508</t>
-  </si>
-  <si>
-    <t>0.19928176441758458</t>
-  </si>
-  <si>
-    <t>0.4355699088597182</t>
-  </si>
-  <si>
-    <t>21.253379957377014</t>
-  </si>
-  <si>
-    <t>0.01572557979300106</t>
-  </si>
-  <si>
-    <t>5.5731536813532205</t>
-  </si>
-  <si>
-    <t>0.0275050775956763</t>
-  </si>
-  <si>
-    <t>2810168.440474594</t>
-  </si>
-  <si>
-    <t>-11.443582917016375</t>
-  </si>
-  <si>
-    <t>11.273175620774504</t>
-  </si>
-  <si>
-    <t>25899824.67080265</t>
-  </si>
-  <si>
-    <t>1.0663814663381095</t>
-  </si>
-  <si>
-    <t>11.88068587638731</t>
-  </si>
-  <si>
-    <t>3.2881028779252452</t>
-  </si>
-  <si>
-    <t>47.30668030446448</t>
-  </si>
-  <si>
-    <t>7.1136650622687245</t>
-  </si>
-  <si>
-    <t>-0.09868157056447138</t>
-  </si>
-  <si>
-    <t>-0.08269737376439229</t>
-  </si>
-  <si>
-    <t>-48.77458717929901</t>
-  </si>
-  <si>
-    <t>96.0812674837635</t>
-  </si>
-  <si>
-    <t>4.925261287344794</t>
-  </si>
-  <si>
-    <t>9.002955781206856</t>
-  </si>
-  <si>
-    <t>-0.003323636551402017</t>
-  </si>
-  <si>
-    <t>0.49220345545075206</t>
-  </si>
-  <si>
-    <t>81.04347474599685</t>
-  </si>
-  <si>
-    <t>6.2375666615066185</t>
-  </si>
-  <si>
-    <t>0.6557897864952325</t>
-  </si>
-  <si>
-    <t>0.002350532383232643</t>
-  </si>
-  <si>
-    <t>0.5471948962666733</t>
-  </si>
-  <si>
-    <t>0.5151184072845585</t>
-  </si>
-  <si>
-    <t>0.03019235273020047</t>
-  </si>
-  <si>
-    <t>0.4993947790515815</t>
-  </si>
-  <si>
-    <t>1.0356632001047001</t>
-  </si>
-  <si>
-    <t>0.2582838337183203</t>
-  </si>
-  <si>
-    <t>0.75288796702524</t>
-  </si>
-  <si>
-    <t>0.7518749732975069</t>
-  </si>
-  <si>
-    <t>0.9699853501889778</t>
-  </si>
-  <si>
-    <t>0.9006411367702725</t>
-  </si>
-  <si>
-    <t>-0.023194602434753617</t>
-  </si>
-  <si>
-    <t>0.1171253748667091</t>
-  </si>
-  <si>
-    <t>0.4859695035843439</t>
-  </si>
-  <si>
-    <t>2.4959060502795762</t>
-  </si>
-  <si>
-    <t>0.2495645598652603</t>
-  </si>
-  <si>
-    <t>2.1068026623066265</t>
-  </si>
-  <si>
-    <t>0.10060357276809222</t>
-  </si>
-  <si>
-    <t>0.2703331559555838</t>
-  </si>
-  <si>
-    <t>4.991812100559153</t>
-  </si>
-  <si>
-    <t>1.5590289222202705</t>
-  </si>
-  <si>
-    <t>0.26557832588780794</t>
-  </si>
-  <si>
-    <t>80482.9882866262</t>
-  </si>
-  <si>
-    <t>0.48531644216252734</t>
-  </si>
-  <si>
-    <t>0.2798204488471734</t>
-  </si>
-  <si>
-    <t>6.523044639326279</t>
-  </si>
-  <si>
-    <t>6.334743856107437</t>
-  </si>
-  <si>
-    <t>40.97755589380821</t>
-  </si>
-  <si>
-    <t>1.1568101253787453</t>
-  </si>
-  <si>
-    <t>0.18611843631107214</t>
-  </si>
-  <si>
-    <t>3.0112084663097582</t>
-  </si>
-  <si>
-    <t>60624.15097927748</t>
-  </si>
-  <si>
-    <t>0.35559106505798815</t>
-  </si>
-  <si>
-    <t>0.5187224078383585</t>
-  </si>
-  <si>
-    <t>2.003651219557445</t>
-  </si>
-  <si>
-    <t>0.5783093971065077</t>
-  </si>
-  <si>
-    <t>3.7913010730379004</t>
-  </si>
-  <si>
-    <t>0.10946649367938581</t>
-  </si>
-  <si>
-    <t>749.1927392739274</t>
-  </si>
-  <si>
-    <t>0.49451665958675073</t>
-  </si>
-  <si>
-    <t>2.2362496051585357</t>
-  </si>
-  <si>
-    <t>8.271947194719472</t>
-  </si>
-  <si>
-    <t>33168435.213861387</t>
-  </si>
-  <si>
-    <t>214352433.13861385</t>
-  </si>
-  <si>
-    <t>6023257.85519802</t>
-  </si>
-  <si>
-    <t>0.5427346901356802</t>
-  </si>
-  <si>
-    <t>628.652805280528</t>
-  </si>
-  <si>
-    <t>0.4149523467198205</t>
-  </si>
-  <si>
-    <t>0.64438781992613</t>
-  </si>
-  <si>
-    <t>5.393156042311293</t>
-  </si>
-  <si>
-    <t>0.3463408501129225</t>
-  </si>
-  <si>
-    <t>2.637264322801905</t>
-  </si>
-  <si>
-    <t>0.004741175623785367</t>
-  </si>
-  <si>
-    <t>33123948.747096255</t>
-  </si>
-  <si>
-    <t>-24.525639874051528</t>
-  </si>
-  <si>
-    <t>39.664592211105564</t>
-  </si>
-  <si>
-    <t>265556588.0268092</t>
-  </si>
-  <si>
-    <t>2.2007025843782935</t>
-  </si>
-  <si>
-    <t>32.06550374905719</t>
-  </si>
-  <si>
-    <t>5.6443387295313014</t>
-  </si>
-  <si>
-    <t>217.55288122164006</t>
-  </si>
-  <si>
-    <t>20.7530722772701</t>
-  </si>
-  <si>
-    <t>7.200339764111734</t>
-  </si>
-  <si>
-    <t>5.915770980386179</t>
-  </si>
-  <si>
-    <t>-137.69254268100983</t>
-  </si>
-  <si>
-    <t>355.2454239026499</t>
-  </si>
-  <si>
-    <t>13.447003259855165</t>
-  </si>
-  <si>
-    <t>28.828048565324366</t>
-  </si>
-  <si>
-    <t>0.5598435491205147</t>
-  </si>
-  <si>
-    <t>0.2712964703233449</t>
-  </si>
-  <si>
-    <t>779.2114913660512</t>
-  </si>
-  <si>
-    <t>46.73116165563171</t>
-  </si>
-  <si>
-    <t>98.76005503523074</t>
-  </si>
-  <si>
-    <t>5.337732340608726</t>
-  </si>
-  <si>
-    <t>4.027322408335365</t>
-  </si>
-  <si>
-    <t>1.1169321916550248</t>
-  </si>
-  <si>
-    <t>0.5638382141495495</t>
-  </si>
-  <si>
-    <t>0.7461040219415267</t>
-  </si>
-  <si>
-    <t>1.4783141674715758</t>
-  </si>
-  <si>
-    <t>0.5301796608905568</t>
-  </si>
-  <si>
-    <t>0.681345700696775</t>
-  </si>
-  <si>
-    <t>0.6634355229942747</t>
-  </si>
-  <si>
-    <t>0.995124867778342</t>
-  </si>
-  <si>
-    <t>0.9546921848414773</t>
-  </si>
-  <si>
-    <t>-0.1493783161712747</t>
-  </si>
-  <si>
-    <t>0.6369005314718924</t>
-  </si>
-  <si>
-    <t>0.4874211084743576</t>
-  </si>
-  <si>
-    <t>6.782590887326753</t>
-  </si>
-  <si>
-    <t>0.09462774794817488</t>
-  </si>
-  <si>
-    <t>4.031898826521307</t>
-  </si>
-  <si>
-    <t>0.6631553130209318</t>
-  </si>
-  <si>
-    <t>0.1845232614694822</t>
-  </si>
-  <si>
-    <t>13.565181774653508</t>
-  </si>
-  <si>
-    <t>2.966096066656606</t>
-  </si>
-  <si>
-    <t>1.2860636499975973</t>
-  </si>
-  <si>
-    <t>47318.648219512455</t>
-  </si>
-  <si>
-    <t>0.24256793798365525</t>
-  </si>
-  <si>
-    <t>1.595029850268553</t>
-  </si>
-  <si>
-    <t>47.89099095098061</t>
-  </si>
-  <si>
-    <t>4.240092101378661</t>
-  </si>
-  <si>
-    <t>198.4022965613237</t>
-  </si>
-  <si>
-    <t>0.09958048938966838</t>
-  </si>
-  <si>
-    <t>0.024300291274399324</t>
-  </si>
-  <si>
-    <t>3.89361926114183</t>
-  </si>
-  <si>
-    <t>90918.77137326621</t>
-  </si>
-  <si>
-    <t>0.45225844213777455</t>
-  </si>
-  <si>
-    <t>0.6107924515765762</t>
-  </si>
-  <si>
-    <t>1.3165509451305613</t>
-  </si>
-  <si>
-    <t>0.686533898418977</t>
-  </si>
-  <si>
-    <t>33.15889569130914</t>
-  </si>
-  <si>
-    <t>0.016923584030066753</t>
-  </si>
-  <si>
-    <t>848.5096260234565</t>
-  </si>
-  <si>
-    <t>0.18776490949844135</t>
-  </si>
-  <si>
-    <t>5.3610164376409575</t>
-  </si>
-  <si>
-    <t>50.087187430847536</t>
-  </si>
-  <si>
-    <t>5747921.400531091</t>
-  </si>
-  <si>
-    <t>261867951.40628457</t>
-  </si>
-  <si>
-    <t>130241.76745664232</t>
-  </si>
-  <si>
-    <t>0.034395044663436125</t>
-  </si>
-  <si>
-    <t>751.0801062181898</t>
-  </si>
-  <si>
-    <t>0.16620493609608097</t>
-  </si>
-  <si>
-    <t>0.40409299797371784</t>
-  </si>
-  <si>
-    <t>20.239606908146403</t>
-  </si>
-  <si>
-    <t>0.014259687574842519</t>
-  </si>
-  <si>
-    <t>6.357439226377471</t>
-  </si>
-  <si>
-    <t>0.014142160160980907</t>
-  </si>
-  <si>
-    <t>5742921.417881503</t>
-  </si>
-  <si>
-    <t>-9.500260958095897</t>
-  </si>
-  <si>
-    <t>9.229453325773145</t>
-  </si>
-  <si>
-    <t>17303274.01791407</t>
-  </si>
-  <si>
-    <t>1.012072708338398</t>
-  </si>
-  <si>
-    <t>9.840899663513742</t>
-  </si>
-  <si>
-    <t>3.1149017123825358</t>
-  </si>
-  <si>
-    <t>35.596597208981194</t>
-  </si>
-  <si>
-    <t>5.847405805943409</t>
-  </si>
-  <si>
-    <t>-0.12308028942942727</t>
-  </si>
-  <si>
-    <t>-0.0905905865480757</t>
-  </si>
-  <si>
-    <t>-39.06662507014806</t>
-  </si>
-  <si>
-    <t>74.66322227912926</t>
-  </si>
-  <si>
-    <t>4.075077394979293</t>
-  </si>
-  <si>
-    <t>7.358695760167122</t>
-  </si>
-  <si>
-    <t>-0.03333563327919083</t>
-  </si>
-  <si>
-    <t>0.4989680482202912</t>
-  </si>
-  <si>
-    <t>54.13525453305556</t>
-  </si>
-  <si>
-    <t>6.237787352679755</t>
-  </si>
-  <si>
-    <t>0.5482874931492894</t>
-  </si>
-  <si>
-    <t>0.0038092415728161735</t>
-  </si>
-  <si>
-    <t>0.53182915278728</t>
-  </si>
-  <si>
-    <t>0.47626493313320256</t>
-  </si>
-  <si>
-    <t>0.05510838160197792</t>
-  </si>
-  <si>
-    <t>0.47460779986293883</t>
-  </si>
-  <si>
-    <t>0.9803356793358016</t>
-  </si>
-  <si>
-    <t>0.24218774546883776</t>
-  </si>
-  <si>
-    <t>0.7629715294164849</t>
-  </si>
-  <si>
-    <t>0.7628618133955569</t>
-  </si>
-  <si>
-    <t>0.9720138522364297</t>
-  </si>
-  <si>
-    <t>0.9051335909996107</t>
-  </si>
-  <si>
-    <t>-0.028783702457956244</t>
-  </si>
-  <si>
-    <t>0.18282515524763962</t>
-  </si>
-  <si>
-    <t>0.47316498159434117</t>
-  </si>
-  <si>
-    <t>2.4947737278112885</t>
-  </si>
-  <si>
-    <t>0.25850240218921405</t>
-  </si>
-  <si>
-    <t>1.9939791910467621</t>
-  </si>
-  <si>
-    <t>0.15610908503607077</t>
-  </si>
-  <si>
-    <t>0.29051627048305567</t>
-  </si>
-  <si>
-    <t>4.989547455622577</t>
-  </si>
-  <si>
-    <t>1.511725170104646</t>
-  </si>
-  <si>
-    <t>0.2520235214801206</t>
-  </si>
-  <si>
-    <t>79864.24870781373</t>
-  </si>
-  <si>
-    <t>0.4978689800874458</t>
-  </si>
-  <si>
-    <t>0.2542758416023986</t>
-  </si>
-  <si>
-    <t>6.497636171482909</t>
-  </si>
-  <si>
-    <t>7.18804911188403</t>
-  </si>
-  <si>
-    <t>46.34656773582809</t>
-  </si>
-  <si>
-    <t>1.3095239015791118</t>
-  </si>
-  <si>
-    <t>0.1816314008718791</t>
-  </si>
-  <si>
-    <t>3.027251554515502</t>
-  </si>
-  <si>
-    <t>55648.1763577152</t>
-  </si>
-  <si>
-    <t>0.335051252622071</t>
-  </si>
-  <si>
-    <t>0.5019471438960644</t>
-  </si>
-  <si>
-    <t>2.4596214978555295</t>
-  </si>
-  <si>
-    <t>0.5719897390106199</t>
-  </si>
-  <si>
-    <t>3.7279806089560603</t>
-  </si>
-  <si>
-    <t>0.10396537314896677</t>
-  </si>
-  <si>
-    <t>106.65400843881856</t>
-  </si>
-  <si>
-    <t>0.4500169132439602</t>
-  </si>
-  <si>
-    <t>2.1054674286528154</t>
-  </si>
-  <si>
-    <t>7.569620253164557</t>
-  </si>
-  <si>
-    <t>214952071.38818565</t>
-  </si>
-  <si>
-    <t>1386815008.5400844</t>
-  </si>
-  <si>
-    <t>39098944.25035162</t>
-  </si>
-  <si>
-    <t>0.5605661040787624</t>
-  </si>
-  <si>
-    <t>122.78059071729957</t>
-  </si>
-  <si>
-    <t>0.5180615642080151</t>
-  </si>
-  <si>
-    <t>0.74676232694236</t>
-  </si>
-  <si>
-    <t>6.206502130038433</t>
-  </si>
-  <si>
-    <t>0.3819409193002689</t>
-  </si>
-  <si>
-    <t>2.61545472134062</t>
-  </si>
-  <si>
-    <t>0.000741688859958503</t>
-  </si>
-  <si>
-    <t>213134227.90368354</t>
-  </si>
-  <si>
-    <t>-10.92872479249587</t>
-  </si>
-  <si>
-    <t>10.850747538779403</t>
-  </si>
-  <si>
-    <t>23668022.9767824</t>
-  </si>
-  <si>
-    <t>1.0481081680373463</t>
-  </si>
-  <si>
-    <t>11.33470068427753</t>
-  </si>
-  <si>
-    <t>3.2446504763398187</t>
-  </si>
-  <si>
-    <t>49.0691165086209</t>
-  </si>
-  <si>
-    <t>6.803511772276829</t>
-  </si>
-  <si>
-    <t>-0.0340196304155148</t>
-  </si>
-  <si>
-    <t>-0.022608032532125455</t>
-  </si>
-  <si>
-    <t>-54.88380044015243</t>
-  </si>
-  <si>
-    <t>103.95291694877332</t>
-  </si>
-  <si>
-    <t>4.707948246172103</t>
-  </si>
-  <si>
-    <t>8.606324085107193</t>
-  </si>
-  <si>
-    <t>-0.0006897292658943468</t>
-  </si>
-  <si>
-    <t>0.4946786916803376</t>
-  </si>
-  <si>
-    <t>74.06765692264257</t>
-  </si>
-  <si>
-    <t>12.249186161290735</t>
-  </si>
-  <si>
-    <t>0.6083030329455379</t>
-  </si>
-  <si>
-    <t>-0.00033624338930181725</t>
-  </si>
-  <si>
-    <t>0.5363327440726137</t>
-  </si>
-  <si>
-    <t>0.5064762277499855</t>
-  </si>
-  <si>
-    <t>0.028631584798477647</t>
-  </si>
-  <si>
-    <t>0.49567566319768347</t>
-  </si>
-  <si>
-    <t>1.0211703539670642</t>
-  </si>
-  <si>
-    <t>0.25363615907026066</t>
-  </si>
-  <si>
-    <t>0.7539438119945936</t>
-  </si>
-  <si>
-    <t>0.7532421180237109</t>
-  </si>
-  <si>
-    <t>0.980608595041081</t>
-  </si>
-  <si>
-    <t>0.9176432230685148</t>
-  </si>
-  <si>
-    <t>-0.022178756858586748</t>
-  </si>
-  <si>
-    <t>0.10912147259553302</t>
-  </si>
-  <si>
-    <t>0.48639867244717383</t>
-  </si>
-  <si>
-    <t>3.4988171908358066</t>
-  </si>
-  <si>
-    <t>0.2517480531000946</t>
-  </si>
-  <si>
-    <t>2.072880550444307</t>
-  </si>
-  <si>
-    <t>0.09370311933507612</t>
-  </si>
-  <si>
-    <t>0.26931205300798927</t>
-  </si>
-  <si>
-    <t>6.997634381671613</t>
-  </si>
-  <si>
-    <t>1.5410089597520684</t>
-  </si>
-  <si>
-    <t>0.2607022429556498</t>
-  </si>
-  <si>
-    <t>81025.4387605968</t>
-  </si>
-  <si>
-    <t>0.48983794986809925</t>
-  </si>
-  <si>
-    <t>0.2705659815110404</t>
-  </si>
-  <si>
-    <t>12.515378428399675</t>
-  </si>
-  <si>
-    <t>6.405011439322299</t>
-  </si>
-  <si>
-    <t>80.00755500622394</t>
-  </si>
-  <si>
-    <t>0.5572581224035494</t>
-  </si>
-  <si>
-    <t>0.08745665480959607</t>
-  </si>
-  <si>
-    <t>2.9891543621697325</t>
-  </si>
-  <si>
-    <t>60324.80566319163</t>
-  </si>
-  <si>
-    <t>0.3548716142261865</t>
-  </si>
-  <si>
-    <t>0.5174407617849931</t>
-  </si>
-  <si>
-    <t>2.0479780386189717</t>
-  </si>
-  <si>
-    <t>0.5767502704239795</t>
-  </si>
-  <si>
-    <t>7.227640573550833</t>
-  </si>
-  <si>
-    <t>0.05067194932189039</t>
-  </si>
-  <si>
-    <t>567.0798611111111</t>
-  </si>
-  <si>
-    <t>0.49225682388117287</t>
-  </si>
-  <si>
-    <t>2.233608669704861</t>
-  </si>
-  <si>
-    <t>14.032118055555555</t>
-  </si>
-  <si>
-    <t>43841636.526909724</t>
-  </si>
-  <si>
-    <t>547491309.2803819</t>
-  </si>
-  <si>
-    <t>3809372.4589667725</t>
-  </si>
-  <si>
-    <t>0.14968364197530862</t>
-  </si>
-  <si>
-    <t>554.6267361111111</t>
-  </si>
-  <si>
-    <t>0.4814468195408951</t>
-  </si>
-  <si>
-    <t>0.7112766371016686</t>
-  </si>
-  <si>
-    <t>9.90315125326837</t>
-  </si>
-  <si>
-    <t>0.10748110468435657</t>
-  </si>
-  <si>
-    <t>2.4305064119599384</t>
-  </si>
-  <si>
-    <t>0.00360517116739323</t>
-  </si>
-  <si>
-    <t>43764697.228496775</t>
-  </si>
-  <si>
-    <t>-4.373216202877977</t>
-  </si>
-  <si>
-    <t>4.377339613628167</t>
-  </si>
-  <si>
-    <t>3802796.3854936054</t>
-  </si>
-  <si>
-    <t>0.9999999489578187</t>
-  </si>
-  <si>
-    <t>4.550557098823207</t>
-  </si>
-  <si>
-    <t>3.2124348146703827</t>
-  </si>
-  <si>
-    <t>18.44912304483397</t>
-  </si>
-  <si>
-    <t>2.7295136153643154</t>
-  </si>
-  <si>
-    <t>0.00078538262981844</t>
-  </si>
-  <si>
-    <t>0.0013072673261264357</t>
-  </si>
-  <si>
-    <t>-22.201162061635586</t>
-  </si>
-  <si>
-    <t>40.65028510646955</t>
-  </si>
-  <si>
-    <t>1.8908642773657531</t>
-  </si>
-  <si>
-    <t>3.449754908319265</t>
-  </si>
-  <si>
-    <t>0.0007470919174822533</t>
-  </si>
-  <si>
-    <t>0.5000000353797431</t>
-  </si>
-  <si>
-    <t>11.900808310646983</t>
-  </si>
-  <si>
-    <t>2.247799669640298</t>
-  </si>
-  <si>
-    <t>0.4945927115992653</t>
-  </si>
-  <si>
-    <t>-0.00014156734638431708</t>
-  </si>
-  <si>
-    <t>0.4945927528395527</t>
-  </si>
-  <si>
-    <t>0.5054068921886197</t>
-  </si>
-  <si>
-    <t>-0.01081415309585061</t>
-  </si>
-  <si>
-    <t>0.9944860509024386</t>
-  </si>
-  <si>
-    <t>0.2480956090722131</t>
-  </si>
-  <si>
-    <t>0.7472965539056903</t>
-  </si>
-  <si>
-    <t>0.898918621562276</t>
-  </si>
-  <si>
-    <t>0.831531035937127</t>
-  </si>
-  <si>
-    <t>-0.005513972298563366</t>
-  </si>
-  <si>
-    <t>0.08542523651482138</t>
-  </si>
-  <si>
-    <t>1.5001677052448694</t>
-  </si>
-  <si>
-    <t>0.2519045684137008</t>
-  </si>
-  <si>
-    <t>1.9944855163943336</t>
-  </si>
-  <si>
-    <t>0.07140579466549657</t>
-  </si>
-  <si>
-    <t>0.2679179364795706</t>
-  </si>
-  <si>
-    <t>3.000335410489739</t>
-  </si>
-  <si>
-    <t>1.4890786242057144</t>
-  </si>
-  <si>
-    <t>0.24999991125704307</t>
-  </si>
-  <si>
-    <t>84997.37291520784</t>
-  </si>
-  <si>
-    <t>0.5000003813690327</t>
-  </si>
-  <si>
-    <t>0.24999980931548368</t>
-  </si>
-  <si>
-    <t>2.499877975516451</t>
-  </si>
-  <si>
-    <t>5.30824259151276</t>
-  </si>
-  <si>
-    <t>13.26962740648716</t>
-  </si>
-  <si>
-    <t>3.3178963877691583</t>
-  </si>
-  <si>
-    <t>0.6250305061208873</t>
-  </si>
-  <si>
-    <t>2.8552417015477047</t>
-  </si>
-  <si>
-    <t>61823.13170060749</t>
-  </si>
-  <si>
-    <t>0.3626595848934336</t>
-  </si>
-  <si>
-    <t>0.5319962552054834</t>
-  </si>
-  <si>
-    <t>1.7125296821092644</t>
-  </si>
-  <si>
-    <t>0.606862037852019</t>
-  </si>
-  <si>
-    <t>1.5165998773082698</t>
-  </si>
-  <si>
-    <t>0.37942757798795623</t>
-  </si>
-  <si>
-    <t>2.0</t>
+    <t>(346, 242, 301)</t>
+  </si>
+  <si>
+    <t>fbf7b50207af5102f26149f4612f61d91c47e55e</t>
+  </si>
+  <si>
+    <t>(68, 66, 80, 188, 159, 148)</t>
+  </si>
+  <si>
+    <t>(150.20963589693406, 146.58212078556534, 156.6510609949792)</t>
+  </si>
+  <si>
+    <t>182.82231811242303</t>
+  </si>
+  <si>
+    <t>188.2179587605816</t>
+  </si>
+  <si>
+    <t>189.06083676954358</t>
+  </si>
+  <si>
+    <t>206.54297373670207</t>
+  </si>
+  <si>
+    <t>795757.8333333334</t>
+  </si>
+  <si>
+    <t>0.39108548538215443</t>
+  </si>
+  <si>
+    <t>106185.78323764105</t>
+  </si>
+  <si>
+    <t>0.13343982150052064</t>
+  </si>
+  <si>
+    <t>-539.0000000000001</t>
+  </si>
+  <si>
+    <t>-274.00000000000017</t>
+  </si>
+  <si>
+    <t>155677965658.00003</t>
+  </si>
+  <si>
+    <t>3.8408745367824215</t>
+  </si>
+  <si>
+    <t>141.00000000000063</t>
+  </si>
+  <si>
+    <t>2.663175598235924</t>
+  </si>
+  <si>
+    <t>-197.0000000000001</t>
+  </si>
+  <si>
+    <t>81.24703816833521</t>
+  </si>
+  <si>
+    <t>-430.8248611811583</t>
+  </si>
+  <si>
+    <t>-454.00000000000097</t>
+  </si>
+  <si>
+    <t>-899.0000000000002</t>
+  </si>
+  <si>
+    <t>702.0000000000001</t>
+  </si>
+  <si>
+    <t>59.612505643236304</t>
+  </si>
+  <si>
+    <t>441.938739815216</t>
+  </si>
+  <si>
+    <t>0.5127747281658267</t>
+  </si>
+  <si>
+    <t>0.08025049819866704</t>
+  </si>
+  <si>
+    <t>9699.788737696861</t>
+  </si>
+  <si>
+    <t>372.6518972591673</t>
+  </si>
+  <si>
+    <t>7732.712203932073</t>
+  </si>
+  <si>
+    <t>202.22919133502552</t>
+  </si>
+  <si>
+    <t>52.64880134648066</t>
+  </si>
+  <si>
+    <t>3.5455866726349097</t>
+  </si>
+  <si>
+    <t>0.8732387608623919</t>
+  </si>
+  <si>
+    <t>1.3542800081502169</t>
+  </si>
+  <si>
+    <t>2.147566331247549</t>
+  </si>
+  <si>
+    <t>1.6585520490457264</t>
+  </si>
+  <si>
+    <t>0.5557702875383559</t>
+  </si>
+  <si>
+    <t>0.5084799178527853</t>
+  </si>
+  <si>
+    <t>0.9958671404123037</t>
+  </si>
+  <si>
+    <t>0.9570578995289203</t>
+  </si>
+  <si>
+    <t>-0.27764088014414384</t>
+  </si>
+  <si>
+    <t>0.930506499811137</t>
+  </si>
+  <si>
+    <t>0.45470270887511904</t>
+  </si>
+  <si>
+    <t>18.98351481743557</t>
+  </si>
+  <si>
+    <t>0.016622194483008487</t>
+  </si>
+  <si>
+    <t>6.530467844272435</t>
+  </si>
+  <si>
+    <t>0.9160746388097272</t>
+  </si>
+  <si>
+    <t>0.04380643592630608</t>
+  </si>
+  <si>
+    <t>37.96702963487114</t>
+  </si>
+  <si>
+    <t>4.740513869708204</t>
+  </si>
+  <si>
+    <t>14.048597004778895</t>
+  </si>
+  <si>
+    <t>45157.62805531295</t>
+  </si>
+  <si>
+    <t>0.07555405624485798</t>
+  </si>
+  <si>
+    <t>16.06793590516167</t>
+  </si>
+  <si>
+    <t>399.2142765352924</t>
+  </si>
+  <si>
+    <t>2.3366779951775394</t>
+  </si>
+  <si>
+    <t>859.3731745229361</t>
+  </si>
+  <si>
+    <t>0.007723997077652524</t>
+  </si>
+  <si>
+    <t>0.0031241984170388426</t>
+  </si>
+  <si>
+    <t>4.941514798349833</t>
+  </si>
+  <si>
+    <t>371834.32781756605</t>
+  </si>
+  <si>
+    <t>0.6198067130747346</t>
+  </si>
+  <si>
+    <t>0.7496857286954165</t>
+  </si>
+  <si>
+    <t>0.5408685360550434</t>
+  </si>
+  <si>
+    <t>0.8148286943360386</t>
+  </si>
+  <si>
+    <t>333.79912530234037</t>
+  </si>
+  <si>
+    <t>0.0024919340515605305</t>
+  </si>
+  <si>
+    <t>2124.5394112723216</t>
+  </si>
+  <si>
+    <t>0.0740980542435938</t>
+  </si>
+  <si>
+    <t>19.38080657258326</t>
+  </si>
+  <si>
+    <t>515.6049107142857</t>
+  </si>
+  <si>
+    <t>1017223.7747628348</t>
+  </si>
+  <si>
+    <t>331229017.4644601</t>
+  </si>
+  <si>
+    <t>3322.7562483582924</t>
+  </si>
+  <si>
+    <t>0.002525106286463535</t>
+  </si>
+  <si>
+    <t>6964.017159598215</t>
+  </si>
+  <si>
+    <t>0.24288564312214755</t>
+  </si>
+  <si>
+    <t>0.5028299098763691</t>
+  </si>
+  <si>
+    <t>262.19050194079074</t>
+  </si>
+  <si>
+    <t>0.0012125819934553157</t>
+  </si>
+  <si>
+    <t>6.929042806839137</t>
+  </si>
+  <si>
+    <t>0.03597120497012855</t>
+  </si>
+  <si>
+    <t>1016450.9339871649</t>
+  </si>
+  <si>
+    <t>-25.004622146076418</t>
+  </si>
+  <si>
+    <t>32.92437760412458</t>
+  </si>
+  <si>
+    <t>459767035.4436313</t>
+  </si>
+  <si>
+    <t>2.018347397893784</t>
+  </si>
+  <si>
+    <t>29.827703299704197</t>
+  </si>
+  <si>
+    <t>4.472980463642965</t>
+  </si>
+  <si>
+    <t>216.97420635997392</t>
+  </si>
+  <si>
+    <t>18.318207501238287</t>
+  </si>
+  <si>
+    <t>3.8922361295458034</t>
+  </si>
+  <si>
+    <t>3.438968504218696</t>
+  </si>
+  <si>
+    <t>-124.96386029826597</t>
+  </si>
+  <si>
+    <t>341.9380666582399</t>
+  </si>
+  <si>
+    <t>12.41376306833247</t>
+  </si>
+  <si>
+    <t>24.016925671200774</t>
+  </si>
+  <si>
+    <t>0.28637727886075737</t>
+  </si>
+  <si>
+    <t>0.2964014149844336</t>
+  </si>
+  <si>
+    <t>561.663216607841</t>
+  </si>
+  <si>
+    <t>32.47072181038288</t>
+  </si>
+  <si>
+    <t>37.18385958467377</t>
+  </si>
+  <si>
+    <t>1.558572330507043</t>
+  </si>
+  <si>
+    <t>2.802949976155508</t>
+  </si>
+  <si>
+    <t>1.0551049300270174</t>
+  </si>
+  <si>
+    <t>0.4521277674366716</t>
+  </si>
+  <si>
+    <t>0.7294666347135504</t>
+  </si>
+  <si>
+    <t>1.4487230543039291</t>
+  </si>
+  <si>
+    <t>0.4971394856074007</t>
+  </si>
+  <si>
+    <t>0.6843736823500038</t>
+  </si>
+  <si>
+    <t>0.6675309281011044</t>
+  </si>
+  <si>
+    <t>0.9947144562615416</t>
+  </si>
+  <si>
+    <t>0.9526933640145465</t>
+  </si>
+  <si>
+    <t>-0.10943805974776882</t>
+  </si>
+  <si>
+    <t>0.5246447080551282</t>
+  </si>
+  <si>
+    <t>0.4912271856172029</t>
+  </si>
+  <si>
+    <t>5.659837421770368</t>
+  </si>
+  <si>
+    <t>0.10437993301277962</t>
+  </si>
+  <si>
+    <t>3.794171815605083</t>
+  </si>
+  <si>
+    <t>0.5688155486793914</t>
+  </si>
+  <si>
+    <t>0.18720775706559617</t>
+  </si>
+  <si>
+    <t>11.319674843540735</t>
+  </si>
+  <si>
+    <t>2.7553140150428117</t>
+  </si>
+  <si>
+    <t>0.9645137265456314</t>
+  </si>
+  <si>
+    <t>128641.32643152325</t>
+  </si>
+  <si>
+    <t>0.26719836399592656</t>
+  </si>
+  <si>
+    <t>1.1716501271451492</t>
+  </si>
+  <si>
+    <t>33.18112459735385</t>
+  </si>
+  <si>
+    <t>4.300511611802417</t>
+  </si>
+  <si>
+    <t>140.69088274460196</t>
+  </si>
+  <si>
+    <t>0.14558474864296345</t>
+  </si>
+  <si>
+    <t>0.03540548262635757</t>
+  </si>
+  <si>
+    <t>3.7218505375239803</t>
+  </si>
+  <si>
+    <t>219832.07166305603</t>
+  </si>
+  <si>
+    <t>0.4439668922948551</t>
+  </si>
+  <si>
+    <t>0.6044309117506104</t>
+  </si>
+  <si>
+    <t>1.3340674005301243</t>
+  </si>
+  <si>
+    <t>0.6798851074620885</t>
+  </si>
+  <si>
+    <t>22.687995719768523</t>
+  </si>
+  <si>
+    <t>0.024517218690019795</t>
+  </si>
+  <si>
+    <t>2596.955025319715</t>
+  </si>
+  <si>
+    <t>0.2228954617903798</t>
+  </si>
+  <si>
+    <t>4.4542610050973135</t>
+  </si>
+  <si>
+    <t>35.20719251566389</t>
+  </si>
+  <si>
+    <t>14329810.51223071</t>
+  </si>
+  <si>
+    <t>459717925.1164707</t>
+  </si>
+  <si>
+    <t>465039.6050233819</t>
+  </si>
+  <si>
+    <t>0.053147641106739384</t>
+  </si>
+  <si>
+    <t>1921.6523045232168</t>
+  </si>
+  <si>
+    <t>0.16493453819613912</t>
+  </si>
+  <si>
+    <t>0.3992484998827505</t>
+  </si>
+  <si>
+    <t>13.863646920340122</t>
+  </si>
+  <si>
+    <t>0.02255958133961281</t>
+  </si>
+  <si>
+    <t>6.076715774422551</t>
+  </si>
+  <si>
+    <t>0.014617065747313326</t>
+  </si>
+  <si>
+    <t>14325130.148565361</t>
+  </si>
+  <si>
+    <t>-31.442229050824224</t>
+  </si>
+  <si>
+    <t>35.87009507516715</t>
+  </si>
+  <si>
+    <t>560997748.0700922</t>
+  </si>
+  <si>
+    <t>2.178984091905988</t>
+  </si>
+  <si>
+    <t>35.24224218324825</t>
+  </si>
+  <si>
+    <t>3.1273913638243105</t>
+  </si>
+  <si>
+    <t>145.50851501216033</t>
+  </si>
+  <si>
+    <t>20.99378722921896</t>
+  </si>
+  <si>
+    <t>2.215818703052718</t>
+  </si>
+  <si>
+    <t>2.2090086365106805</t>
+  </si>
+  <si>
+    <t>-123.51267698686796</t>
+  </si>
+  <si>
+    <t>269.0211919990283</t>
+  </si>
+  <si>
+    <t>14.613737669978144</t>
+  </si>
+  <si>
+    <t>26.529499579179014</t>
+  </si>
+  <si>
+    <t>0.005384795806832716</t>
+  </si>
+  <si>
+    <t>0.25882245085125055</t>
+  </si>
+  <si>
+    <t>698.9044953968611</t>
+  </si>
+  <si>
+    <t>31.4681780722778</t>
+  </si>
+  <si>
+    <t>26.55401661838573</t>
+  </si>
+  <si>
+    <t>0.02823327516041705</t>
+  </si>
+  <si>
+    <t>2.8160339760463824</t>
+  </si>
+  <si>
+    <t>1.9667787376122527</t>
+  </si>
+  <si>
+    <t>0.1771779656346302</t>
+  </si>
+  <si>
+    <t>1.0355933977849583</t>
+  </si>
+  <si>
+    <t>1.77430711585226</t>
+  </si>
+  <si>
+    <t>0.8321955735923576</t>
+  </si>
+  <si>
+    <t>0.6066590856471454</t>
+  </si>
+  <si>
+    <t>0.5717767271759093</t>
+  </si>
+  <si>
+    <t>0.9845919592318612</t>
+  </si>
+  <si>
+    <t>0.9192908527642564</t>
+  </si>
+  <si>
+    <t>-0.05419195343388388</t>
+  </si>
+  <si>
+    <t>0.25554115708868264</t>
+  </si>
+  <si>
+    <t>0.48638792594392216</t>
+  </si>
+  <si>
+    <t>5.590694299840593</t>
+  </si>
+  <si>
+    <t>0.07392715331990697</t>
+  </si>
+  <si>
+    <t>4.233550426898566</t>
+  </si>
+  <si>
+    <t>0.21933852594633574</t>
+  </si>
+  <si>
+    <t>0.13130551086345849</t>
+  </si>
+  <si>
+    <t>11.181388599681185</t>
+  </si>
+  <si>
+    <t>2.7709337656830324</t>
+  </si>
+  <si>
+    <t>1.1957031784146588</t>
+  </si>
+  <si>
+    <t>131999.09394048926</t>
+  </si>
+  <si>
+    <t>0.23656840175007426</t>
+  </si>
+  <si>
+    <t>1.391697127274072</t>
+  </si>
+  <si>
+    <t>32.62583813374617</t>
+  </si>
+  <si>
+    <t>2.9038052310675178</t>
+  </si>
+  <si>
+    <t>93.45695613002498</t>
+  </si>
+  <si>
+    <t>0.10345231010140377</t>
+  </si>
+  <si>
+    <t>0.03769495226089445</t>
+  </si>
+  <si>
+    <t>3.4920796550417115</t>
+  </si>
+  <si>
+    <t>317116.3861579483</t>
+  </si>
+  <si>
+    <t>0.5561751471260054</t>
+  </si>
+  <si>
+    <t>0.7010936815110037</t>
+  </si>
+  <si>
+    <t>0.7610942346520309</t>
+  </si>
+  <si>
+    <t>0.7675818867914932</t>
+  </si>
+  <si>
+    <t>25.16071938900979</t>
+  </si>
+  <si>
+    <t>0.029513356793259</t>
+  </si>
+  <si>
+    <t>4702.011791928091</t>
+  </si>
+  <si>
+    <t>0.20922937711600995</t>
+  </si>
+  <si>
+    <t>5.453334078864745</t>
+  </si>
+  <si>
+    <t>36.47594891647755</t>
+  </si>
+  <si>
+    <t>6514675.77875673</t>
+  </si>
+  <si>
+    <t>207445371.19650248</t>
+  </si>
+  <si>
+    <t>217562.47229076733</t>
+  </si>
+  <si>
+    <t>0.06117617000150945</t>
+  </si>
+  <si>
+    <t>4799.835224491612</t>
+  </si>
+  <si>
+    <t>0.21358230874790246</t>
+  </si>
+  <si>
+    <t>0.4535975116792447</t>
+  </si>
+  <si>
+    <t>16.590265658422485</t>
+  </si>
+  <si>
+    <t>0.029568719345055873</t>
+  </si>
+  <si>
+    <t>5.415519110753335</t>
+  </si>
+  <si>
+    <t>0.028194087935745633</t>
+  </si>
+  <si>
+    <t>6513417.769316523</t>
+  </si>
+  <si>
+    <t>-12.182602344526673</t>
+  </si>
+  <si>
+    <t>12.063933091746511</t>
+  </si>
+  <si>
+    <t>72475831.1380809</t>
+  </si>
+  <si>
+    <t>1.0801744907000277</t>
+  </si>
+  <si>
+    <t>12.70301996028285</t>
+  </si>
+  <si>
+    <t>3.134529251937511</t>
+  </si>
+  <si>
+    <t>52.183798508413</t>
+  </si>
+  <si>
+    <t>7.567210260179722</t>
+  </si>
+  <si>
+    <t>-0.06125821368467942</t>
+  </si>
+  <si>
+    <t>-0.06812052654193133</t>
+  </si>
+  <si>
+    <t>-51.16990027047111</t>
+  </si>
+  <si>
+    <t>103.35369877888411</t>
+  </si>
+  <si>
+    <t>5.261606377641604</t>
+  </si>
+  <si>
+    <t>9.535535806859283</t>
+  </si>
+  <si>
+    <t>-0.00016189652637285364</t>
+  </si>
+  <si>
+    <t>0.4902118199887732</t>
+  </si>
+  <si>
+    <t>90.92269055515177</t>
+  </si>
+  <si>
+    <t>12.233321671784456</t>
+  </si>
+  <si>
+    <t>0.683427921170365</t>
+  </si>
+  <si>
+    <t>0.0021688812095162326</t>
+  </si>
+  <si>
+    <t>0.5506351027199193</t>
+  </si>
+  <si>
+    <t>0.5285760116200271</t>
+  </si>
+  <si>
+    <t>0.02044816641896978</t>
+  </si>
+  <si>
+    <t>0.5081734196450278</t>
+  </si>
+  <si>
+    <t>1.048422795654457</t>
+  </si>
+  <si>
+    <t>0.26237136995719557</t>
+  </si>
+  <si>
+    <t>0.74927579297167</t>
+  </si>
+  <si>
+    <t>0.7479533651971753</t>
+  </si>
+  <si>
+    <t>0.9857997656644184</t>
+  </si>
+  <si>
+    <t>0.9277663168283146</t>
+  </si>
+  <si>
+    <t>-0.024054751304266493</t>
+  </si>
+  <si>
+    <t>0.11930499193975636</t>
+  </si>
+  <si>
+    <t>0.49067807637155014</t>
+  </si>
+  <si>
+    <t>3.496828048149868</t>
+  </si>
+  <si>
+    <t>0.24773250494196242</t>
+  </si>
+  <si>
+    <t>2.1342990929194667</t>
+  </si>
+  <si>
+    <t>0.10195558530242857</t>
+  </si>
+  <si>
+    <t>0.26909722061431307</t>
+  </si>
+  <si>
+    <t>6.993656096299736</t>
+  </si>
+  <si>
+    <t>1.5670757738188332</t>
+  </si>
+  <si>
+    <t>0.2698027785849867</t>
+  </si>
+  <si>
+    <t>199646.2539534559</t>
+  </si>
+  <si>
+    <t>0.4815179054385799</t>
+  </si>
+  <si>
+    <t>0.2877298544809518</t>
+  </si>
+  <si>
+    <t>12.533777871441668</t>
+  </si>
+  <si>
+    <t>6.401777633576471</t>
+  </si>
+  <si>
+    <t>79.79580193327621</t>
+  </si>
+  <si>
+    <t>0.5589264629472962</t>
+  </si>
+  <si>
+    <t>0.08794462500557643</t>
+  </si>
+  <si>
+    <t>3.0254445710839737</t>
+  </si>
+  <si>
+    <t>152518.93728617462</t>
+  </si>
+  <si>
+    <t>0.3573533126508553</t>
+  </si>
+  <si>
+    <t>0.519767776040029</t>
+  </si>
+  <si>
+    <t>2.028554194815543</t>
+  </si>
+  <si>
+    <t>0.5790384180379662</t>
+  </si>
+  <si>
+    <t>7.281211844276577</t>
+  </si>
+  <si>
+    <t>0.051285629420889385</t>
+  </si>
+  <si>
+    <t>2480.2349421619465</t>
+  </si>
+  <si>
+    <t>0.49466193501434913</t>
+  </si>
+  <si>
+    <t>2.2439498880597433</t>
+  </si>
+  <si>
+    <t>14.436777024331871</t>
+  </si>
+  <si>
+    <t>58521018.290386915</t>
+  </si>
+  <si>
+    <t>729344960.4297966</t>
+  </si>
+  <si>
+    <t>5095003.693340702</t>
+  </si>
+  <si>
+    <t>0.14562319948588395</t>
+  </si>
+  <si>
+    <t>2231.3482249700837</t>
+  </si>
+  <si>
+    <t>0.44502357897289263</t>
+  </si>
+  <si>
+    <t>0.6769918683761543</t>
+  </si>
+  <si>
+    <t>9.908582489151312</t>
+  </si>
+  <si>
+    <t>0.09737774185944541</t>
+  </si>
+  <si>
+    <t>2.530516664767915</t>
+  </si>
+  <si>
+    <t>0.00629044439593417</t>
+  </si>
+  <si>
+    <t>58495746.42239018</t>
+  </si>
+  <si>
+    <t>-23.54219265260597</t>
+  </si>
+  <si>
+    <t>32.394008604983746</t>
+  </si>
+  <si>
+    <t>437319896.37839586</t>
+  </si>
+  <si>
+    <t>1.9778129753799276</t>
+  </si>
+  <si>
+    <t>28.635685878736908</t>
+  </si>
+  <si>
+    <t>4.462680487354956</t>
+  </si>
+  <si>
+    <t>186.25599936472315</t>
+  </si>
+  <si>
+    <t>17.71059912239945</t>
+  </si>
+  <si>
+    <t>4.283178256144418</t>
+  </si>
+  <si>
+    <t>3.632139828813993</t>
+  </si>
+  <si>
+    <t>-128.2106529819138</t>
+  </si>
+  <si>
+    <t>314.4666523466369</t>
+  </si>
+  <si>
+    <t>11.922045922522763</t>
+  </si>
+  <si>
+    <t>23.423301971968904</t>
+  </si>
+  <si>
+    <t>0.34990550371212753</t>
+  </si>
+  <si>
+    <t>0.30602695092729004</t>
+  </si>
+  <si>
+    <t>530.305459296134</t>
+  </si>
+  <si>
+    <t>44.898637251411444</t>
+  </si>
+  <si>
+    <t>32.55054329096703</t>
+  </si>
+  <si>
+    <t>1.602548197151696</t>
+  </si>
+  <si>
+    <t>2.670937293648795</t>
+  </si>
+  <si>
+    <t>0.9558331962680422</t>
+  </si>
+  <si>
+    <t>0.4713353992255062</t>
+  </si>
+  <si>
+    <t>0.6877631751454807</t>
+  </si>
+  <si>
+    <t>1.3988533551637512</t>
+  </si>
+  <si>
+    <t>0.45980344637801424</t>
+  </si>
+  <si>
+    <t>0.6972272180911901</t>
+  </si>
+  <si>
+    <t>0.6827629268735396</t>
+  </si>
+  <si>
+    <t>0.9952027298278825</t>
+  </si>
+  <si>
+    <t>0.9552440434447996</t>
+  </si>
+  <si>
+    <t>-0.1190700842522879</t>
+  </si>
+  <si>
+    <t>0.5455753435977154</t>
+  </si>
+  <si>
+    <t>0.4857756271618292</t>
+  </si>
+  <si>
+    <t>6.6685718152135625</t>
+  </si>
+  <si>
+    <t>0.11278445584089081</t>
+  </si>
+  <si>
+    <t>3.687957719370639</t>
+  </si>
+  <si>
+    <t>0.5370009592072942</t>
+  </si>
+  <si>
+    <t>0.20147397458568117</t>
+  </si>
+  <si>
+    <t>13.337143630427125</t>
+  </si>
+  <si>
+    <t>2.716518169766778</t>
+  </si>
+  <si>
+    <t>0.9066926224792091</t>
+  </si>
+  <si>
+    <t>127849.75257124945</t>
+  </si>
+  <si>
+    <t>0.27384194231683606</t>
+  </si>
+  <si>
+    <t>1.1286347068016616</t>
+  </si>
+  <si>
+    <t>45.736910045708704</t>
+  </si>
+  <si>
+    <t>4.667821362057105</t>
+  </si>
+  <si>
+    <t>210.69771021523576</t>
+  </si>
+  <si>
+    <t>0.11046168453290198</t>
+  </si>
+  <si>
+    <t>0.024294670733222758</t>
+  </si>
+  <si>
+    <t>3.7587370490791985</t>
+  </si>
+  <si>
+    <t>204509.17740753133</t>
+  </si>
+  <si>
+    <t>0.42496122044759777</t>
+  </si>
+  <si>
+    <t>0.5861076352920354</t>
+  </si>
+  <si>
+    <t>1.4880368481692245</t>
+  </si>
+  <si>
+    <t>0.6626418330020412</t>
+  </si>
+  <si>
+    <t>30.48999186788334</t>
+  </si>
+  <si>
+    <t>0.016273018642735494</t>
+  </si>
+  <si>
+    <t>2553.9004035216435</t>
+  </si>
+  <si>
+    <t>0.23421683818063493</t>
+  </si>
+  <si>
+    <t>4.172558245602655</t>
+  </si>
+  <si>
+    <t>48.221294937637566</t>
+  </si>
+  <si>
+    <t>15642508.776228907</t>
+  </si>
+  <si>
+    <t>687804121.9038885</t>
+  </si>
+  <si>
+    <t>365050.74718529434</t>
+  </si>
+  <si>
+    <t>0.030578075594090773</t>
+  </si>
+  <si>
+    <t>1729.9719369038885</t>
+  </si>
+  <si>
+    <t>0.15865479978942484</t>
+  </si>
+  <si>
+    <t>0.3895951238170876</t>
+  </si>
+  <si>
+    <t>18.82498316833543</t>
+  </si>
+  <si>
+    <t>0.012215856995871388</t>
+  </si>
+  <si>
+    <t>6.090491506795074</t>
+  </si>
+  <si>
+    <t>0.013679897425860827</t>
+  </si>
+  <si>
+    <t>15637165.171592075</t>
+  </si>
+  <si>
+    <t>-8.960996514685121</t>
+  </si>
+  <si>
+    <t>8.838718003326505</t>
+  </si>
+  <si>
+    <t>38617007.58834448</t>
+  </si>
+  <si>
+    <t>1.0056359800374655</t>
+  </si>
+  <si>
+    <t>9.326562166175274</t>
+  </si>
+  <si>
+    <t>3.052720697605369</t>
+  </si>
+  <si>
+    <t>37.05798848726367</t>
+  </si>
+  <si>
+    <t>5.540884105162416</t>
+  </si>
+  <si>
+    <t>-0.053067875244941665</t>
+  </si>
+  <si>
+    <t>-0.046319271522704576</t>
+  </si>
+  <si>
+    <t>-36.64347824700129</t>
+  </si>
+  <si>
+    <t>73.70146673426495</t>
+  </si>
+  <si>
+    <t>3.8680028604361016</t>
+  </si>
+  <si>
+    <t>6.960457849068373</t>
+  </si>
+  <si>
+    <t>-0.012125336565880019</t>
+  </si>
+  <si>
+    <t>0.4995627891290871</t>
+  </si>
+  <si>
+    <t>48.44515726927451</t>
+  </si>
+  <si>
+    <t>6.250569591613195</t>
+  </si>
+  <si>
+    <t>0.5364559591420653</t>
+  </si>
+  <si>
+    <t>0.002517557006515364</t>
+  </si>
+  <si>
+    <t>0.5298601194733085</t>
+  </si>
+  <si>
+    <t>0.47360076779134946</t>
+  </si>
+  <si>
+    <t>0.05606593836229274</t>
+  </si>
+  <si>
+    <t>0.472882408423082</t>
+  </si>
+  <si>
+    <t>0.9798405590038529</t>
+  </si>
+  <si>
+    <t>0.24256612273345649</t>
+  </si>
+  <si>
+    <t>0.763678446834864</t>
+  </si>
+  <si>
+    <t>0.7636306317252857</t>
+  </si>
+  <si>
+    <t>0.9721538274261067</t>
+  </si>
+  <si>
+    <t>0.9054474549973766</t>
+  </si>
+  <si>
+    <t>-0.024527884153873025</t>
+  </si>
+  <si>
+    <t>0.16424526267336292</t>
+  </si>
+  <si>
+    <t>0.472254557172815</t>
+  </si>
+  <si>
+    <t>2.4972994405959392</t>
+  </si>
+  <si>
+    <t>0.25773895838956096</t>
+  </si>
+  <si>
+    <t>1.9862773722461353</t>
+  </si>
+  <si>
+    <t>0.14005909431177202</t>
+  </si>
+  <si>
+    <t>0.2859685888368009</t>
+  </si>
+  <si>
+    <t>4.9945988811918784</t>
+  </si>
+  <si>
+    <t>1.5096279946345712</t>
+  </si>
+  <si>
+    <t>0.25086522181616444</t>
+  </si>
+  <si>
+    <t>197123.89662805418</t>
+  </si>
+  <si>
+    <t>0.4990818038606877</t>
+  </si>
+  <si>
+    <t>0.25184155387065316</t>
+  </si>
+  <si>
+    <t>6.498459479325727</t>
+  </si>
+  <si>
+    <t>7.189368605309948</t>
+  </si>
+  <si>
+    <t>46.54281143461739</t>
+  </si>
+  <si>
+    <t>1.303776749974786</t>
+  </si>
+  <si>
+    <t>0.181019087368429</t>
+  </si>
+  <si>
+    <t>3.0356624632312768</t>
+  </si>
+  <si>
+    <t>134448.56604500994</t>
+  </si>
+  <si>
+    <t>0.33048405657162055</t>
+  </si>
+  <si>
+    <t>0.49549645794574165</t>
+  </si>
+  <si>
+    <t>2.471653388919369</t>
+  </si>
+  <si>
+    <t>0.5672203361825592</t>
+  </si>
+  <si>
+    <t>3.6924687645096474</t>
+  </si>
+  <si>
+    <t>0.10267008092338382</t>
+  </si>
+  <si>
+    <t>133.81456953642385</t>
+  </si>
+  <si>
+    <t>0.44309460111398624</t>
+  </si>
+  <si>
+    <t>2.0953466953203805</t>
+  </si>
+  <si>
+    <t>7.622516556291391</t>
+  </si>
+  <si>
+    <t>990269362.4304636</t>
+  </si>
+  <si>
+    <t>6411591769.70861</t>
+  </si>
+  <si>
+    <t>179497499.30884382</t>
+  </si>
+  <si>
+    <t>0.5545897718910964</t>
+  </si>
+  <si>
+    <t>181.6291390728477</t>
+  </si>
+  <si>
+    <t>0.6014209903074427</t>
+  </si>
+  <si>
+    <t>0.8020833423933598</t>
+  </si>
+  <si>
+    <t>6.628794208825761</t>
+  </si>
+  <si>
+    <t>0.4223406473360576</t>
+  </si>
+  <si>
+    <t>2.339488881311951</t>
+  </si>
+  <si>
+    <t>0.00037888197199284387</t>
+  </si>
+  <si>
+    <t>983303223.7224681</t>
+  </si>
+  <si>
+    <t>-11.217593134897314</t>
+  </si>
+  <si>
+    <t>11.161941439704139</t>
+  </si>
+  <si>
+    <t>61532158.281816654</t>
+  </si>
+  <si>
+    <t>1.0484027744863755</t>
+  </si>
+  <si>
+    <t>11.688011906926093</t>
+  </si>
+  <si>
+    <t>3.1200200163651632</t>
+  </si>
+  <si>
+    <t>47.82766177776202</t>
+  </si>
+  <si>
+    <t>6.976386165923124</t>
+  </si>
+  <si>
+    <t>-0.02386826309573696</t>
+  </si>
+  <si>
+    <t>-0.02182059453398056</t>
+  </si>
+  <si>
+    <t>-43.22569393169563</t>
+  </si>
+  <si>
+    <t>91.05335570945765</t>
+  </si>
+  <si>
+    <t>4.852851711385896</t>
+  </si>
+  <si>
+    <t>8.786169420292767</t>
+  </si>
+  <si>
+    <t>-0.0009656773574457672</t>
+  </si>
+  <si>
+    <t>0.4946361917679262</t>
+  </si>
+  <si>
+    <t>77.1962033881045</t>
+  </si>
+  <si>
+    <t>6.250739904311577</t>
+  </si>
+  <si>
+    <t>0.6033436978158065</t>
+  </si>
+  <si>
+    <t>0.0004528717242489611</t>
+  </si>
+  <si>
+    <t>0.5324387913789598</t>
+  </si>
+  <si>
+    <t>0.5108841714808836</t>
+  </si>
+  <si>
+    <t>0.02066127341302456</t>
+  </si>
+  <si>
+    <t>0.499770682849164</t>
+  </si>
+  <si>
+    <t>1.0219332312442715</t>
+  </si>
+  <si>
+    <t>0.2537103688829853</t>
+  </si>
+  <si>
+    <t>0.7519541424428022</t>
+  </si>
+  <si>
+    <t>0.7512260074385899</t>
+  </si>
+  <si>
+    <t>0.97014735391861</t>
+  </si>
+  <si>
+    <t>0.9004148542811785</t>
+  </si>
+  <si>
+    <t>-0.022567484189132313</t>
+  </si>
+  <si>
+    <t>0.11487058417511481</t>
+  </si>
+  <si>
+    <t>0.49016693143215345</t>
+  </si>
+  <si>
+    <t>2.4990700050805716</t>
+  </si>
+  <si>
+    <t>0.25180130197344724</t>
+  </si>
+  <si>
+    <t>2.0734630400860015</t>
+  </si>
+  <si>
+    <t>0.09823737493295119</t>
+  </si>
+  <si>
+    <t>0.27061054699868603</t>
+  </si>
+  <si>
+    <t>4.998140010161145</t>
+  </si>
+  <si>
+    <t>1.5366442372023388</t>
+  </si>
+  <si>
+    <t>0.2608307407149609</t>
+  </si>
+  <si>
+    <t>201530.6815903758</t>
+  </si>
+  <si>
+    <t>0.4896945279244628</t>
+  </si>
+  <si>
+    <t>0.2708360077940645</t>
+  </si>
+  <si>
+    <t>6.517313833238143</t>
+  </si>
+  <si>
+    <t>6.476041617530469</t>
+  </si>
+  <si>
+    <t>42.075628980760854</t>
+  </si>
+  <si>
+    <t>1.1747600055234766</t>
+  </si>
+  <si>
+    <t>0.18436021749478262</t>
+  </si>
+  <si>
+    <t>2.9949039561180113</t>
+  </si>
+  <si>
+    <t>149914.59153261382</t>
+  </si>
+  <si>
+    <t>0.3539921037484524</t>
+  </si>
+  <si>
+    <t>0.516068031220801</t>
+  </si>
+  <si>
+    <t>2.064920638487099</t>
+  </si>
+  <si>
+    <t>0.5747051884223772</t>
+  </si>
+  <si>
+    <t>3.755790996940561</t>
+  </si>
+  <si>
+    <t>0.10735237401034924</t>
+  </si>
+  <si>
+    <t>1466.639499492729</t>
+  </si>
+  <si>
+    <t>0.49598900895932674</t>
+  </si>
+  <si>
+    <t>2.2395466801862653</t>
+  </si>
+  <si>
+    <t>8.28745350016909</t>
+  </si>
+  <si>
+    <t>100142472.0297599</t>
+  </si>
+  <si>
+    <t>650065382.6422049</t>
+  </si>
+  <si>
+    <t>18105188.692326117</t>
+  </si>
+  <si>
+    <t>0.5424134821327923</t>
+  </si>
+  <si>
+    <t>1467.2022319918838</t>
+  </si>
+  <si>
+    <t>0.4961793141670219</t>
+  </si>
+  <si>
+    <t>0.7203756545771084</t>
+  </si>
+  <si>
+    <t>5.962724942207622</t>
+  </si>
+  <si>
+    <t>0.3919937505726212</t>
+  </si>
+  <si>
+    <t>2.3324314368800008</t>
+  </si>
+  <si>
+    <t>0.0037097814277577464</t>
+  </si>
+  <si>
+    <t>100069810.69780827</t>
+  </si>
+  <si>
+    <t>-4.619438894325622</t>
+  </si>
+  <si>
+    <t>4.619423522674362</t>
+  </si>
+  <si>
+    <t>10492397.745074438</t>
+  </si>
+  <si>
+    <t>0.9999999480044597</t>
+  </si>
+  <si>
+    <t>4.831480335695949</t>
+  </si>
+  <si>
+    <t>3.130589438291599</t>
+  </si>
+  <si>
+    <t>20.73413781951116</t>
+  </si>
+  <si>
+    <t>2.880142505363352</t>
+  </si>
+  <si>
+    <t>0.001533820885860417</t>
+  </si>
+  <si>
+    <t>-0.0011825216892040503</t>
+  </si>
+  <si>
+    <t>-23.110049222312373</t>
+  </si>
+  <si>
+    <t>43.84418704182353</t>
+  </si>
+  <si>
+    <t>2.003911303728972</t>
+  </si>
+  <si>
+    <t>3.6281553285432335</t>
+  </si>
+  <si>
+    <t>0.001832466033004082</t>
+  </si>
+  <si>
+    <t>0.5000000360405614</t>
+  </si>
+  <si>
+    <t>13.16350873543015</t>
+  </si>
+  <si>
+    <t>2.246464410254103</t>
+  </si>
+  <si>
+    <t>0.4937568730693601</t>
+  </si>
+  <si>
+    <t>0.00013782141638016276</t>
+  </si>
+  <si>
+    <t>0.49375689400454387</t>
+  </si>
+  <si>
+    <t>0.5062427696477094</t>
+  </si>
+  <si>
+    <t>-0.012485882621569577</t>
+  </si>
+  <si>
+    <t>0.9941162863648716</t>
+  </si>
+  <si>
+    <t>0.24796878500136277</t>
+  </si>
+  <si>
+    <t>0.7468786151761453</t>
+  </si>
+  <si>
+    <t>0.8987514460704582</t>
+  </si>
+  <si>
+    <t>0.8312524101174303</t>
+  </si>
+  <si>
+    <t>-0.00588372571963143</t>
+  </si>
+  <si>
+    <t>0.08775551396658018</t>
+  </si>
+  <si>
+    <t>1.4998619316926527</t>
+  </si>
+  <si>
+    <t>0.25203138317251067</t>
+  </si>
+  <si>
+    <t>1.9941157895565707</t>
+  </si>
+  <si>
+    <t>0.07338088129304854</t>
+  </si>
+  <si>
+    <t>0.2684262649858135</t>
+  </si>
+  <si>
+    <t>2.9997238633853054</t>
+  </si>
+  <si>
+    <t>1.4878730199088617</t>
+  </si>
+  <si>
+    <t>0.2499999159130633</t>
+  </si>
+  <si>
+    <t>210356.4416000581</t>
+  </si>
+  <si>
+    <t>0.5000004009227177</t>
+  </si>
+  <si>
+    <t>0.24999979953864118</t>
+  </si>
+  <si>
+    <t>2.49999257714201</t>
+  </si>
+  <si>
+    <t>5.435330386720493</t>
+  </si>
+  <si>
+    <t>13.58044821735162</t>
+  </si>
+  <si>
+    <t>3.39905092906271</t>
+  </si>
+  <si>
+    <t>0.6250018557144975</t>
+  </si>
+  <si>
+    <t>2.8707090390497774</t>
+  </si>
+  <si>
+    <t>151667.9259783151</t>
+  </si>
+  <si>
+    <t>0.3593420551766391</t>
+  </si>
+  <si>
+    <t>0.5278158815047116</t>
+  </si>
+  <si>
+    <t>1.7757479767770872</t>
+  </si>
+  <si>
+    <t>0.6033126693152628</t>
+  </si>
+  <si>
+    <t>1.5081849158452345</t>
+  </si>
+  <si>
+    <t>0.3770946076827698</t>
+  </si>
+  <si>
+    <t>5.0</t>
   </si>
   <si>
     <t>0.5</t>
@@ -3901,259 +3901,259 @@
     <t>2.5</t>
   </si>
   <si>
-    <t>12763147468.75</t>
-  </si>
-  <si>
-    <t>31918053977.5</t>
-  </si>
-  <si>
-    <t>7974420841.5625</t>
+    <t>29933069403.8</t>
+  </si>
+  <si>
+    <t>74794279591.4</t>
+  </si>
+  <si>
+    <t>18717766856.9</t>
   </si>
   <si>
     <t>0.625</t>
   </si>
   <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>0.375</t>
-  </si>
-  <si>
-    <t>0.5000000000195877</t>
-  </si>
-  <si>
-    <t>1.2500000000489535</t>
-  </si>
-  <si>
-    <t>0.3125000000122462</t>
-  </si>
-  <si>
-    <t>1.9999999999999987</t>
-  </si>
-  <si>
-    <t>1.2517955442337603e-05</t>
-  </si>
-  <si>
-    <t>6381494301.1875</t>
-  </si>
-  <si>
-    <t>-1665.9481476447586</t>
-  </si>
-  <si>
-    <t>-788.370220877914</t>
-  </si>
-  <si>
-    <t>533593848277.46564</t>
-  </si>
-  <si>
-    <t>5.673671365290879</t>
-  </si>
-  <si>
-    <t>493.6723612222895</t>
-  </si>
-  <si>
-    <t>2.291581911176245</t>
-  </si>
-  <si>
-    <t>-496.0533609084466</t>
-  </si>
-  <si>
-    <t>269.74784712549956</t>
-  </si>
-  <si>
-    <t>-1251.0407974484258</t>
-  </si>
-  <si>
-    <t>-1275.5916947326941</t>
-  </si>
-  <si>
-    <t>-2514.789658011665</t>
-  </si>
-  <si>
-    <t>2018.7362971032182</t>
-  </si>
-  <si>
-    <t>201.88034976568537</t>
-  </si>
-  <si>
-    <t>1292.236822049539</t>
-  </si>
-  <si>
-    <t>0.10588428750411923</t>
-  </si>
-  <si>
-    <t>0.02114412894191158</t>
-  </si>
-  <si>
-    <t>104772.9273802981</t>
-  </si>
-  <si>
-    <t>2685.08114183526</t>
-  </si>
-  <si>
-    <t>794986.4283391817</t>
-  </si>
-  <si>
-    <t>1192.3881226942622</t>
-  </si>
-  <si>
-    <t>584.9825549211602</t>
-  </si>
-  <si>
-    <t>32.71252326668609</t>
-  </si>
-  <si>
-    <t>0.8937159010075324</t>
-  </si>
-  <si>
-    <t>4.024888317844451</t>
-  </si>
-  <si>
-    <t>3.52354012371801</t>
-  </si>
-  <si>
-    <t>15.975861089915925</t>
-  </si>
-  <si>
-    <t>0.34121109810823186</t>
-  </si>
-  <si>
-    <t>0.25502928403585523</t>
-  </si>
-  <si>
-    <t>0.9952716054112992</t>
-  </si>
-  <si>
-    <t>0.9551666344593704</t>
-  </si>
-  <si>
-    <t>-0.23482335608806465</t>
-  </si>
-  <si>
-    <t>0.9587683940878067</t>
-  </si>
-  <si>
-    <t>0.2598287653740691</t>
-  </si>
-  <si>
-    <t>50.4676342760296</t>
-  </si>
-  <si>
-    <t>0.0014723233223935905</t>
-  </si>
-  <si>
-    <t>9.939385246879745</t>
-  </si>
-  <si>
-    <t>0.9102381812757343</t>
-  </si>
-  <si>
-    <t>0.0037285881864045586</t>
-  </si>
-  <si>
-    <t>100.93526855205914</t>
-  </si>
-  <si>
-    <t>6.588278390842016</t>
-  </si>
-  <si>
-    <t>154.42376954696144</t>
-  </si>
-  <si>
-    <t>6072.381970435846</t>
-  </si>
-  <si>
-    <t>0.021019581663172852</t>
-  </si>
-  <si>
-    <t>168.9243464929746</t>
-  </si>
-  <si>
-    <t>2857.2585289564204</t>
-  </si>
-  <si>
-    <t>1.3599323732879063</t>
-  </si>
-  <si>
-    <t>3726.2381439112205</t>
-  </si>
-  <si>
-    <t>0.0007010233084011293</t>
-  </si>
-  <si>
-    <t>0.0005044892358868562</t>
-  </si>
-  <si>
-    <t>6.170428697122613</t>
-  </si>
-  <si>
-    <t>241059.90962818314</t>
-  </si>
-  <si>
-    <t>0.834004035464457</t>
-  </si>
-  <si>
-    <t>0.9040676855479964</t>
-  </si>
-  <si>
-    <t>0.13508137848828167</t>
-  </si>
-  <si>
-    <t>0.9303608697072286</t>
-  </si>
-  <si>
-    <t>2687.489748065739</t>
-  </si>
-  <si>
-    <t>0.000466362435029483</t>
-  </si>
-  <si>
-    <t>1942.209642925125</t>
-  </si>
-  <si>
-    <t>0.021747076363245868</t>
-  </si>
-  <si>
-    <t>166.6951591330482</t>
-  </si>
-  <si>
-    <t>3420.4466291191256</t>
-  </si>
-  <si>
-    <t>583.3870830487409</t>
-  </si>
-  <si>
-    <t>1058764.6308882644</t>
-  </si>
-  <si>
-    <t>0.37180756168040213</t>
-  </si>
-  <si>
-    <t>0.00047227190529393174</t>
-  </si>
-  <si>
-    <t>34905.32104267207</t>
-  </si>
-  <si>
-    <t>0.39083766521483915</t>
-  </si>
-  <si>
-    <t>0.6493838115194182</t>
-  </si>
-  <si>
-    <t>2289.39192095569</t>
-  </si>
-  <si>
-    <t>0.00031048449975104646</t>
-  </si>
-  <si>
-    <t>7.78782971319352</t>
-  </si>
-  <si>
-    <t>0.27949152064993227</t>
-  </si>
-  <si>
-    <t>570.5855280371292</t>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.2000002733453797</t>
+  </si>
+  <si>
+    <t>0.5000006750635028</t>
+  </si>
+  <si>
+    <t>0.1250001729158489</t>
+  </si>
+  <si>
+    <t>3.3219280948873595</t>
+  </si>
+  <si>
+    <t>1.2545760662014699e-05</t>
+  </si>
+  <si>
+    <t>23579672256.56</t>
+  </si>
+  <si>
+    <t>-1518.2094619213694</t>
+  </si>
+  <si>
+    <t>-776.8386956964818</t>
+  </si>
+  <si>
+    <t>1243294190804.6455</t>
+  </si>
+  <si>
+    <t>5.315101562635595</t>
+  </si>
+  <si>
+    <t>397.6262683168202</t>
+  </si>
+  <si>
+    <t>2.6737938413502405</t>
+  </si>
+  <si>
+    <t>-504.269494173365</t>
+  </si>
+  <si>
+    <t>228.2614016191708</t>
+  </si>
+  <si>
+    <t>-1217.979249010214</t>
+  </si>
+  <si>
+    <t>-1287.1903535132262</t>
+  </si>
+  <si>
+    <t>-2534.1054598771684</t>
+  </si>
+  <si>
+    <t>2029.8359657038034</t>
+  </si>
+  <si>
+    <t>167.77400991765722</t>
+  </si>
+  <si>
+    <t>1248.9223895145894</t>
+  </si>
+  <si>
+    <t>0.5331618449978468</t>
+  </si>
+  <si>
+    <t>0.029152276347223203</t>
+  </si>
+  <si>
+    <t>76333.68401134748</t>
+  </si>
+  <si>
+    <t>2907.425192945365</t>
+  </si>
+  <si>
+    <t>484400.55742194125</t>
+  </si>
+  <si>
+    <t>4633.17073345339</t>
+  </si>
+  <si>
+    <t>415.74324751384944</t>
+  </si>
+  <si>
+    <t>23.33114437228223</t>
+  </si>
+  <si>
+    <t>0.8931564127175867</t>
+  </si>
+  <si>
+    <t>3.43923258663933</t>
+  </si>
+  <si>
+    <t>3.3130002795089393</t>
+  </si>
+  <si>
+    <t>11.082832878833106</t>
+  </si>
+  <si>
+    <t>0.3680465906569757</t>
+  </si>
+  <si>
+    <t>0.28425581190748045</t>
+  </si>
+  <si>
+    <t>0.9965964290065167</t>
+  </si>
+  <si>
+    <t>0.9611583241124693</t>
+  </si>
+  <si>
+    <t>-0.2351396045371299</t>
+  </si>
+  <si>
+    <t>0.9505095095674915</t>
+  </si>
+  <si>
+    <t>0.28698708798929634</t>
+  </si>
+  <si>
+    <t>53.00286645484065</t>
+  </si>
+  <si>
+    <t>0.002668931965569931</t>
+  </si>
+  <si>
+    <t>9.282509589323778</t>
+  </si>
+  <si>
+    <t>0.9312161720940219</t>
+  </si>
+  <si>
+    <t>0.007822431788423616</t>
+  </si>
+  <si>
+    <t>106.00573290968126</t>
+  </si>
+  <si>
+    <t>6.221858655539572</t>
+  </si>
+  <si>
+    <t>109.7685979715329</t>
+  </si>
+  <si>
+    <t>20054.003420715497</t>
+  </si>
+  <si>
+    <t>0.028306749922571785</t>
+  </si>
+  <si>
+    <t>123.93744062274382</t>
+  </si>
+  <si>
+    <t>3064.3370879550203</t>
+  </si>
+  <si>
+    <t>1.4319772877594228</t>
+  </si>
+  <si>
+    <t>4190.876696371722</t>
+  </si>
+  <si>
+    <t>0.0006131893403917608</t>
+  </si>
+  <si>
+    <t>0.0004171587107788387</t>
+  </si>
+  <si>
+    <t>5.887123858061982</t>
+  </si>
+  <si>
+    <t>574523.4355894313</t>
+  </si>
+  <si>
+    <t>0.810322065535657</t>
+  </si>
+  <si>
+    <t>0.8887334822997653</t>
+  </si>
+  <si>
+    <t>0.16360017800536766</t>
+  </si>
+  <si>
+    <t>0.9191309067762827</t>
+  </si>
+  <si>
+    <t>2851.5105992431627</t>
+  </si>
+  <si>
+    <t>0.0003804430897767644</t>
+  </si>
+  <si>
+    <t>4623.973977530822</t>
+  </si>
+  <si>
+    <t>0.025552605714724452</t>
+  </si>
+  <si>
+    <t>118.89463531874848</t>
+  </si>
+  <si>
+    <t>3749.943561801292</t>
+  </si>
+  <si>
+    <t>9896.57019545864</t>
+  </si>
+  <si>
+    <t>19541082.050768405</t>
+  </si>
+  <si>
+    <t>5.090349424290013</t>
+  </si>
+  <si>
+    <t>0.00036540935177736887</t>
+  </si>
+  <si>
+    <t>64709.75820489724</t>
+  </si>
+  <si>
+    <t>0.3575934781077329</t>
+  </si>
+  <si>
+    <t>0.6199149044254288</t>
+  </si>
+  <si>
+    <t>2389.81950319149</t>
+  </si>
+  <si>
+    <t>0.00022169593557581444</t>
+  </si>
+  <si>
+    <t>7.703027699981712</t>
+  </si>
+  <si>
+    <t>0.2270268303637518</t>
+  </si>
+  <si>
+    <t>9877.168234406927</t>
   </si>
 </sst>
 </file>
@@ -4618,7 +4618,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-608.2946661134241</v>
+        <v>-355.9919116646957</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4626,7 +4626,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-4817.999999999999</v>
+        <v>-1125</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4634,7 +4634,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>3127</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4674,7 +4674,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>319541</v>
+        <v>797082</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4682,7 +4682,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4706,7 +4706,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.5844332862025283</v>
+        <v>0.7366641905396496</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4714,7 +4714,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.3485348416404004</v>
+        <v>0.4050335837174094</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4722,7 +4722,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>59.49599731996035</v>
+        <v>77.59974680941059</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4730,7 +4730,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>170.7031556441784</v>
+        <v>191.5884260687669</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4778,7 +4778,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>99.76460621826887</v>
+        <v>141.1363328067137</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4810,7 +4810,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>319541</v>
+        <v>797082</v>
       </c>
     </row>
     <row r="38" spans="1:2">

</xml_diff>